<commit_message>
update spreadsheet of particpants
</commit_message>
<xml_diff>
--- a/planning/workshop-participants.xlsx
+++ b/planning/workshop-participants.xlsx
@@ -8,24 +8,33 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RicardD\Documents\GitHub\ageing-best-practices-2022\planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C81F8043-D593-4676-882D-695B1E1AFB1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76A729B0-B1A6-4F4B-9D79-E7F22E938DCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="16440" windowHeight="28440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="615" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="110">
   <si>
     <t>Name</t>
   </si>
@@ -39,9 +48,6 @@
     <t>Replied to planning survey, if so when</t>
   </si>
   <si>
-    <t>Survey was sent to the following participants on Monday October 31 2022</t>
-  </si>
-  <si>
     <t>https://forms.gle/5MXqYDZbVZLRG2GN6</t>
   </si>
   <si>
@@ -325,13 +331,46 @@
   </si>
   <si>
     <t>Perreault, Andrea</t>
+  </si>
+  <si>
+    <t>Yes, 2022-11-04</t>
+  </si>
+  <si>
+    <t>yeongha.jung@dfo-mpo.gc.ca</t>
+  </si>
+  <si>
+    <t>Jung, Yeongha</t>
+  </si>
+  <si>
+    <t>Campbell, Barbara</t>
+  </si>
+  <si>
+    <t>barbara.campbell@dfo-mpo.gc.ca</t>
+  </si>
+  <si>
+    <t>stephen.wischniowski@dfo-mpo.gc.ca</t>
+  </si>
+  <si>
+    <t>Wischniowski, Stephen</t>
+  </si>
+  <si>
+    <t>Potential participants</t>
+  </si>
+  <si>
+    <t>Participant</t>
+  </si>
+  <si>
+    <t>Responded</t>
+  </si>
+  <si>
+    <t>Survey was sent to potential participants on Monday October 31 2022</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -371,6 +410,11 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="7"/>
+      <color rgb="FF202124"/>
+      <name val="Roboto"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -393,7 +437,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -405,6 +449,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -686,34 +732,51 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:G66"/>
+  <dimension ref="A2:I69"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F45" sqref="F45"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="15" customWidth="1"/>
-    <col min="3" max="3" width="21.7109375" customWidth="1"/>
-    <col min="5" max="5" width="38.42578125" customWidth="1"/>
+    <col min="3" max="3" width="21.7265625" customWidth="1"/>
+    <col min="5" max="5" width="38.453125" customWidth="1"/>
+    <col min="6" max="6" width="19.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B3" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F3" t="s">
+        <v>106</v>
+      </c>
+      <c r="G3">
+        <f>SUM(H8:H62)</f>
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B4" s="1"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F4" t="s">
+        <v>108</v>
+      </c>
+      <c r="G4">
+        <f>SUM(I8:I62)</f>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B5" s="1"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" s="6" t="s">
         <v>1</v>
       </c>
@@ -729,8 +792,14 @@
         <v>3</v>
       </c>
       <c r="G6" s="6"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H6" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="I6" s="6" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
@@ -739,67 +808,103 @@
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
     </row>
-    <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D8" s="2"/>
       <c r="E8" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F8" s="2"/>
+        <v>13</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>99</v>
+      </c>
       <c r="G8" s="2"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H8">
+        <f>IF(ISBLANK(C8), "",1)</f>
+        <v>1</v>
+      </c>
+      <c r="I8">
+        <f>IF(LEFT(F8,3)="Yes",1,"")</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" s="5"/>
       <c r="B9" s="8"/>
       <c r="C9" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D9" s="2"/>
       <c r="E9" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G9" s="2"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H9">
+        <f t="shared" ref="H9:H62" si="0">IF(ISBLANK(C9), "",1)</f>
+        <v>1</v>
+      </c>
+      <c r="I9">
+        <f t="shared" ref="I9:I62" si="1">IF(LEFT(F9,3)="Yes",1,"")</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" s="5"/>
       <c r="B10" s="8"/>
       <c r="C10" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G10" s="2"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H10">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" s="5"/>
       <c r="B11" s="8"/>
       <c r="C11" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D11" s="2"/>
       <c r="E11" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="F11" s="2"/>
+        <v>35</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>99</v>
+      </c>
       <c r="G11" s="2"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H11">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" s="5"/>
       <c r="B12" s="8"/>
       <c r="C12" s="2"/>
@@ -807,85 +912,133 @@
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H12" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I12" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" s="5"/>
       <c r="B13" s="8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D13" s="2"/>
       <c r="E13" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G13" s="2"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H13">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" s="5"/>
       <c r="B14" s="8"/>
       <c r="C14" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D14" s="2"/>
       <c r="E14" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G14" s="2"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H14">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" s="5"/>
       <c r="B15" s="8"/>
       <c r="C15" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D15" s="2"/>
       <c r="E15" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G15" s="2"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H15">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" s="5"/>
       <c r="B16" s="8"/>
       <c r="C16" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D16" s="2"/>
       <c r="E16" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G16" s="2"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H16">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I16">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" s="5"/>
       <c r="B17" s="8"/>
       <c r="C17" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D17" s="2"/>
       <c r="E17" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G17" s="2"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H17">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I17">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" s="5"/>
       <c r="B18" s="8"/>
       <c r="C18" s="2"/>
@@ -893,8 +1046,16 @@
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H18" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19" s="5"/>
       <c r="B19" s="8"/>
       <c r="C19" s="2"/>
@@ -902,102 +1063,158 @@
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
-    </row>
-    <row r="20" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="H19" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I19" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A20" s="5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D20" s="2"/>
       <c r="E20" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G20" s="2"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H20">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I20">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21" s="5"/>
       <c r="B21" s="8"/>
       <c r="C21" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D21" s="2"/>
       <c r="E21" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G21" s="2"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H21">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I21">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22" s="5"/>
       <c r="B22" s="8"/>
       <c r="C22" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D22" s="2"/>
       <c r="E22" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G22" s="2"/>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H22">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I22">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23" s="5"/>
       <c r="B23" s="8"/>
       <c r="C23" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D23" s="2"/>
       <c r="E23" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G23" s="2"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H23">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I23">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24" s="5"/>
       <c r="B24" s="8"/>
       <c r="C24" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D24" s="2"/>
       <c r="E24" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G24" s="2"/>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H24">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I24">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25" s="5"/>
       <c r="B25" s="8"/>
       <c r="C25" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D25" s="2"/>
       <c r="E25" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="F25" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="F25" s="2" t="s">
-        <v>54</v>
-      </c>
       <c r="G25" s="2"/>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H25">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I25">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A26" s="5"/>
       <c r="B26" s="8"/>
       <c r="C26" s="2"/>
@@ -1005,25 +1222,41 @@
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
       <c r="G26" s="2"/>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H26" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I26" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A27" s="5"/>
       <c r="B27" s="8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D27" s="2"/>
       <c r="E27" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G27" s="2"/>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H27">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I27">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A28" s="5"/>
       <c r="B28" s="8"/>
       <c r="C28" s="2"/>
@@ -1031,8 +1264,16 @@
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
       <c r="G28" s="2"/>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H28" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A29" s="5"/>
       <c r="B29" s="8"/>
       <c r="C29" s="2"/>
@@ -1040,25 +1281,41 @@
       <c r="E29" s="2"/>
       <c r="F29" s="2"/>
       <c r="G29" s="2"/>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H29" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I29" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A30" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B30" s="8"/>
       <c r="C30" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D30" s="2"/>
       <c r="E30" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G30" s="2"/>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H30">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I30">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A31" s="5"/>
       <c r="B31" s="8"/>
       <c r="C31" s="2"/>
@@ -1066,8 +1323,16 @@
       <c r="E31" s="2"/>
       <c r="F31" s="2"/>
       <c r="G31" s="2"/>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H31" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I31" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A32" s="5"/>
       <c r="B32" s="8"/>
       <c r="C32" s="2"/>
@@ -1075,51 +1340,85 @@
       <c r="E32" s="2"/>
       <c r="F32" s="2"/>
       <c r="G32" s="2"/>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H32" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I32" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A33" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B33" s="8"/>
       <c r="C33" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D33" s="2"/>
       <c r="E33" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F33" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F33" s="2" t="s">
-        <v>19</v>
-      </c>
       <c r="G33" s="2"/>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H33">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I33">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A34" s="5"/>
       <c r="B34" s="8"/>
       <c r="C34" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D34" s="2"/>
       <c r="E34" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F34" s="2"/>
       <c r="G34" s="2"/>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H34">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I34" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A35" s="5"/>
       <c r="B35" s="8"/>
       <c r="C35" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D35" s="2"/>
       <c r="E35" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="F35" s="2"/>
+        <v>70</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>53</v>
+      </c>
       <c r="G35" s="2"/>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H35">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I35">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A36" s="5"/>
       <c r="B36" s="8"/>
       <c r="C36" s="2"/>
@@ -1127,38 +1426,62 @@
       <c r="E36" s="2"/>
       <c r="F36" s="2"/>
       <c r="G36" s="2"/>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H36" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I36" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A37" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B37" s="8"/>
       <c r="C37" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D37" s="2"/>
       <c r="E37" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G37" s="2"/>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H37">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I37">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A38" s="5"/>
       <c r="B38" s="8"/>
       <c r="C38" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D38" s="2"/>
       <c r="E38" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F38" s="2"/>
       <c r="G38" s="2"/>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H38">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I38" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A39" s="5"/>
       <c r="B39" s="8"/>
       <c r="C39" s="2"/>
@@ -1166,8 +1489,16 @@
       <c r="E39" s="2"/>
       <c r="F39" s="2"/>
       <c r="G39" s="2"/>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H39" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I39" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A40" s="5"/>
       <c r="B40" s="8"/>
       <c r="C40" s="2"/>
@@ -1175,334 +1506,569 @@
       <c r="E40" s="2"/>
       <c r="F40" s="2"/>
       <c r="G40" s="2"/>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H40" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I40" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A41" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B41" s="8"/>
       <c r="C41" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D41" s="2"/>
-      <c r="E41" s="7" t="s">
-        <v>22</v>
+      <c r="E41" s="10" t="s">
+        <v>21</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G41" s="2"/>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H41">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I41">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A42" s="5"/>
       <c r="B42" s="8"/>
       <c r="C42" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D42" s="2"/>
       <c r="E42" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G42" s="2"/>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H42">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I42">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A43" s="5"/>
       <c r="B43" s="8"/>
       <c r="C43" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D43" s="2"/>
       <c r="E43" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G43" s="2"/>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H43">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I43">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A44" s="5"/>
       <c r="B44" s="8"/>
       <c r="C44" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D44" s="2"/>
       <c r="E44" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G44" s="2"/>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H44">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I44">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A45" s="5"/>
       <c r="B45" s="8"/>
       <c r="C45" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D45" s="2"/>
       <c r="E45" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="F45" s="2"/>
+        <v>54</v>
+      </c>
+      <c r="F45" s="2" t="s">
+        <v>53</v>
+      </c>
       <c r="G45" s="2"/>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H45">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I45">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A46" s="5"/>
       <c r="B46" s="8"/>
       <c r="C46" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D46" s="2"/>
       <c r="E46" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F46" s="2"/>
       <c r="G46" s="2"/>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H46">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I46" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A47" s="5"/>
       <c r="B47" s="8"/>
       <c r="C47" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D47" s="2"/>
       <c r="E47" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F47" s="2"/>
       <c r="G47" s="2"/>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H47">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I47" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A48" s="5"/>
       <c r="B48" s="8"/>
       <c r="C48" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D48" s="2"/>
       <c r="E48" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F48" s="2"/>
       <c r="G48" s="2"/>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H48">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I48" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A49" s="5"/>
       <c r="B49" s="8"/>
       <c r="C49" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D49" s="2"/>
       <c r="E49" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F49" s="2"/>
       <c r="G49" s="2"/>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H49">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I49" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A50" s="5"/>
       <c r="B50" s="8"/>
       <c r="C50" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D50" s="2"/>
       <c r="E50" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F50" s="2"/>
       <c r="G50" s="2"/>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H50">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I50" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A51" s="5"/>
       <c r="B51" s="8"/>
       <c r="C51" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D51" s="2"/>
       <c r="E51" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G51" s="2"/>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H51">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I51">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A52" s="5"/>
       <c r="B52" s="8"/>
-      <c r="C52" s="2"/>
+      <c r="C52" s="2" t="s">
+        <v>101</v>
+      </c>
       <c r="D52" s="2"/>
-      <c r="E52" s="2"/>
-      <c r="F52" s="2"/>
+      <c r="E52" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="F52" s="2" t="s">
+        <v>99</v>
+      </c>
       <c r="G52" s="2"/>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H52">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I52">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A53" s="5"/>
       <c r="B53" s="8"/>
-      <c r="C53" s="2"/>
+      <c r="C53" s="2" t="s">
+        <v>102</v>
+      </c>
       <c r="D53" s="2"/>
-      <c r="E53" s="2"/>
-      <c r="F53" s="2"/>
+      <c r="E53" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="F53" s="2" t="s">
+        <v>99</v>
+      </c>
       <c r="G53" s="2"/>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A54" s="5" t="s">
-        <v>9</v>
-      </c>
+      <c r="H53">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I53">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A54" s="5"/>
       <c r="B54" s="8"/>
       <c r="C54" s="2" t="s">
-        <v>95</v>
+        <v>105</v>
       </c>
       <c r="D54" s="2"/>
-      <c r="E54" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="F54" s="2"/>
+      <c r="E54" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="F54" s="2" t="s">
+        <v>53</v>
+      </c>
       <c r="G54" s="2"/>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H54">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I54">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A55" s="5"/>
       <c r="B55" s="8"/>
-      <c r="C55" s="2" t="s">
-        <v>96</v>
-      </c>
+      <c r="C55" s="2"/>
       <c r="D55" s="2"/>
-      <c r="E55" s="2" t="s">
-        <v>44</v>
-      </c>
+      <c r="E55" s="9"/>
       <c r="F55" s="2"/>
       <c r="G55" s="2"/>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H55" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I55" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A56" s="5"/>
       <c r="B56" s="8"/>
-      <c r="C56" s="2" t="s">
-        <v>97</v>
-      </c>
+      <c r="C56" s="2"/>
       <c r="D56" s="2"/>
-      <c r="E56" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="F56" s="2" t="s">
-        <v>54</v>
-      </c>
+      <c r="E56" s="2"/>
+      <c r="F56" s="2"/>
       <c r="G56" s="2"/>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A57" s="5"/>
+      <c r="H56" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I56" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A57" s="5" t="s">
+        <v>8</v>
+      </c>
       <c r="B57" s="8"/>
       <c r="C57" s="2" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="D57" s="2"/>
       <c r="E57" s="2" t="s">
-        <v>61</v>
+        <v>42</v>
       </c>
       <c r="F57" s="2"/>
       <c r="G57" s="2"/>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H57">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I57" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A58" s="5"/>
       <c r="B58" s="8"/>
       <c r="C58" s="2" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="D58" s="2"/>
       <c r="E58" s="2" t="s">
-        <v>63</v>
+        <v>43</v>
       </c>
       <c r="F58" s="2"/>
       <c r="G58" s="2"/>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H58">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I58" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A59" s="5"/>
       <c r="B59" s="8"/>
-      <c r="C59" s="2"/>
+      <c r="C59" s="2" t="s">
+        <v>96</v>
+      </c>
       <c r="D59" s="2"/>
-      <c r="E59" s="2"/>
-      <c r="F59" s="2"/>
+      <c r="E59" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F59" s="2" t="s">
+        <v>53</v>
+      </c>
       <c r="G59" s="2"/>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H59">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I59">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A60" s="5"/>
       <c r="B60" s="8"/>
-      <c r="C60" s="2"/>
+      <c r="C60" s="2" t="s">
+        <v>97</v>
+      </c>
       <c r="D60" s="2"/>
-      <c r="E60" s="2"/>
-      <c r="F60" s="2"/>
+      <c r="E60" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="F60" s="2" t="s">
+        <v>99</v>
+      </c>
       <c r="G60" s="2"/>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H60">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I60">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A61" s="5"/>
       <c r="B61" s="8"/>
-      <c r="C61" s="2"/>
+      <c r="C61" s="2" t="s">
+        <v>98</v>
+      </c>
       <c r="D61" s="2"/>
-      <c r="E61" s="2"/>
-      <c r="F61" s="2"/>
+      <c r="E61" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="F61" s="2" t="s">
+        <v>99</v>
+      </c>
       <c r="G61" s="2"/>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A62" s="5" t="s">
-        <v>12</v>
-      </c>
+      <c r="H61">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I61">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A62" s="5"/>
       <c r="B62" s="8"/>
       <c r="C62" s="2"/>
       <c r="D62" s="2"/>
       <c r="E62" s="2"/>
       <c r="F62" s="2"/>
       <c r="G62" s="2"/>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A63" s="2"/>
+      <c r="H62" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I62" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A63" s="5"/>
       <c r="B63" s="8"/>
-      <c r="C63" s="2" t="s">
-        <v>65</v>
-      </c>
+      <c r="C63" s="2"/>
       <c r="D63" s="2"/>
-      <c r="E63" s="2" t="s">
-        <v>66</v>
-      </c>
+      <c r="E63" s="2"/>
       <c r="F63" s="2"/>
       <c r="G63" s="2"/>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A64" s="2"/>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A64" s="5"/>
       <c r="B64" s="8"/>
-      <c r="C64" s="2" t="s">
-        <v>67</v>
-      </c>
+      <c r="C64" s="2"/>
       <c r="D64" s="2"/>
-      <c r="E64" s="2" t="s">
-        <v>68</v>
-      </c>
+      <c r="E64" s="2"/>
       <c r="F64" s="2"/>
       <c r="G64" s="2"/>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A65" s="2"/>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A65" s="5" t="s">
+        <v>11</v>
+      </c>
       <c r="B65" s="8"/>
-      <c r="C65" s="2" t="s">
-        <v>69</v>
-      </c>
+      <c r="C65" s="2"/>
       <c r="D65" s="2"/>
-      <c r="E65" s="2" t="s">
-        <v>70</v>
-      </c>
+      <c r="E65" s="2"/>
       <c r="F65" s="2"/>
       <c r="G65" s="2"/>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A66" s="2"/>
-      <c r="B66" s="2"/>
-      <c r="C66" s="2"/>
+      <c r="B66" s="8"/>
+      <c r="C66" s="2" t="s">
+        <v>64</v>
+      </c>
       <c r="D66" s="2"/>
-      <c r="E66" s="2"/>
+      <c r="E66" s="2" t="s">
+        <v>65</v>
+      </c>
       <c r="F66" s="2"/>
       <c r="G66" s="2"/>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A67" s="2"/>
+      <c r="B67" s="8"/>
+      <c r="C67" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D67" s="2"/>
+      <c r="E67" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="F67" s="2"/>
+      <c r="G67" s="2"/>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A68" s="2"/>
+      <c r="B68" s="8"/>
+      <c r="C68" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D68" s="2"/>
+      <c r="E68" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="F68" s="2"/>
+      <c r="G68" s="2"/>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A69" s="2"/>
+      <c r="B69" s="2"/>
+      <c r="C69" s="2"/>
+      <c r="D69" s="2"/>
+      <c r="E69" s="2"/>
+      <c r="F69" s="2"/>
+      <c r="G69" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
update README with participants list
</commit_message>
<xml_diff>
--- a/planning/workshop-participants.xlsx
+++ b/planning/workshop-participants.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RicardD\Documents\GitHub\ageing-best-practices-2022\planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E304BB7-6B5B-4DEE-A990-9CB27A529031}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{556A65FD-13A7-40C2-A7B7-E743653EBA58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="16440" windowHeight="28440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="133">
   <si>
     <t>Name</t>
   </si>
@@ -412,6 +412,27 @@
   </si>
   <si>
     <t>Daniel.Ricard@dfo-mpo.gc.ca</t>
+  </si>
+  <si>
+    <t>Robichaud, Sylvie</t>
+  </si>
+  <si>
+    <t>Sylvie.Robichaud@dfo-mpo.gc.ca</t>
+  </si>
+  <si>
+    <t>Dionne, Hélène</t>
+  </si>
+  <si>
+    <t>helene.dionne@dfo-mpo.gc.ca</t>
+  </si>
+  <si>
+    <t>andrew.smith4@dfo-mpo.gc.ca</t>
+  </si>
+  <si>
+    <t>In person of virtual?</t>
+  </si>
+  <si>
+    <t>In person</t>
   </si>
 </sst>
 </file>
@@ -774,11 +795,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:I74"/>
+  <dimension ref="A2:K76"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A75" sqref="A75"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -790,12 +809,12 @@
     <col min="6" max="6" width="19.42578125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B3" s="8" t="s">
         <v>4</v>
       </c>
@@ -803,24 +822,24 @@
         <v>106</v>
       </c>
       <c r="G3">
-        <f>SUM(H8:H67)</f>
-        <v>47</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+        <f>SUM(H8:H69)</f>
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B4" s="8"/>
       <c r="F4" s="1" t="s">
         <v>108</v>
       </c>
       <c r="G4">
-        <f>SUM(I8:I67)</f>
+        <f>SUM(I8:I69)</f>
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B5" s="8"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>1</v>
       </c>
@@ -842,11 +861,14 @@
       <c r="I6" s="5" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K6" s="5" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="G7" s="1"/>
     </row>
-    <row r="8" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>5</v>
       </c>
@@ -871,8 +893,11 @@
         <f>IF(LEFT(F8,3)="Yes",1,"")</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K8" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" s="6"/>
       <c r="C9" s="1" t="s">
@@ -886,15 +911,18 @@
       </c>
       <c r="G9" s="1"/>
       <c r="H9">
-        <f t="shared" ref="H9:H67" si="0">IF(ISBLANK(C9), "",1)</f>
+        <f t="shared" ref="H9:H69" si="0">IF(ISBLANK(C9), "",1)</f>
         <v>1</v>
       </c>
       <c r="I9">
-        <f t="shared" ref="I9:I67" si="1">IF(LEFT(F9,3)="Yes",1,"")</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+        <f t="shared" ref="I9:I69" si="1">IF(LEFT(F9,3)="Yes",1,"")</f>
+        <v>1</v>
+      </c>
+      <c r="K9" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="B10" s="6"/>
       <c r="C10" s="1" t="s">
@@ -915,8 +943,11 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K10" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" s="6"/>
       <c r="C11" s="1" t="s">
@@ -937,8 +968,11 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K11" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
       <c r="B12" s="6"/>
       <c r="G12" s="1"/>
@@ -951,7 +985,7 @@
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
       <c r="B13" s="6" t="s">
         <v>10</v>
@@ -974,8 +1008,11 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K13" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="B14" s="6"/>
       <c r="C14" s="1" t="s">
@@ -996,8 +1033,11 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K14" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="6"/>
       <c r="C15" s="1" t="s">
@@ -1018,40 +1058,39 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K15" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="B16" s="6"/>
       <c r="C16" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>18</v>
+        <v>126</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>127</v>
       </c>
       <c r="G16" s="1"/>
       <c r="H16">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="I16">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K16" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
       <c r="B17" s="6"/>
       <c r="C17" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>50</v>
+        <v>71</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>31</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>48</v>
+        <v>18</v>
       </c>
       <c r="G17" s="1"/>
       <c r="H17">
@@ -1062,18 +1101,21 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K17" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="B18" s="6"/>
       <c r="C18" s="1" t="s">
-        <v>111</v>
+        <v>49</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>112</v>
+        <v>50</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>113</v>
+        <v>48</v>
       </c>
       <c r="G18" s="1"/>
       <c r="H18">
@@ -1084,97 +1126,93 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K18" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
       <c r="B19" s="6"/>
       <c r="C19" s="1" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="G19" s="1"/>
       <c r="H19">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I19">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="K19" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
       <c r="B20" s="6"/>
+      <c r="C20" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>116</v>
+      </c>
       <c r="G20" s="1"/>
-      <c r="H20" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="I20" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="21" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B21" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E21" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>53</v>
-      </c>
+      <c r="H20">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="K20" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" s="4"/>
+      <c r="B21" s="6"/>
       <c r="G21" s="1"/>
-      <c r="H21">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="I21">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H21" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
       <c r="B22" s="6"/>
-      <c r="C22" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>48</v>
-      </c>
       <c r="G22" s="1"/>
-      <c r="H22">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="I22">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="4"/>
-      <c r="B23" s="6"/>
+      <c r="H22" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I22" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="23" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>9</v>
+      </c>
       <c r="C23" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>22</v>
+        <v>38</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>37</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>18</v>
+        <v>53</v>
       </c>
       <c r="G23" s="1"/>
       <c r="H23">
@@ -1186,17 +1224,17 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
       <c r="B24" s="6"/>
       <c r="C24" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>19</v>
+        <v>39</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>18</v>
+        <v>48</v>
       </c>
       <c r="G24" s="1"/>
       <c r="H24">
@@ -1208,14 +1246,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
       <c r="B25" s="6"/>
       <c r="C25" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F25" s="1" t="s">
         <v>18</v>
@@ -1230,17 +1268,17 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
       <c r="B26" s="6"/>
-      <c r="C26" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="E26" s="7" t="s">
-        <v>52</v>
+      <c r="C26" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>19</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>53</v>
+        <v>18</v>
       </c>
       <c r="G26" s="1"/>
       <c r="H26">
@@ -1252,32 +1290,39 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
       <c r="B27" s="6"/>
+      <c r="C27" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>18</v>
+      </c>
       <c r="G27" s="1"/>
-      <c r="H27" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="I27" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H27">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I27">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
-      <c r="B28" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>40</v>
+      <c r="B28" s="6"/>
+      <c r="C28" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="E28" s="7" t="s">
+        <v>52</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="G28" s="1"/>
       <c r="H28">
@@ -1289,7 +1334,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
       <c r="B29" s="6"/>
       <c r="G29" s="1"/>
@@ -1302,56 +1347,50 @@
         <v/>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="4"/>
-      <c r="B30" s="6"/>
+      <c r="B30" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>51</v>
+      </c>
       <c r="G30" s="1"/>
-      <c r="H30" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="I30" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" s="4" t="s">
-        <v>7</v>
-      </c>
+      <c r="H30">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I30">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A31" s="4"/>
       <c r="B31" s="6"/>
-      <c r="C31" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F31" s="1" t="s">
-        <v>48</v>
-      </c>
       <c r="G31" s="1"/>
-      <c r="H31">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="I31">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H31" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I31" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="4"/>
       <c r="B32" s="6"/>
-      <c r="C32" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>118</v>
-      </c>
       <c r="G32" s="1"/>
-      <c r="H32">
-        <f t="shared" si="0"/>
-        <v>1</v>
+      <c r="H32" t="str">
+        <f t="shared" si="0"/>
+        <v/>
       </c>
       <c r="I32" t="str">
         <f t="shared" si="1"/>
@@ -1359,14 +1398,26 @@
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" s="4"/>
+      <c r="A33" s="4" t="s">
+        <v>7</v>
+      </c>
       <c r="B33" s="6"/>
       <c r="C33" s="1" t="s">
-        <v>119</v>
+        <v>81</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>48</v>
       </c>
       <c r="G33" s="1"/>
       <c r="H33">
         <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I33">
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -1374,25 +1425,29 @@
       <c r="A34" s="4"/>
       <c r="B34" s="6"/>
       <c r="C34" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="E34" s="9" t="s">
-        <v>123</v>
+        <v>117</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>118</v>
       </c>
       <c r="G34" s="1"/>
       <c r="H34">
         <f t="shared" si="0"/>
         <v>1</v>
+      </c>
+      <c r="I34" t="str">
+        <f t="shared" si="1"/>
+        <v/>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="4"/>
       <c r="B35" s="6"/>
       <c r="C35" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="E35" s="9" t="s">
-        <v>122</v>
+        <v>119</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>130</v>
       </c>
       <c r="G35" s="1"/>
       <c r="H35">
@@ -1403,58 +1458,55 @@
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="4"/>
       <c r="B36" s="6"/>
+      <c r="C36" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="E36" s="9" t="s">
+        <v>123</v>
+      </c>
       <c r="G36" s="1"/>
+      <c r="H36">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="4"/>
       <c r="B37" s="6"/>
+      <c r="C37" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="E37" s="9" t="s">
+        <v>122</v>
+      </c>
       <c r="G37" s="1"/>
-      <c r="H37" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="I37" t="str">
-        <f t="shared" si="1"/>
-        <v/>
+      <c r="H37">
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A38" s="4" t="s">
-        <v>16</v>
-      </c>
+      <c r="A38" s="4"/>
       <c r="B38" s="6"/>
       <c r="C38" s="1" t="s">
-        <v>82</v>
+        <v>128</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F38" s="1" t="s">
-        <v>18</v>
+        <v>129</v>
       </c>
       <c r="G38" s="1"/>
       <c r="H38">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="I38">
-        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="4"/>
       <c r="B39" s="6"/>
-      <c r="C39" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="E39" s="1" t="s">
-        <v>61</v>
-      </c>
       <c r="G39" s="1"/>
-      <c r="H39">
-        <f t="shared" si="0"/>
-        <v>1</v>
+      <c r="H39" t="str">
+        <f t="shared" si="0"/>
+        <v/>
       </c>
       <c r="I39" t="str">
         <f t="shared" si="1"/>
@@ -1462,16 +1514,18 @@
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A40" s="4"/>
+      <c r="A40" s="4" t="s">
+        <v>16</v>
+      </c>
       <c r="B40" s="6"/>
       <c r="C40" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>70</v>
+        <v>17</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>53</v>
+        <v>18</v>
       </c>
       <c r="G40" s="1"/>
       <c r="H40">
@@ -1486,10 +1540,16 @@
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="4"/>
       <c r="B41" s="6"/>
+      <c r="C41" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>61</v>
+      </c>
       <c r="G41" s="1"/>
-      <c r="H41" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+      <c r="H41">
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="I41" t="str">
         <f t="shared" si="1"/>
@@ -1497,18 +1557,16 @@
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A42" s="4" t="s">
-        <v>25</v>
-      </c>
+      <c r="A42" s="4"/>
       <c r="B42" s="6"/>
       <c r="C42" s="1" t="s">
-        <v>26</v>
+        <v>84</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>27</v>
+        <v>70</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>18</v>
+        <v>53</v>
       </c>
       <c r="G42" s="1"/>
       <c r="H42">
@@ -1523,16 +1581,10 @@
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="4"/>
       <c r="B43" s="6"/>
-      <c r="C43" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="E43" s="1" t="s">
-        <v>63</v>
-      </c>
       <c r="G43" s="1"/>
-      <c r="H43">
-        <f t="shared" si="0"/>
-        <v>1</v>
+      <c r="H43" t="str">
+        <f t="shared" si="0"/>
+        <v/>
       </c>
       <c r="I43" t="str">
         <f t="shared" si="1"/>
@@ -1540,25 +1592,42 @@
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A44" s="4"/>
+      <c r="A44" s="4" t="s">
+        <v>25</v>
+      </c>
       <c r="B44" s="6"/>
+      <c r="C44" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>18</v>
+      </c>
       <c r="G44" s="1"/>
-      <c r="H44" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="I44" t="str">
-        <f t="shared" si="1"/>
-        <v/>
+      <c r="H44">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I44">
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="4"/>
       <c r="B45" s="6"/>
+      <c r="C45" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>63</v>
+      </c>
       <c r="G45" s="1"/>
-      <c r="H45" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+      <c r="H45">
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="I45" t="str">
         <f t="shared" si="1"/>
@@ -1566,59 +1635,41 @@
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A46" s="4" t="s">
-        <v>20</v>
-      </c>
+      <c r="A46" s="4"/>
       <c r="B46" s="6"/>
-      <c r="C46" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="E46" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="F46" s="1" t="s">
-        <v>18</v>
-      </c>
       <c r="G46" s="1"/>
-      <c r="H46">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="I46">
-        <f t="shared" si="1"/>
-        <v>1</v>
+      <c r="H46" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I46" t="str">
+        <f t="shared" si="1"/>
+        <v/>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="4"/>
       <c r="B47" s="6"/>
-      <c r="C47" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E47" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="F47" s="1" t="s">
-        <v>18</v>
-      </c>
       <c r="G47" s="1"/>
-      <c r="H47">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="I47">
-        <f t="shared" si="1"/>
-        <v>1</v>
+      <c r="H47" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I47" t="str">
+        <f t="shared" si="1"/>
+        <v/>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A48" s="4"/>
+      <c r="A48" s="4" t="s">
+        <v>20</v>
+      </c>
       <c r="B48" s="6"/>
       <c r="C48" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="E48" s="1" t="s">
-        <v>45</v>
+        <v>86</v>
+      </c>
+      <c r="E48" s="7" t="s">
+        <v>21</v>
       </c>
       <c r="F48" s="1" t="s">
         <v>18</v>
@@ -1636,11 +1687,11 @@
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="4"/>
       <c r="B49" s="6"/>
-      <c r="C49" s="2" t="s">
-        <v>47</v>
+      <c r="C49" s="1" t="s">
+        <v>29</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>46</v>
+        <v>28</v>
       </c>
       <c r="F49" s="1" t="s">
         <v>18</v>
@@ -1659,13 +1710,13 @@
       <c r="A50" s="4"/>
       <c r="B50" s="6"/>
       <c r="C50" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="E50" s="2" t="s">
-        <v>54</v>
+        <v>87</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>45</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>53</v>
+        <v>18</v>
       </c>
       <c r="G50" s="1"/>
       <c r="H50">
@@ -1680,49 +1731,55 @@
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" s="4"/>
       <c r="B51" s="6"/>
-      <c r="C51" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="E51" s="1" t="s">
-        <v>55</v>
+      <c r="C51" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E51" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>18</v>
       </c>
       <c r="G51" s="1"/>
       <c r="H51">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="I51" t="str">
-        <f t="shared" si="1"/>
-        <v/>
+      <c r="I51">
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="4"/>
       <c r="B52" s="6"/>
       <c r="C52" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="E52" s="1" t="s">
-        <v>56</v>
+        <v>88</v>
+      </c>
+      <c r="E52" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="F52" s="1" t="s">
+        <v>53</v>
       </c>
       <c r="G52" s="1"/>
       <c r="H52">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="I52" t="str">
-        <f t="shared" si="1"/>
-        <v/>
+      <c r="I52">
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="4"/>
       <c r="B53" s="6"/>
       <c r="C53" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="G53" s="1"/>
       <c r="H53">
@@ -1738,10 +1795,10 @@
       <c r="A54" s="4"/>
       <c r="B54" s="6"/>
       <c r="C54" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="G54" s="1"/>
       <c r="H54">
@@ -1757,57 +1814,51 @@
       <c r="A55" s="4"/>
       <c r="B55" s="6"/>
       <c r="C55" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="F55" s="1" t="s">
-        <v>110</v>
+        <v>57</v>
       </c>
       <c r="G55" s="1"/>
       <c r="H55">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="I55">
-        <f t="shared" si="1"/>
-        <v>1</v>
+      <c r="I55" t="str">
+        <f t="shared" si="1"/>
+        <v/>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" s="4"/>
       <c r="B56" s="6"/>
       <c r="C56" s="1" t="s">
-        <v>64</v>
+        <v>92</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="F56" s="1" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="G56" s="1"/>
       <c r="H56">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="I56">
-        <f t="shared" si="1"/>
-        <v>1</v>
+      <c r="I56" t="str">
+        <f t="shared" si="1"/>
+        <v/>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" s="4"/>
       <c r="B57" s="6"/>
       <c r="C57" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="E57" s="2" t="s">
-        <v>100</v>
+        <v>93</v>
+      </c>
+      <c r="E57" s="1" t="s">
+        <v>59</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>99</v>
+        <v>110</v>
       </c>
       <c r="G57" s="1"/>
       <c r="H57">
@@ -1823,13 +1874,13 @@
       <c r="A58" s="4"/>
       <c r="B58" s="6"/>
       <c r="C58" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="E58" s="2" t="s">
-        <v>103</v>
+        <v>64</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>65</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>99</v>
+        <v>53</v>
       </c>
       <c r="G58" s="1"/>
       <c r="H58">
@@ -1845,13 +1896,13 @@
       <c r="A59" s="4"/>
       <c r="B59" s="6"/>
       <c r="C59" s="1" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>53</v>
+        <v>99</v>
       </c>
       <c r="G59" s="1"/>
       <c r="H59">
@@ -1866,45 +1917,55 @@
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" s="4"/>
       <c r="B60" s="6"/>
-      <c r="E60" s="2"/>
+      <c r="C60" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="E60" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="F60" s="1" t="s">
+        <v>99</v>
+      </c>
       <c r="G60" s="1"/>
-      <c r="H60" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="I60" t="str">
-        <f t="shared" si="1"/>
-        <v/>
+      <c r="H60">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I60">
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" s="4"/>
       <c r="B61" s="6"/>
+      <c r="C61" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="E61" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="F61" s="1" t="s">
+        <v>53</v>
+      </c>
       <c r="G61" s="1"/>
-      <c r="H61" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="I61" t="str">
-        <f t="shared" si="1"/>
-        <v/>
+      <c r="H61">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I61">
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A62" s="4" t="s">
-        <v>8</v>
-      </c>
+      <c r="A62" s="4"/>
       <c r="B62" s="6"/>
-      <c r="C62" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="E62" s="1" t="s">
-        <v>42</v>
-      </c>
+      <c r="E62" s="2"/>
       <c r="G62" s="1"/>
-      <c r="H62">
-        <f t="shared" si="0"/>
-        <v>1</v>
+      <c r="H62" t="str">
+        <f t="shared" si="0"/>
+        <v/>
       </c>
       <c r="I62" t="str">
         <f t="shared" si="1"/>
@@ -1914,16 +1975,10 @@
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" s="4"/>
       <c r="B63" s="6"/>
-      <c r="C63" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="E63" s="1" t="s">
-        <v>43</v>
-      </c>
       <c r="G63" s="1"/>
-      <c r="H63">
-        <f t="shared" si="0"/>
-        <v>1</v>
+      <c r="H63" t="str">
+        <f t="shared" si="0"/>
+        <v/>
       </c>
       <c r="I63" t="str">
         <f t="shared" si="1"/>
@@ -1931,60 +1986,56 @@
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A64" s="4"/>
+      <c r="A64" s="4" t="s">
+        <v>8</v>
+      </c>
       <c r="B64" s="6"/>
       <c r="C64" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="F64" s="1" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="G64" s="1"/>
       <c r="H64">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="I64">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I64" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A65" s="4"/>
       <c r="B65" s="6"/>
       <c r="C65" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="F65" s="1" t="s">
-        <v>99</v>
+        <v>43</v>
       </c>
       <c r="G65" s="1"/>
       <c r="H65">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="I65">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I65" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66" s="4"/>
       <c r="B66" s="6"/>
       <c r="C66" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>62</v>
+        <v>44</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>99</v>
+        <v>53</v>
       </c>
       <c r="G66" s="1"/>
       <c r="H66">
@@ -1996,74 +2047,124 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67" s="4"/>
       <c r="B67" s="6"/>
+      <c r="C67" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="E67" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="F67" s="1" t="s">
+        <v>99</v>
+      </c>
       <c r="G67" s="1"/>
-      <c r="H67" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="I67" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H67">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I67">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A68" s="4"/>
       <c r="B68" s="6"/>
+      <c r="C68" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="E68" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="F68" s="1" t="s">
+        <v>99</v>
+      </c>
       <c r="G68" s="1"/>
-    </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H68">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I68">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A69" s="4"/>
       <c r="B69" s="6"/>
       <c r="G69" s="1"/>
-    </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A70" s="4" t="s">
-        <v>11</v>
-      </c>
+      <c r="H69" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="I69" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A70" s="4"/>
       <c r="B70" s="6"/>
       <c r="G70" s="1"/>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A71" s="4"/>
       <c r="B71" s="6"/>
-      <c r="C71" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="E71" s="1" t="s">
-        <v>65</v>
-      </c>
       <c r="G71" s="1"/>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A72" s="4" t="s">
+        <v>11</v>
+      </c>
       <c r="B72" s="6"/>
-      <c r="C72" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="E72" s="1" t="s">
-        <v>67</v>
-      </c>
       <c r="G72" s="1"/>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B73" s="6"/>
       <c r="C73" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E73" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G73" s="1"/>
+    </row>
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B74" s="6"/>
+      <c r="C74" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E74" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="G74" s="1"/>
+    </row>
+    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B75" s="6"/>
+      <c r="C75" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="E73" s="1" t="s">
+      <c r="E75" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="G73" s="1"/>
-    </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C74" s="1" t="s">
+      <c r="G75" s="1"/>
+      <c r="K75" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C76" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="E74" s="9" t="s">
+      <c r="E76" s="9" t="s">
         <v>125</v>
       </c>
-      <c r="G74" s="1"/>
+      <c r="G76" s="1"/>
+      <c r="K76" t="s">
+        <v>132</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
add slides to growth modelling presentation
</commit_message>
<xml_diff>
--- a/planning/workshop-participants.xlsx
+++ b/planning/workshop-participants.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RicardD\Documents\GitHub\ageing-best-practices-2022\planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE664CDA-A550-49FA-B0B9-37F52A5D8D1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55D81361-EAAF-4E24-B09A-93719421AACC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="16440" windowHeight="28440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="emails" sheetId="2" r:id="rId2"/>
+    <sheet name="outlook-responses" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="171">
   <si>
     <t>Name</t>
   </si>
@@ -67,15 +68,9 @@
     <t>TESA chair, NCR contact, workshop co-chair</t>
   </si>
   <si>
-    <t xml:space="preserve"> Rolland, Nicolas</t>
-  </si>
-  <si>
     <t>Nicolas.Rolland@dfo-mpo.gc.ca</t>
   </si>
   <si>
-    <t xml:space="preserve"> Sylvain, François-Étienne</t>
-  </si>
-  <si>
     <t>Francois-Etienne.Sylvain@dfo-mpo.gc.ca</t>
   </si>
   <si>
@@ -127,9 +122,6 @@
     <t>Andrew.Darcy@dfo-mpo.gc.ca</t>
   </si>
   <si>
-    <t xml:space="preserve"> Sutton, Jolene</t>
-  </si>
-  <si>
     <t>Jolene.Sutton@dfo-mpo.gc.ca</t>
   </si>
   <si>
@@ -247,9 +239,6 @@
     <t>Savoie, Joeleen</t>
   </si>
   <si>
-    <t>Robertson, Karen  (Gulf)</t>
-  </si>
-  <si>
     <t>McCurdy, Quinn</t>
   </si>
   <si>
@@ -467,6 +456,99 @@
   </si>
   <si>
     <t>Laura.Wheeland@dfo-mpo.gc.ca</t>
+  </si>
+  <si>
+    <t>Virtual</t>
+  </si>
+  <si>
+    <t>Rolland, Nicolas</t>
+  </si>
+  <si>
+    <t>Sylvain, François-Étienne</t>
+  </si>
+  <si>
+    <t>Sutton, Jolene</t>
+  </si>
+  <si>
+    <t>Drover, Dwigth</t>
+  </si>
+  <si>
+    <t>dwight.drover@dfo-mpo.gc.ca</t>
+  </si>
+  <si>
+    <t>Ty, Audrey</t>
+  </si>
+  <si>
+    <t>audrey.ty@dfo-mpo.gc.ca</t>
+  </si>
+  <si>
+    <t>tentative</t>
+  </si>
+  <si>
+    <t>accepted</t>
+  </si>
+  <si>
+    <t>Robertson, Karen</t>
+  </si>
+  <si>
+    <t>hannah.polaczek@dfo-mpo.gc.ca</t>
+  </si>
+  <si>
+    <t>Polaczek, Hannah</t>
+  </si>
+  <si>
+    <t>marc.legresley@dfo-mpo.gc.ca</t>
+  </si>
+  <si>
+    <t>Legresley, Marc</t>
+  </si>
+  <si>
+    <t>Central and Arctic</t>
+  </si>
+  <si>
+    <t>Legge, Michael</t>
+  </si>
+  <si>
+    <t>In person or virtual</t>
+  </si>
+  <si>
+    <t>michael.legge@dfo-mpo.gc.ca</t>
+  </si>
+  <si>
+    <t>Vandenbyllaardt, Lenore</t>
+  </si>
+  <si>
+    <t>lenore.vandenbyllaardt@dfo-mpo.gc.ca</t>
+  </si>
+  <si>
+    <t>Harper, Danni</t>
+  </si>
+  <si>
+    <t>danni.harper@dfo-mpo.gc.ca</t>
+  </si>
+  <si>
+    <t>Hedges, Kevin</t>
+  </si>
+  <si>
+    <t>kevin.hedges@dfo-mpo.gc.ca</t>
+  </si>
+  <si>
+    <t>rick.wastle@dfo-mpo.gc.ca</t>
+  </si>
+  <si>
+    <t>Wastle, Rick</t>
+  </si>
+  <si>
+    <t>region</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>aaron.adamack@dfo-mpo.gc.ca</t>
   </si>
 </sst>
 </file>
@@ -831,64 +913,66 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:H87"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B59" sqref="B59:C59"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="1"/>
-    <col min="2" max="2" width="24.7109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="37.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="25.140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="21.28515625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="12.140625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="11.42578125" customWidth="1"/>
+    <col min="1" max="1" width="9.1796875" style="1"/>
+    <col min="2" max="2" width="24.7265625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="37.7265625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="25.1796875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="21.26953125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="12.1796875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="11.453125" customWidth="1"/>
     <col min="8" max="8" width="11" customWidth="1"/>
-    <col min="9" max="9" width="10.85546875" customWidth="1"/>
-    <col min="10" max="10" width="10.5703125" customWidth="1"/>
+    <col min="9" max="9" width="10.81640625" customWidth="1"/>
+    <col min="10" max="10" width="10.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B2" s="1" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B3" s="7" t="s">
         <v>4</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="F3">
         <f>SUM(E9:E76)</f>
         <v>55</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B4" s="7"/>
       <c r="E4" s="1" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="F4">
         <f>SUM(F9:F76)</f>
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B5" s="7"/>
       <c r="E5" s="1" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="F5">
         <f>SUM(G9:G76)</f>
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B6" s="7"/>
       <c r="F6"/>
     </row>
-    <row r="7" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
         <v>1</v>
       </c>
@@ -902,31 +986,31 @@
         <v>3</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="E8"/>
       <c r="F8"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="E9">
         <v>1</v>
@@ -936,22 +1020,22 @@
         <v>1</v>
       </c>
       <c r="H9" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" s="4"/>
       <c r="B10" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>11</v>
-      </c>
       <c r="D10" s="1" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="E10">
-        <f>IF(ISBLANK(B10), "",1)</f>
+        <f t="shared" ref="E10:E24" si="0">IF(ISBLANK(B10), "",1)</f>
         <v>1</v>
       </c>
       <c r="F10">
@@ -962,186 +1046,186 @@
         <v>1</v>
       </c>
       <c r="H10" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" s="4"/>
       <c r="B11" s="1" t="s">
-        <v>12</v>
+        <v>142</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="E11">
-        <f>IF(ISBLANK(B11), "",1)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="F11">
-        <f t="shared" ref="F11:F76" si="0">IF(LEFT(D11,3)="Yes",1,"")</f>
+        <f t="shared" ref="F11:F76" si="1">IF(LEFT(D11,3)="Yes",1,"")</f>
         <v>1</v>
       </c>
       <c r="G11">
         <v>1</v>
       </c>
       <c r="H11" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" s="4"/>
       <c r="B12" s="1" t="s">
-        <v>30</v>
+        <v>143</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="E12">
-        <f>IF(ISBLANK(B12), "",1)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="F12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="G12">
         <v>1</v>
       </c>
       <c r="H12" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" s="4"/>
       <c r="B13" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="E13">
-        <f>IF(ISBLANK(B13), "",1)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="F13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="G13">
         <v>1</v>
       </c>
       <c r="H13" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" s="4"/>
       <c r="E14" t="str">
-        <f>IF(ISBLANK(B14), "",1)</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="F14" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" s="4"/>
       <c r="B15" s="1" t="s">
-        <v>70</v>
+        <v>150</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="E15">
-        <f>IF(ISBLANK(B15), "",1)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="F15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="G15">
         <v>1</v>
       </c>
       <c r="H15" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" s="4"/>
       <c r="B16" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E16">
-        <f>IF(ISBLANK(B16), "",1)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="F16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="G16">
         <v>0</v>
       </c>
       <c r="H16" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17" s="4"/>
       <c r="B17" s="1" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E17">
-        <f>IF(ISBLANK(B17), "",1)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="F17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="G17">
         <v>0</v>
       </c>
       <c r="H17" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A18" s="4"/>
       <c r="B18" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="E18">
-        <f>IF(ISBLANK(B18), "",1)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="F18"/>
@@ -1149,100 +1233,100 @@
         <v>1</v>
       </c>
       <c r="H18" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A19" s="4"/>
       <c r="B19" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E19">
-        <f>IF(ISBLANK(B19), "",1)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="F19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="G19">
         <v>1</v>
       </c>
       <c r="H19" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A20" s="4"/>
       <c r="B20" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="E20">
-        <f>IF(ISBLANK(B20), "",1)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="F20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="G20">
         <v>1</v>
       </c>
       <c r="H20" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A21" s="4"/>
       <c r="B21" s="1" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="E21">
-        <f>IF(ISBLANK(B21), "",1)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="F21">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="G21">
         <v>1</v>
       </c>
       <c r="H21" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A22" s="4"/>
       <c r="B22" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="E22">
-        <f>IF(ISBLANK(B22), "",1)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="F22"/>
@@ -1250,37 +1334,37 @@
         <v>1</v>
       </c>
       <c r="H22" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A23" s="4"/>
       <c r="E23" t="str">
-        <f>IF(ISBLANK(B23), "",1)</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="F23"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A24" s="4" t="s">
         <v>6</v>
       </c>
       <c r="E24" t="str">
-        <f>IF(ISBLANK(B24), "",1)</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="F24" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A25" s="4"/>
       <c r="B25" s="1" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="E25">
         <v>1</v>
@@ -1290,22 +1374,22 @@
         <v>1</v>
       </c>
       <c r="H25" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A26" s="4"/>
       <c r="B26" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E26">
-        <f>IF(ISBLANK(B26), "",1)</f>
+        <f t="shared" ref="E26:E35" si="2">IF(ISBLANK(B26), "",1)</f>
         <v>1</v>
       </c>
       <c r="F26">
@@ -1316,267 +1400,267 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A27" s="4"/>
       <c r="B27" s="1" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="E27">
-        <f>IF(ISBLANK(B27), "",1)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="F27">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="G27">
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A28" s="4"/>
       <c r="B28" s="1" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E28">
-        <f>IF(ISBLANK(B28), "",1)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="F28">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="G28">
         <v>0</v>
       </c>
       <c r="H28" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A29" s="4"/>
       <c r="B29" s="1" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E29">
-        <f>IF(ISBLANK(B29), "",1)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="F29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="G29">
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A30" s="4"/>
       <c r="B30" s="1" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E30">
-        <f>IF(ISBLANK(B30), "",1)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="F30">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="G30">
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A31" s="4"/>
       <c r="B31" s="2" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E31">
-        <f>IF(ISBLANK(B31), "",1)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="F31">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="G31">
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A32" s="4"/>
       <c r="B32" s="1" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="C32" s="8" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="E32">
-        <f>IF(ISBLANK(B32), "",1)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="F32" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A33" s="4"/>
       <c r="B33" s="1" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="E33">
-        <f>IF(ISBLANK(B33), "",1)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="F33">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="G33">
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A34" s="4"/>
       <c r="B34" s="1" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="C34" s="8" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="E34">
-        <f>IF(ISBLANK(B34), "",1)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="F34" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A35" s="4"/>
       <c r="B35" s="1" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="C35" s="8" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="E35">
-        <f>IF(ISBLANK(B35), "",1)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="F35"/>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A36" s="4"/>
       <c r="C36" s="8"/>
       <c r="E36"/>
       <c r="F36"/>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A37" s="4" t="s">
         <v>7</v>
       </c>
       <c r="E37" t="str">
-        <f>IF(ISBLANK(B37), "",1)</f>
+        <f t="shared" ref="E37:E43" si="3">IF(ISBLANK(B37), "",1)</f>
         <v/>
       </c>
       <c r="F37" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A38" s="4"/>
       <c r="B38" s="1" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="E38">
-        <f>IF(ISBLANK(B38), "",1)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="F38">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="G38">
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A39" s="4"/>
       <c r="B39" s="1" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="E39">
-        <f>IF(ISBLANK(B39), "",1)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="F39" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="G39">
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A40" s="4"/>
       <c r="B40" s="1" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="E40">
-        <f>IF(ISBLANK(B40), "",1)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="F40"/>
@@ -1584,16 +1668,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A41" s="4"/>
       <c r="B41" s="1" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="C41" s="8" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="E41">
-        <f>IF(ISBLANK(B41), "",1)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="F41"/>
@@ -1601,16 +1685,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A42" s="4"/>
       <c r="B42" s="1" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="C42" s="8" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="E42">
-        <f>IF(ISBLANK(B42), "",1)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="F42"/>
@@ -1618,16 +1702,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A43" s="4"/>
       <c r="B43" s="1" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="E43">
-        <f>IF(ISBLANK(B43), "",1)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="F43"/>
@@ -1635,686 +1719,686 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A44" s="4"/>
       <c r="E44"/>
       <c r="F44"/>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A45" s="4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E45" t="str">
         <f>IF(ISBLANK(B45), "",1)</f>
         <v/>
       </c>
       <c r="F45" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A46" s="4"/>
       <c r="B46" s="1" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E46">
         <f>IF(ISBLANK(B46), "",1)</f>
         <v>1</v>
       </c>
       <c r="F46">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="G46">
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A47" s="4"/>
       <c r="B47" s="1" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="E47">
         <f>IF(ISBLANK(B47), "",1)</f>
         <v>1</v>
       </c>
       <c r="F47" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A48" s="4"/>
       <c r="B48" s="1" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E48">
         <f>IF(ISBLANK(B48), "",1)</f>
         <v>1</v>
       </c>
       <c r="F48">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="G48">
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A49" s="4"/>
       <c r="E49"/>
       <c r="F49"/>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A50" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E50" t="str">
-        <f>IF(ISBLANK(B50), "",1)</f>
+        <f t="shared" ref="E50:E76" si="4">IF(ISBLANK(B50), "",1)</f>
         <v/>
       </c>
       <c r="F50" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A51" s="4"/>
       <c r="B51" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E51">
-        <f>IF(ISBLANK(B51), "",1)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="F51">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="G51">
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A52" s="4"/>
       <c r="B52" s="1" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E52">
-        <f>IF(ISBLANK(B52), "",1)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="F52" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A53" s="4"/>
       <c r="E53" t="str">
-        <f>IF(ISBLANK(B53), "",1)</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="F53" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A54" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E54" t="str">
-        <f>IF(ISBLANK(B54), "",1)</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="F54" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A55" s="4"/>
       <c r="B55" s="1" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="C55" s="6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E55">
-        <f>IF(ISBLANK(B55), "",1)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="F55">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="G55">
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A56" s="4"/>
       <c r="B56" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E56">
-        <f>IF(ISBLANK(B56), "",1)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="F56">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="G56">
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A57" s="4"/>
       <c r="B57" s="1" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E57">
-        <f>IF(ISBLANK(B57), "",1)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="F57">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="G57">
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A58" s="4"/>
       <c r="B58" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E58">
-        <f>IF(ISBLANK(B58), "",1)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="F58">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="G58">
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A59" s="4"/>
       <c r="B59" s="1" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E59">
-        <f>IF(ISBLANK(B59), "",1)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="F59">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="G59">
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A60" s="4"/>
       <c r="B60" s="1" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E60">
-        <f>IF(ISBLANK(B60), "",1)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="F60" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A61" s="4"/>
       <c r="B61" s="1" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="E61">
-        <f>IF(ISBLANK(B61), "",1)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="F61" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A62" s="4"/>
       <c r="B62" s="1" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="E62">
-        <f>IF(ISBLANK(B62), "",1)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="F62" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A63" s="4"/>
       <c r="B63" s="1" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E63">
-        <f>IF(ISBLANK(B63), "",1)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="F63" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A64" s="4"/>
       <c r="B64" s="1" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="E64">
-        <f>IF(ISBLANK(B64), "",1)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="F64">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="G64">
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A65" s="4"/>
       <c r="B65" s="1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E65">
-        <f>IF(ISBLANK(B65), "",1)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="F65">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="G65">
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A66" s="4"/>
       <c r="B66" s="1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="E66">
-        <f>IF(ISBLANK(B66), "",1)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="F66">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="G66">
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A67" s="4"/>
       <c r="B67" s="1" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="E67">
-        <f>IF(ISBLANK(B67), "",1)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="F67">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="G67">
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A68" s="4"/>
       <c r="B68" s="1" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E68">
-        <f>IF(ISBLANK(B68), "",1)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="F68">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A69" s="4"/>
       <c r="C69" s="2"/>
       <c r="E69" t="str">
-        <f>IF(ISBLANK(B69), "",1)</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="F69" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A70" s="4" t="s">
         <v>8</v>
       </c>
       <c r="E70" t="str">
-        <f>IF(ISBLANK(B70), "",1)</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="F70" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A71" s="4"/>
       <c r="B71" s="1" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="C71" s="8" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="E71">
-        <f>IF(ISBLANK(B71), "",1)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="F71" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A72" s="4"/>
       <c r="B72" s="1" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E72">
-        <f>IF(ISBLANK(B72), "",1)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="F72" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A73" s="4"/>
       <c r="B73" s="1" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E73">
-        <f>IF(ISBLANK(B73), "",1)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="F73">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="G73">
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A74" s="4"/>
       <c r="B74" s="1" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="E74">
-        <f>IF(ISBLANK(B74), "",1)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="F74">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="G74">
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A75" s="4"/>
       <c r="B75" s="1" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="E75">
-        <f>IF(ISBLANK(B75), "",1)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="F75">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="G75">
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A76" s="4"/>
       <c r="B76" s="1" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="C76" s="8" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="E76">
-        <f>IF(ISBLANK(B76), "",1)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="F76" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="G76">
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A77" s="4"/>
       <c r="E77"/>
       <c r="F77"/>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A78" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E78"/>
       <c r="F78"/>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.35">
       <c r="E79"/>
       <c r="F79"/>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B80" s="1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="E80"/>
       <c r="F80"/>
     </row>
-    <row r="81" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B81" s="1" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="E81"/>
       <c r="F81"/>
     </row>
-    <row r="82" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B82" s="1" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="E82"/>
       <c r="F82"/>
       <c r="H82" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="83" spans="2:8" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="83" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B83" s="1" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="C83" s="8" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="E83"/>
       <c r="F83"/>
       <c r="H83" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="84" spans="2:8" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="84" spans="2:8" x14ac:dyDescent="0.35">
       <c r="E84"/>
       <c r="F84"/>
     </row>
-    <row r="85" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:8" x14ac:dyDescent="0.35">
       <c r="E85"/>
       <c r="F85"/>
     </row>
-    <row r="86" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:8" x14ac:dyDescent="0.35">
       <c r="F86"/>
     </row>
-    <row r="87" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="87" spans="2:8" x14ac:dyDescent="0.35">
       <c r="F87"/>
     </row>
   </sheetData>
@@ -2332,20 +2416,20 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="37.42578125" customWidth="1"/>
+    <col min="1" max="1" width="37.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="B3" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="str">
         <f>IF(Sheet1!E10=1,Sheet1!C10,"")</f>
         <v>Nicolas.Rolland@dfo-mpo.gc.ca</v>
@@ -2355,7 +2439,7 @@
         <v>Nicolas.Rolland@dfo-mpo.gc.ca</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="str">
         <f>IF(Sheet1!E11=1,Sheet1!C11,"")</f>
         <v>Francois-Etienne.Sylvain@dfo-mpo.gc.ca</v>
@@ -2365,7 +2449,7 @@
         <v>Francois-Etienne.Sylvain@dfo-mpo.gc.ca</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="str">
         <f>IF(Sheet1!E12=1,Sheet1!C12,"")</f>
         <v>Jolene.Sutton@dfo-mpo.gc.ca</v>
@@ -2375,7 +2459,7 @@
         <v>Jolene.Sutton@dfo-mpo.gc.ca</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="str">
         <f>IF(Sheet1!E13=1,Sheet1!C13,"")</f>
         <v>Suncica.Avlijas@dfo-mpo.gc.ca</v>
@@ -2385,7 +2469,7 @@
         <v>Suncica.Avlijas@dfo-mpo.gc.ca</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="str">
         <f>IF(Sheet1!E14=1,Sheet1!C14,"")</f>
         <v/>
@@ -2395,7 +2479,7 @@
         <v/>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="str">
         <f>IF(Sheet1!E15=1,Sheet1!C15,"")</f>
         <v>Karen.Robertson@dfo-mpo.gc.ca</v>
@@ -2405,7 +2489,7 @@
         <v>Karen.Robertson@dfo-mpo.gc.ca</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="str">
         <f>IF(Sheet1!E16=1,Sheet1!C16,"")</f>
         <v>Joeleen.Savoie@dfo-mpo.gc.ca</v>
@@ -2415,7 +2499,7 @@
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="str">
         <f>IF(Sheet1!E17=1,Sheet1!C17,"")</f>
         <v>Marie-France.Robichaud@dfo-mpo.gc.ca</v>
@@ -2425,7 +2509,7 @@
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="str">
         <f>IF(Sheet1!E18=1,Sheet1!C18,"")</f>
         <v>Sylvie.Robichaud@dfo-mpo.gc.ca</v>
@@ -2435,7 +2519,7 @@
         <v>Sylvie.Robichaud@dfo-mpo.gc.ca</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="str">
         <f>IF(Sheet1!E19=1,Sheet1!C19,"")</f>
         <v>Andrew.Darcy@dfo-mpo.gc.ca</v>
@@ -2445,7 +2529,7 @@
         <v>Andrew.Darcy@dfo-mpo.gc.ca</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="str">
         <f>IF(Sheet1!E20=1,Sheet1!C20,"")</f>
         <v>abby.daigle@dfo-mpo.gc.ca</v>
@@ -2455,7 +2539,7 @@
         <v>abby.daigle@dfo-mpo.gc.ca</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="str">
         <f>IF(Sheet1!E21=1,Sheet1!C21,"")</f>
         <v>matthew.horsman@dfo-mpo.gc.ca</v>
@@ -2465,7 +2549,7 @@
         <v>matthew.horsman@dfo-mpo.gc.ca</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" t="str">
         <f>IF(Sheet1!E22=1,Sheet1!C22,"")</f>
         <v>kirby.morrill@dfo-mpo.gc.ca</v>
@@ -2475,7 +2559,7 @@
         <v>kirby.morrill@dfo-mpo.gc.ca</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" t="str">
         <f>IF(Sheet1!E23=1,Sheet1!C23,"")</f>
         <v/>
@@ -2485,7 +2569,7 @@
         <v/>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" t="str">
         <f>IF(Sheet1!E24=1,Sheet1!C24,"")</f>
         <v/>
@@ -2495,7 +2579,7 @@
         <v/>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" t="str">
         <f>IF(Sheet1!E25=1,Sheet1!C25,"")</f>
         <v>Peter.Comeau@dfo-mpo.gc.ca</v>
@@ -2505,7 +2589,7 @@
         <v>Peter.Comeau@dfo-mpo.gc.ca</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" t="str">
         <f>IF(Sheet1!E26=1,Sheet1!C26,"")</f>
         <v>Nell.denHeyer@dfo-mpo.gc.ca</v>
@@ -2515,7 +2599,7 @@
         <v>Nell.denHeyer@dfo-mpo.gc.ca</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" t="str">
         <f>IF(Sheet1!E27=1,Sheet1!C27,"")</f>
         <v>Quinn.McCurdy@dfo-mpo.gc.ca</v>
@@ -2525,7 +2609,7 @@
         <v>Quinn.McCurdy@dfo-mpo.gc.ca</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" t="str">
         <f>IF(Sheet1!E28=1,Sheet1!C28,"")</f>
         <v>Dheeraj.Busawon@dfo-mpo.gc.ca</v>
@@ -2535,7 +2619,7 @@
         <v/>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" t="str">
         <f>IF(Sheet1!E29=1,Sheet1!C29,"")</f>
         <v>George.Nau@dfo-mpo.gc.ca</v>
@@ -2545,7 +2629,7 @@
         <v>George.Nau@dfo-mpo.gc.ca</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" t="str">
         <f>IF(Sheet1!E30=1,Sheet1!C30,"")</f>
         <v>Mark.Billard@dfo-mpo.gc.ca</v>
@@ -2555,7 +2639,7 @@
         <v>Mark.Billard@dfo-mpo.gc.ca</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" t="str">
         <f>IF(Sheet1!E31=1,Sheet1!C31,"")</f>
         <v>lynn.collier@dfo-mpo.gc.ca</v>
@@ -2565,7 +2649,7 @@
         <v>lynn.collier@dfo-mpo.gc.ca</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" t="str">
         <f>IF(Sheet1!E32=1,Sheet1!C32,"")</f>
         <v>Kelly.Kraska@dfo-mpo.gc.ca</v>
@@ -2575,7 +2659,7 @@
         <v/>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" t="str">
         <f>IF(Sheet1!E33=1,Sheet1!C33,"")</f>
         <v>Tania.Davignon-Burton@dfo-mpo.gc.ca</v>
@@ -2585,7 +2669,7 @@
         <v>Tania.Davignon-Burton@dfo-mpo.gc.ca</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" t="str">
         <f>IF(Sheet1!E34=1,Sheet1!C34,"")</f>
         <v>Gregory.Puncher@dfo-mpo.gc.ca</v>
@@ -2595,7 +2679,7 @@
         <v/>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" t="str">
         <f>IF(Sheet1!E35=1,Sheet1!C35,"")</f>
         <v>Catriona.Regnier-McKellar@dfo-mpo.gc.ca</v>
@@ -2605,7 +2689,7 @@
         <v/>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30" t="str">
         <f>IF(Sheet1!E36=1,Sheet1!C36,"")</f>
         <v/>
@@ -2615,7 +2699,7 @@
         <v/>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31" t="str">
         <f>IF(Sheet1!E37=1,Sheet1!C37,"")</f>
         <v/>
@@ -2625,7 +2709,7 @@
         <v/>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32" t="str">
         <f>IF(Sheet1!E38=1,Sheet1!C38,"")</f>
         <v>Kim.Emond@dfo-mpo.gc.ca</v>
@@ -2635,7 +2719,7 @@
         <v>Kim.Emond@dfo-mpo.gc.ca</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33" t="str">
         <f>IF(Sheet1!E39=1,Sheet1!C39,"")</f>
         <v>Nicolas.LeCorre@dfo-mpo.gc.ca</v>
@@ -2645,7 +2729,7 @@
         <v>Nicolas.LeCorre@dfo-mpo.gc.ca</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34" t="str">
         <f>IF(Sheet1!E40=1,Sheet1!C40,"")</f>
         <v>andrew.smith4@dfo-mpo.gc.ca</v>
@@ -2655,7 +2739,7 @@
         <v>andrew.smith4@dfo-mpo.gc.ca</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35" t="str">
         <f>IF(Sheet1!E41=1,Sheet1!C41,"")</f>
         <v>Renald.Belley@dfo-mpo.gc.ca</v>
@@ -2665,7 +2749,7 @@
         <v>Renald.Belley@dfo-mpo.gc.ca</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A36" t="str">
         <f>IF(Sheet1!E42=1,Sheet1!C42,"")</f>
         <v>Mathieu.Desgagnes@dfo-mpo.gc.ca</v>
@@ -2675,7 +2759,7 @@
         <v>Mathieu.Desgagnes@dfo-mpo.gc.ca</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A37" t="str">
         <f>IF(Sheet1!E43=1,Sheet1!C43,"")</f>
         <v>helene.dionne@dfo-mpo.gc.ca</v>
@@ -2685,7 +2769,7 @@
         <v>helene.dionne@dfo-mpo.gc.ca</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A38" t="str">
         <f>IF(Sheet1!E44=1,Sheet1!C44,"")</f>
         <v/>
@@ -2695,7 +2779,7 @@
         <v/>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A39" t="str">
         <f>IF(Sheet1!E45=1,Sheet1!C45,"")</f>
         <v/>
@@ -2705,7 +2789,7 @@
         <v/>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A40" t="str">
         <f>IF(Sheet1!E46=1,Sheet1!C46,"")</f>
         <v>Laura.Alsip@dfo-mpo.gc.ca</v>
@@ -2715,7 +2799,7 @@
         <v>Laura.Alsip@dfo-mpo.gc.ca</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A41" t="str">
         <f>IF(Sheet1!E47=1,Sheet1!C47,"")</f>
         <v>Wojciech.Walkusz@dfo-mpo.gc.ca</v>
@@ -2725,7 +2809,7 @@
         <v/>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A42" t="str">
         <f>IF(Sheet1!E48=1,Sheet1!C48,"")</f>
         <v>Lauren.Wiens@dfo-mpo.gc.ca</v>
@@ -2735,7 +2819,7 @@
         <v>Lauren.Wiens@dfo-mpo.gc.ca</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A43" t="str">
         <f>IF(Sheet1!E49=1,Sheet1!C49,"")</f>
         <v/>
@@ -2745,7 +2829,7 @@
         <v/>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A44" t="str">
         <f>IF(Sheet1!E50=1,Sheet1!C50,"")</f>
         <v/>
@@ -2755,7 +2839,7 @@
         <v/>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A45" t="str">
         <f>IF(Sheet1!E51=1,Sheet1!C51,"")</f>
         <v>Tracey.Loewen@dfo-mpo.gc.ca</v>
@@ -2765,7 +2849,7 @@
         <v>Tracey.Loewen@dfo-mpo.gc.ca</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A46" t="str">
         <f>IF(Sheet1!E52=1,Sheet1!C52,"")</f>
         <v>Brendan.Malley@dfo-mpo.gc.ca</v>
@@ -2775,7 +2859,7 @@
         <v/>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A47" t="str">
         <f>IF(Sheet1!E53=1,Sheet1!C53,"")</f>
         <v/>
@@ -2785,7 +2869,7 @@
         <v/>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A48" t="str">
         <f>IF(Sheet1!E54=1,Sheet1!C54,"")</f>
         <v/>
@@ -2795,7 +2879,7 @@
         <v/>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A49" t="str">
         <f>IF(Sheet1!E55=1,Sheet1!C55,"")</f>
         <v>Sarah.Hawkshaw@dfo-mpo.gc.ca</v>
@@ -2805,7 +2889,7 @@
         <v>Sarah.Hawkshaw@dfo-mpo.gc.ca</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A50" t="str">
         <f>IF(Sheet1!E56=1,Sheet1!C56,"")</f>
         <v>Madeline.Lavery@dfo-mpo.gc.ca</v>
@@ -2815,7 +2899,7 @@
         <v>Madeline.Lavery@dfo-mpo.gc.ca</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A51" t="str">
         <f>IF(Sheet1!E57=1,Sheet1!C57,"")</f>
         <v>Emily.Yungwirth@dfo-mpo.gc.ca</v>
@@ -2825,7 +2909,7 @@
         <v>Emily.Yungwirth@dfo-mpo.gc.ca</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A52" t="str">
         <f>IF(Sheet1!E58=1,Sheet1!C58,"")</f>
         <v>dana.haggarty@dfo-mpo.gc.ca</v>
@@ -2835,7 +2919,7 @@
         <v>dana.haggarty@dfo-mpo.gc.ca</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A53" t="str">
         <f>IF(Sheet1!E59=1,Sheet1!C59,"")</f>
         <v>Kendra.Holt@dfo-mpo.gc.ca</v>
@@ -2845,7 +2929,7 @@
         <v>Kendra.Holt@dfo-mpo.gc.ca</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A54" t="str">
         <f>IF(Sheet1!E60=1,Sheet1!C60,"")</f>
         <v>Matthew.Siegle@dfo-mpo.gc.ca</v>
@@ -2855,7 +2939,7 @@
         <v/>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A55" t="str">
         <f>IF(Sheet1!E61=1,Sheet1!C61,"")</f>
         <v>Mackenzie.Mazur@dfo-mpo.gc.ca</v>
@@ -2865,7 +2949,7 @@
         <v/>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A56" t="str">
         <f>IF(Sheet1!E62=1,Sheet1!C62,"")</f>
         <v>Karalea.Cantera@dfo-mpo.gc.ca</v>
@@ -2875,7 +2959,7 @@
         <v/>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A57" t="str">
         <f>IF(Sheet1!E63=1,Sheet1!C63,"")</f>
         <v>Kiana.Matwichuk@dfo-mpo.gc.ca</v>
@@ -2885,7 +2969,7 @@
         <v/>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A58" t="str">
         <f>IF(Sheet1!E64=1,Sheet1!C64,"")</f>
         <v>Erin.Herder@dfo-mpo.gc.ca</v>
@@ -2895,7 +2979,7 @@
         <v>Erin.Herder@dfo-mpo.gc.ca</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A59" t="str">
         <f>IF(Sheet1!E65=1,Sheet1!C65,"")</f>
         <v>Robyn.Forrest@dfo-mpo.gc.ca</v>
@@ -2905,7 +2989,7 @@
         <v>Robyn.Forrest@dfo-mpo.gc.ca</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A60" t="str">
         <f>IF(Sheet1!E66=1,Sheet1!C66,"")</f>
         <v>yeongha.jung@dfo-mpo.gc.ca</v>
@@ -2915,7 +2999,7 @@
         <v>yeongha.jung@dfo-mpo.gc.ca</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A61" t="str">
         <f>IF(Sheet1!E67=1,Sheet1!C67,"")</f>
         <v>barbara.campbell@dfo-mpo.gc.ca</v>
@@ -2925,7 +3009,7 @@
         <v>barbara.campbell@dfo-mpo.gc.ca</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A62" t="str">
         <f>IF(Sheet1!E68=1,Sheet1!C68,"")</f>
         <v>stephen.wischniowski@dfo-mpo.gc.ca</v>
@@ -2935,7 +3019,7 @@
         <v/>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A63" t="str">
         <f>IF(Sheet1!E69=1,Sheet1!C69,"")</f>
         <v/>
@@ -2945,7 +3029,7 @@
         <v/>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A64" t="str">
         <f>IF(Sheet1!E70=1,Sheet1!C70,"")</f>
         <v/>
@@ -2955,7 +3039,7 @@
         <v/>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A65" t="str">
         <f>IF(Sheet1!E71=1,Sheet1!C71,"")</f>
         <v>Gillian.Forbes@dfo-mpo.gc.ca</v>
@@ -2965,7 +3049,7 @@
         <v/>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A66" t="str">
         <f>IF(Sheet1!E72=1,Sheet1!C72,"")</f>
         <v>Divya.Varkey@dfo-mpo.gc.ca</v>
@@ -2975,7 +3059,7 @@
         <v/>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A67" t="str">
         <f>IF(Sheet1!E73=1,Sheet1!C73,"")</f>
         <v>Aaron.Adamack@dfo-mpo.gc.ca</v>
@@ -2985,7 +3069,7 @@
         <v>Aaron.Adamack@dfo-mpo.gc.ca</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A68" t="str">
         <f>IF(Sheet1!E74=1,Sheet1!C74,"")</f>
         <v>Meredith.Schofield@dfo-mpo.gc.ca</v>
@@ -2995,7 +3079,7 @@
         <v>Meredith.Schofield@dfo-mpo.gc.ca</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A69" t="str">
         <f>IF(Sheet1!E75=1,Sheet1!C75,"")</f>
         <v>Andrea.Perreault@dfo-mpo.gc.ca</v>
@@ -3005,7 +3089,7 @@
         <v>Andrea.Perreault@dfo-mpo.gc.ca</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A70" t="str">
         <f>IF(Sheet1!E76=1,Sheet1!C76,"")</f>
         <v>Laura.Wheeland@dfo-mpo.gc.ca</v>
@@ -3015,7 +3099,7 @@
         <v>Laura.Wheeland@dfo-mpo.gc.ca</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A71" t="str">
         <f>IF(Sheet1!E77=1,Sheet1!C77,"")</f>
         <v/>
@@ -3025,7 +3109,7 @@
         <v/>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A72" t="str">
         <f>IF(Sheet1!E78=1,Sheet1!C78,"")</f>
         <v/>
@@ -3035,7 +3119,7 @@
         <v/>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A73" t="str">
         <f>IF(Sheet1!E79=1,Sheet1!C79,"")</f>
         <v/>
@@ -3045,7 +3129,7 @@
         <v/>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A74" t="str">
         <f>IF(Sheet1!E80=1,Sheet1!C80,"")</f>
         <v/>
@@ -3055,7 +3139,7 @@
         <v/>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A75" t="str">
         <f>IF(Sheet1!E81=1,Sheet1!C81,"")</f>
         <v/>
@@ -3065,7 +3149,7 @@
         <v/>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A76" t="str">
         <f>IF(Sheet1!E82=1,Sheet1!C82,"")</f>
         <v/>
@@ -3075,7 +3159,7 @@
         <v/>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A77" t="str">
         <f>IF(Sheet1!E83=1,Sheet1!C83,"")</f>
         <v/>
@@ -3085,10 +3169,590 @@
         <v/>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B78" t="str">
         <f>IF(Sheet1!G88=1,Sheet1!C88,"")</f>
         <v/>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7648514F-C50B-429E-8CE0-7F6A61E6FA38}">
+  <dimension ref="B3:G51"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="A40" sqref="A40"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="4" max="4" width="22.26953125" customWidth="1"/>
+    <col min="6" max="6" width="29.81640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="C3" t="s">
+        <v>167</v>
+      </c>
+      <c r="D3" t="s">
+        <v>168</v>
+      </c>
+      <c r="E3" t="s">
+        <v>169</v>
+      </c>
+      <c r="G3" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B5" t="s">
+        <v>149</v>
+      </c>
+      <c r="C5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="F5" s="2"/>
+      <c r="G5" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B6" t="s">
+        <v>149</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F6" s="2"/>
+      <c r="G6" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B7" t="s">
+        <v>149</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F7" s="2"/>
+      <c r="G7" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B8" t="s">
+        <v>149</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F8" s="2"/>
+      <c r="G8" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="2"/>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="D10" s="1"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="D11" s="1"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B12" t="s">
+        <v>149</v>
+      </c>
+      <c r="C12" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G12" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B13" t="s">
+        <v>149</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="G13" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B14" t="s">
+        <v>149</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="G14" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B15" t="s">
+        <v>149</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="G15" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B16" t="s">
+        <v>148</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="G16" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B17" t="s">
+        <v>149</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="G17" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B18" t="s">
+        <v>149</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="G18" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B19" t="s">
+        <v>149</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="G19" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="D21" s="1"/>
+      <c r="E21" s="2"/>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="D22" s="1"/>
+      <c r="E22" s="2"/>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="D23" s="1"/>
+      <c r="E23" s="2"/>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="D24" s="1"/>
+      <c r="E24" s="6"/>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B25" t="s">
+        <v>149</v>
+      </c>
+      <c r="C25" t="s">
+        <v>6</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G25" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="26" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B26" t="s">
+        <v>149</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="E26" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="G26" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="27" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B27" t="s">
+        <v>149</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G27" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="28" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B28" t="s">
+        <v>149</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G28" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="29" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B29" t="s">
+        <v>149</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="G29" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="30" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B30" t="s">
+        <v>149</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="E30" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="G30" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="31" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B31" t="s">
+        <v>149</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="E31" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="G31" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="32" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="D32" s="1"/>
+      <c r="E32" s="8"/>
+    </row>
+    <row r="34" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B34" t="s">
+        <v>149</v>
+      </c>
+      <c r="C34" t="s">
+        <v>8</v>
+      </c>
+      <c r="D34" t="s">
+        <v>144</v>
+      </c>
+      <c r="E34" t="s">
+        <v>145</v>
+      </c>
+      <c r="G34" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="35" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B35" t="s">
+        <v>149</v>
+      </c>
+      <c r="D35" t="s">
+        <v>152</v>
+      </c>
+      <c r="E35" t="s">
+        <v>151</v>
+      </c>
+      <c r="G35" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="36" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B36" t="s">
+        <v>149</v>
+      </c>
+      <c r="D36" t="s">
+        <v>154</v>
+      </c>
+      <c r="E36" t="s">
+        <v>153</v>
+      </c>
+      <c r="G36" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="37" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B37" t="s">
+        <v>149</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G37" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="38" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B38" t="s">
+        <v>149</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="E38" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="G38" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="39" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B39" t="s">
+        <v>149</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E39" t="s">
+        <v>170</v>
+      </c>
+      <c r="G39" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="41" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B41" t="s">
+        <v>149</v>
+      </c>
+      <c r="C41" t="s">
+        <v>7</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="G41" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="42" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B42" t="s">
+        <v>149</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G42" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="43" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B43" t="s">
+        <v>149</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="G43" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="44" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B44" t="s">
+        <v>149</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="G44" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="45" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B45" t="s">
+        <v>149</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="E45" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="G45" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="47" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B47" t="s">
+        <v>149</v>
+      </c>
+      <c r="C47" t="s">
+        <v>155</v>
+      </c>
+      <c r="D47" t="s">
+        <v>156</v>
+      </c>
+      <c r="E47" t="s">
+        <v>158</v>
+      </c>
+      <c r="G47" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="48" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B48" t="s">
+        <v>149</v>
+      </c>
+      <c r="D48" t="s">
+        <v>159</v>
+      </c>
+      <c r="E48" t="s">
+        <v>160</v>
+      </c>
+      <c r="G48" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="49" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B49" t="s">
+        <v>148</v>
+      </c>
+      <c r="D49" t="s">
+        <v>163</v>
+      </c>
+      <c r="E49" t="s">
+        <v>164</v>
+      </c>
+      <c r="G49" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="50" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B50" t="s">
+        <v>149</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G50" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="51" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B51" t="s">
+        <v>149</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="E51" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="G51" t="s">
+        <v>140</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update README and Excel file of participants
</commit_message>
<xml_diff>
--- a/planning/workshop-participants.xlsx
+++ b/planning/workshop-participants.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RicardD\Documents\GitHub\ageing-best-practices-2022\planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55D81361-EAAF-4E24-B09A-93719421AACC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D00A274-D07B-45DD-A714-D1E088CA77BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="615" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="emails" sheetId="2" r:id="rId2"/>
-    <sheet name="outlook-responses" sheetId="3" r:id="rId3"/>
+    <sheet name="outlook-responses" sheetId="3" r:id="rId1"/>
+    <sheet name="list-pre-google-forms" sheetId="1" r:id="rId2"/>
+    <sheet name="emails" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="198">
   <si>
     <t>Name</t>
   </si>
@@ -482,12 +482,6 @@
     <t>audrey.ty@dfo-mpo.gc.ca</t>
   </si>
   <si>
-    <t>tentative</t>
-  </si>
-  <si>
-    <t>accepted</t>
-  </si>
-  <si>
     <t>Robertson, Karen</t>
   </si>
   <si>
@@ -539,9 +533,6 @@
     <t>Wastle, Rick</t>
   </si>
   <si>
-    <t>region</t>
-  </si>
-  <si>
     <t>name</t>
   </si>
   <si>
@@ -549,6 +540,96 @@
   </si>
   <si>
     <t>aaron.adamack@dfo-mpo.gc.ca</t>
+  </si>
+  <si>
+    <t>Robertson, Karen  (Gulf)</t>
+  </si>
+  <si>
+    <t>Morrill, Kirby</t>
+  </si>
+  <si>
+    <t>Le Corre, Nicolas</t>
+  </si>
+  <si>
+    <t>Smith, Andrew (IML)</t>
+  </si>
+  <si>
+    <t>Drover, Dwight</t>
+  </si>
+  <si>
+    <t>Ty, Audrey (Audrey.Ty@dfo-mpo.gc.ca)</t>
+  </si>
+  <si>
+    <t>Wastle, Rick J</t>
+  </si>
+  <si>
+    <t>Vandenbyllaardt, Lenore J</t>
+  </si>
+  <si>
+    <t>Burke, Lauren (Lauren.Burke@dfo-mpo.gc.ca)</t>
+  </si>
+  <si>
+    <t>Hedges, Kevin J</t>
+  </si>
+  <si>
+    <t>Zhu, Xinhua</t>
+  </si>
+  <si>
+    <t>Lynn.Collier@dfo-mpo.gc.ca</t>
+  </si>
+  <si>
+    <t>Xinhua.Zhu@dfo-mpo.gc.ca</t>
+  </si>
+  <si>
+    <t>Lauren.Burke@dfo-mpo.gc.ca</t>
+  </si>
+  <si>
+    <t>In Person</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Desgagnés, Mathieu </t>
+  </si>
+  <si>
+    <t>Antaya, Kelly</t>
+  </si>
+  <si>
+    <t>Kelly.Antaya@dfo-mpo.gc.ca</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Forest, Isabelle </t>
+  </si>
+  <si>
+    <t>Isabelle.Forest@dfo-mpo.gc.ca</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Horsman, Matthew </t>
+  </si>
+  <si>
+    <t>Matthew.Horsman@dfo-mpo.gc.ca</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Robichaud, Sylvie </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sylvain, François-Étienne </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sutton, Jolene </t>
+  </si>
+  <si>
+    <t>Barbara.Campbell@dfo-mpo.gc.ca</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Forrest, Robyn </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yungwirth, Emily </t>
+  </si>
+  <si>
+    <t>Num.</t>
+  </si>
+  <si>
+    <t>Total</t>
   </si>
 </sst>
 </file>
@@ -910,11 +991,1541 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7648514F-C50B-429E-8CE0-7F6A61E6FA38}">
+  <dimension ref="A2:O66"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="5" max="5" width="22.26953125" customWidth="1"/>
+    <col min="7" max="7" width="29.81640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="L2" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="M2">
+        <f>SUM(M6:M66)</f>
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="B3" t="s">
+        <v>196</v>
+      </c>
+      <c r="D3" t="s">
+        <v>165</v>
+      </c>
+      <c r="E3" t="s">
+        <v>166</v>
+      </c>
+      <c r="G3" t="s">
+        <v>155</v>
+      </c>
+      <c r="L3" t="s">
+        <v>140</v>
+      </c>
+      <c r="M3">
+        <f>SUM(O6:O66)</f>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>197</v>
+      </c>
+      <c r="B4">
+        <f>B6+B18+B32+B42+B51+B58</f>
+        <v>56</v>
+      </c>
+      <c r="L4" t="s">
+        <v>182</v>
+      </c>
+      <c r="M4">
+        <f>SUM(N6:N66)</f>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="N5" t="s">
+        <v>182</v>
+      </c>
+      <c r="O5" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <f>SUM(M6:M16)</f>
+        <v>11</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="F6" s="2"/>
+      <c r="G6" t="s">
+        <v>122</v>
+      </c>
+      <c r="I6" t="s">
+        <v>169</v>
+      </c>
+      <c r="M6">
+        <v>1</v>
+      </c>
+      <c r="N6">
+        <f>IF(G6="In person",1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="O6">
+        <f>IF(G6="Virtual",1,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="D7" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F7" s="2"/>
+      <c r="G7" t="s">
+        <v>122</v>
+      </c>
+      <c r="I7" t="s">
+        <v>43</v>
+      </c>
+      <c r="M7">
+        <v>1</v>
+      </c>
+      <c r="N7">
+        <f>IF(G7="In person",1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="O7">
+        <f>IF(G7="Virtual",1,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="D8" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F8" s="2"/>
+      <c r="G8" t="s">
+        <v>122</v>
+      </c>
+      <c r="I8" t="s">
+        <v>168</v>
+      </c>
+      <c r="M8">
+        <v>1</v>
+      </c>
+      <c r="N8">
+        <f>IF(G8="In person",1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="O8">
+        <f>IF(G8="Virtual",1,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="D9" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F9" s="2"/>
+      <c r="G9" t="s">
+        <v>122</v>
+      </c>
+      <c r="I9" t="s">
+        <v>29</v>
+      </c>
+      <c r="M9">
+        <v>1</v>
+      </c>
+      <c r="N9">
+        <f>IF(G9="In person",1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="O9">
+        <f>IF(G9="Virtual",1,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="D10" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="F10" s="2"/>
+      <c r="G10" t="s">
+        <v>122</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="M10">
+        <v>1</v>
+      </c>
+      <c r="N10">
+        <f>IF(G10="In person",1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="O10">
+        <f>IF(G10="Virtual",1,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="D11" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>187</v>
+      </c>
+      <c r="F11" s="2"/>
+      <c r="G11" t="s">
+        <v>122</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="M11">
+        <v>1</v>
+      </c>
+      <c r="N11">
+        <f>IF(G11="In person",1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="O11">
+        <f>IF(G11="Virtual",1,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="D12" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>189</v>
+      </c>
+      <c r="F12" s="2"/>
+      <c r="G12" t="s">
+        <v>122</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="M12">
+        <v>1</v>
+      </c>
+      <c r="N12">
+        <f>IF(G12="In person",1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="O12">
+        <f>IF(G12="Virtual",1,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="D13" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="F13" s="2"/>
+      <c r="G13" t="s">
+        <v>122</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="M13">
+        <v>1</v>
+      </c>
+      <c r="N13">
+        <f>IF(G13="In person",1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="O13">
+        <f>IF(G13="Virtual",1,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="D14" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F14" s="2"/>
+      <c r="G14" t="s">
+        <v>122</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="M14">
+        <v>1</v>
+      </c>
+      <c r="N14">
+        <f>IF(G14="In person",1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="O14">
+        <f>IF(G14="Virtual",1,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="D15" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F15" s="2"/>
+      <c r="G15" t="s">
+        <v>122</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="M15">
+        <v>1</v>
+      </c>
+      <c r="N15">
+        <f>IF(G15="In person",1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="O15">
+        <f>IF(G15="Virtual",1,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="D16" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="F16" s="2"/>
+      <c r="G16" t="s">
+        <v>122</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="M16">
+        <v>1</v>
+      </c>
+      <c r="N16">
+        <f>IF(G16="In person",1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="O16">
+        <f>IF(G16="Virtual",1,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="D17" s="1"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18">
+        <f>SUM(M18:M30)</f>
+        <v>13</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G18" t="s">
+        <v>140</v>
+      </c>
+      <c r="I18" t="s">
+        <v>84</v>
+      </c>
+      <c r="M18">
+        <v>1</v>
+      </c>
+      <c r="N18">
+        <f>IF(G18="In person",1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="O18">
+        <f>IF(G18="Virtual",1,0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="D19" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="G19" t="s">
+        <v>140</v>
+      </c>
+      <c r="I19" t="s">
+        <v>85</v>
+      </c>
+      <c r="M19">
+        <v>1</v>
+      </c>
+      <c r="N19">
+        <f>IF(G19="In person",1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="O19">
+        <f t="shared" ref="O19:O30" si="0">IF(G19="Virtual",1,0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="D20" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="G20" t="s">
+        <v>140</v>
+      </c>
+      <c r="I20" t="s">
+        <v>78</v>
+      </c>
+      <c r="M20">
+        <v>1</v>
+      </c>
+      <c r="N20">
+        <f>IF(G20="In person",1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="O20">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="D21" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="G21" t="s">
+        <v>140</v>
+      </c>
+      <c r="I21" t="s">
+        <v>83</v>
+      </c>
+      <c r="M21">
+        <v>1</v>
+      </c>
+      <c r="N21">
+        <f>IF(G21="In person",1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="O21">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="D22" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="G22" t="s">
+        <v>140</v>
+      </c>
+      <c r="I22" t="s">
+        <v>173</v>
+      </c>
+      <c r="M22">
+        <v>1</v>
+      </c>
+      <c r="N22">
+        <f>IF(G22="In person",1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="O22">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="D23" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="G23" t="s">
+        <v>140</v>
+      </c>
+      <c r="I23" t="s">
+        <v>92</v>
+      </c>
+      <c r="M23">
+        <v>1</v>
+      </c>
+      <c r="N23">
+        <f>IF(G23="In person",1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="O23">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="D24" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="G24" t="s">
+        <v>140</v>
+      </c>
+      <c r="I24" t="s">
+        <v>80</v>
+      </c>
+      <c r="M24">
+        <v>1</v>
+      </c>
+      <c r="N24">
+        <f>IF(G24="In person",1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="O24">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="D25" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E25" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="G25" t="s">
+        <v>122</v>
+      </c>
+      <c r="I25" t="s">
+        <v>82</v>
+      </c>
+      <c r="M25">
+        <v>1</v>
+      </c>
+      <c r="N25">
+        <f>IF(G25="In person",1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="O25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="D26" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="E26" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="G26" t="s">
+        <v>140</v>
+      </c>
+      <c r="I26" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="M26">
+        <v>1</v>
+      </c>
+      <c r="N26">
+        <f>IF(G26="In person",1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="O26">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="D27" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="E27" s="8" t="s">
+        <v>193</v>
+      </c>
+      <c r="G27" t="s">
+        <v>140</v>
+      </c>
+      <c r="I27" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="M27">
+        <v>1</v>
+      </c>
+      <c r="N27">
+        <f>IF(G27="In person",1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="O27">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="D28" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="E28" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="G28" t="s">
+        <v>140</v>
+      </c>
+      <c r="I28" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="M28">
+        <v>1</v>
+      </c>
+      <c r="N28">
+        <f>IF(G28="In person",1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="O28">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="D29" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="E29" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="G29" t="s">
+        <v>140</v>
+      </c>
+      <c r="I29" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="M29">
+        <v>1</v>
+      </c>
+      <c r="N29">
+        <f>IF(G29="In person",1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="O29">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="D30" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E30" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="G30" t="s">
+        <v>140</v>
+      </c>
+      <c r="I30" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="M30">
+        <v>1</v>
+      </c>
+      <c r="N30">
+        <f>IF(G30="In person",1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="O30">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="D31" s="1"/>
+      <c r="E31" s="6"/>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>6</v>
+      </c>
+      <c r="B32">
+        <f>SUM(M32:M40)</f>
+        <v>9</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G32" t="s">
+        <v>140</v>
+      </c>
+      <c r="I32" t="s">
+        <v>70</v>
+      </c>
+      <c r="M32">
+        <v>1</v>
+      </c>
+      <c r="N32">
+        <f>IF(G32="In person",1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="O32">
+        <f t="shared" ref="O32:O40" si="1">IF(G32="Virtual",1,0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="D33" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="E33" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="G33" t="s">
+        <v>140</v>
+      </c>
+      <c r="I33" t="s">
+        <v>130</v>
+      </c>
+      <c r="M33">
+        <v>1</v>
+      </c>
+      <c r="N33">
+        <f>IF(G33="In person",1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="O33">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="D34" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G34" t="s">
+        <v>122</v>
+      </c>
+      <c r="I34" t="s">
+        <v>72</v>
+      </c>
+      <c r="M34">
+        <v>1</v>
+      </c>
+      <c r="N34">
+        <f>IF(G34="In person",1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="O34">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="D35" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G35" t="s">
+        <v>140</v>
+      </c>
+      <c r="I35" t="s">
+        <v>32</v>
+      </c>
+      <c r="M35">
+        <v>1</v>
+      </c>
+      <c r="N35">
+        <f>IF(G35="In person",1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="O35">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="D36" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="G36" t="s">
+        <v>140</v>
+      </c>
+      <c r="I36" t="s">
+        <v>159</v>
+      </c>
+      <c r="M36">
+        <v>1</v>
+      </c>
+      <c r="N36">
+        <f>IF(G36="In person",1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="O36">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="D37" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="E37" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="G37" t="s">
+        <v>140</v>
+      </c>
+      <c r="I37" t="s">
+        <v>129</v>
+      </c>
+      <c r="M37">
+        <v>1</v>
+      </c>
+      <c r="N37">
+        <f>IF(G37="In person",1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="O37">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="D38" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="E38" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="G38" t="s">
+        <v>122</v>
+      </c>
+      <c r="M38">
+        <v>1</v>
+      </c>
+      <c r="N38">
+        <f>IF(G38="In person",1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="O38">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="D39" t="s">
+        <v>69</v>
+      </c>
+      <c r="E39" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="G39" t="s">
+        <v>122</v>
+      </c>
+      <c r="I39" t="s">
+        <v>69</v>
+      </c>
+      <c r="M39">
+        <v>1</v>
+      </c>
+      <c r="N39">
+        <f>IF(G39="In person",1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="O39">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="D40" t="s">
+        <v>71</v>
+      </c>
+      <c r="E40" t="s">
+        <v>179</v>
+      </c>
+      <c r="G40" t="s">
+        <v>140</v>
+      </c>
+      <c r="I40" t="s">
+        <v>71</v>
+      </c>
+      <c r="M40">
+        <v>1</v>
+      </c>
+      <c r="N40">
+        <f>IF(G40="In person",1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="O40">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
+        <v>8</v>
+      </c>
+      <c r="B42">
+        <f>SUM(M42:M49)</f>
+        <v>8</v>
+      </c>
+      <c r="D42" t="s">
+        <v>144</v>
+      </c>
+      <c r="E42" t="s">
+        <v>145</v>
+      </c>
+      <c r="G42" t="s">
+        <v>140</v>
+      </c>
+      <c r="I42" t="s">
+        <v>172</v>
+      </c>
+      <c r="M42">
+        <v>1</v>
+      </c>
+      <c r="N42">
+        <f>IF(G42="In person",1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="O42">
+        <f t="shared" ref="O42:O66" si="2">IF(G42="Virtual",1,0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="D43" t="s">
+        <v>150</v>
+      </c>
+      <c r="E43" t="s">
+        <v>149</v>
+      </c>
+      <c r="G43" t="s">
+        <v>140</v>
+      </c>
+      <c r="I43" t="s">
+        <v>150</v>
+      </c>
+      <c r="M43">
+        <v>1</v>
+      </c>
+      <c r="N43">
+        <f>IF(G43="In person",1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="O43">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="D44" t="s">
+        <v>152</v>
+      </c>
+      <c r="E44" t="s">
+        <v>151</v>
+      </c>
+      <c r="G44" t="s">
+        <v>140</v>
+      </c>
+      <c r="I44" t="s">
+        <v>152</v>
+      </c>
+      <c r="M44">
+        <v>1</v>
+      </c>
+      <c r="N44">
+        <f>IF(G44="In person",1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="O44">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="D45" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G45" t="s">
+        <v>122</v>
+      </c>
+      <c r="I45" t="s">
+        <v>88</v>
+      </c>
+      <c r="M45">
+        <v>1</v>
+      </c>
+      <c r="N45">
+        <f>IF(G45="In person",1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="O45">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="D46" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="E46" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="G46" t="s">
+        <v>122</v>
+      </c>
+      <c r="I46" t="s">
+        <v>136</v>
+      </c>
+      <c r="M46">
+        <v>1</v>
+      </c>
+      <c r="N46">
+        <f>IF(G46="In person",1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="O46">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="D47" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E47" t="s">
+        <v>167</v>
+      </c>
+      <c r="G47" t="s">
+        <v>140</v>
+      </c>
+      <c r="I47" t="s">
+        <v>87</v>
+      </c>
+      <c r="M47">
+        <v>1</v>
+      </c>
+      <c r="N47">
+        <f>IF(G47="In person",1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="O47">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="D48" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="E48" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="G48" t="s">
+        <v>140</v>
+      </c>
+      <c r="I48" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="M48">
+        <v>1</v>
+      </c>
+      <c r="N48">
+        <f>IF(G48="In person",1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="O48">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="D49" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="E49" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="G49" t="s">
+        <v>140</v>
+      </c>
+      <c r="I49" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="M49">
+        <v>1</v>
+      </c>
+      <c r="N49">
+        <f>IF(G49="In person",1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="O49">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A51" t="s">
+        <v>7</v>
+      </c>
+      <c r="B51">
+        <f>SUM(M51:M56)</f>
+        <v>6</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="G51" t="s">
+        <v>140</v>
+      </c>
+      <c r="I51" t="s">
+        <v>171</v>
+      </c>
+      <c r="M51">
+        <v>1</v>
+      </c>
+      <c r="N51">
+        <f>IF(G51="In person",1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="O51">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="D52" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G52" t="s">
+        <v>122</v>
+      </c>
+      <c r="I52" t="s">
+        <v>73</v>
+      </c>
+      <c r="M52">
+        <v>1</v>
+      </c>
+      <c r="N52">
+        <f>IF(G52="In person",1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="O52">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="D53" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="G53" t="s">
+        <v>140</v>
+      </c>
+      <c r="I53" t="s">
+        <v>170</v>
+      </c>
+      <c r="M53">
+        <v>1</v>
+      </c>
+      <c r="N53">
+        <f>IF(G53="In person",1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="O53">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="D54" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="G54" t="s">
+        <v>122</v>
+      </c>
+      <c r="I54" t="s">
+        <v>118</v>
+      </c>
+      <c r="M54">
+        <v>1</v>
+      </c>
+      <c r="N54">
+        <f>IF(G54="In person",1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="O54">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="D55" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="E55" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="G55" t="s">
+        <v>140</v>
+      </c>
+      <c r="I55" t="s">
+        <v>110</v>
+      </c>
+      <c r="M55">
+        <v>1</v>
+      </c>
+      <c r="N55">
+        <f>IF(G55="In person",1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="O55">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="D56" t="s">
+        <v>183</v>
+      </c>
+      <c r="E56" t="s">
+        <v>112</v>
+      </c>
+      <c r="G56" t="s">
+        <v>140</v>
+      </c>
+      <c r="I56" t="s">
+        <v>183</v>
+      </c>
+      <c r="M56">
+        <v>1</v>
+      </c>
+      <c r="N56">
+        <f>IF(G56="In person",1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="O56">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A58" t="s">
+        <v>153</v>
+      </c>
+      <c r="B58">
+        <f>SUM(M58:M66)</f>
+        <v>9</v>
+      </c>
+      <c r="D58" t="s">
+        <v>154</v>
+      </c>
+      <c r="E58" t="s">
+        <v>156</v>
+      </c>
+      <c r="G58" t="s">
+        <v>122</v>
+      </c>
+      <c r="I58" t="s">
+        <v>154</v>
+      </c>
+      <c r="M58">
+        <v>1</v>
+      </c>
+      <c r="N58">
+        <f>IF(G58="In person",1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="O58">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="D59" t="s">
+        <v>157</v>
+      </c>
+      <c r="E59" t="s">
+        <v>158</v>
+      </c>
+      <c r="G59" t="s">
+        <v>140</v>
+      </c>
+      <c r="I59" t="s">
+        <v>175</v>
+      </c>
+      <c r="M59">
+        <v>1</v>
+      </c>
+      <c r="N59">
+        <f>IF(G59="In person",1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="O59">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="D60" t="s">
+        <v>161</v>
+      </c>
+      <c r="E60" t="s">
+        <v>162</v>
+      </c>
+      <c r="G60" t="s">
+        <v>140</v>
+      </c>
+      <c r="I60" t="s">
+        <v>177</v>
+      </c>
+      <c r="M60">
+        <v>1</v>
+      </c>
+      <c r="N60">
+        <f>IF(G60="In person",1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="O60">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="D61" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G61" t="s">
+        <v>122</v>
+      </c>
+      <c r="I61" t="s">
+        <v>22</v>
+      </c>
+      <c r="M61">
+        <v>1</v>
+      </c>
+      <c r="N61">
+        <f>IF(G61="In person",1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="O61">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="D62" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="E62" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="G62" t="s">
+        <v>140</v>
+      </c>
+      <c r="I62" t="s">
+        <v>174</v>
+      </c>
+      <c r="M62">
+        <v>1</v>
+      </c>
+      <c r="N62">
+        <f>IF(G62="In person",1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="O62">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="D63" t="s">
+        <v>178</v>
+      </c>
+      <c r="E63" t="s">
+        <v>180</v>
+      </c>
+      <c r="G63" t="s">
+        <v>140</v>
+      </c>
+      <c r="I63" t="s">
+        <v>178</v>
+      </c>
+      <c r="M63">
+        <v>1</v>
+      </c>
+      <c r="N63">
+        <f>IF(G63="In person",1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="O63">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="D64" t="s">
+        <v>77</v>
+      </c>
+      <c r="E64" t="s">
+        <v>57</v>
+      </c>
+      <c r="G64" t="s">
+        <v>140</v>
+      </c>
+      <c r="I64" t="s">
+        <v>77</v>
+      </c>
+      <c r="M64">
+        <v>1</v>
+      </c>
+      <c r="N64">
+        <f t="shared" ref="N64:N66" si="3">IF(G64="In person",1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="O64">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="4:15" x14ac:dyDescent="0.35">
+      <c r="D65" t="s">
+        <v>176</v>
+      </c>
+      <c r="E65" t="s">
+        <v>181</v>
+      </c>
+      <c r="G65" t="s">
+        <v>140</v>
+      </c>
+      <c r="I65" t="s">
+        <v>176</v>
+      </c>
+      <c r="M65">
+        <v>1</v>
+      </c>
+      <c r="N65">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="O65">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="4:15" x14ac:dyDescent="0.35">
+      <c r="D66" t="s">
+        <v>74</v>
+      </c>
+      <c r="E66" t="s">
+        <v>13</v>
+      </c>
+      <c r="G66" t="s">
+        <v>140</v>
+      </c>
+      <c r="I66" t="s">
+        <v>74</v>
+      </c>
+      <c r="M66">
+        <v>1</v>
+      </c>
+      <c r="N66">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="O66">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:H87"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B59" sqref="B59:C59"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E5" sqref="E5:F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1141,7 +2752,7 @@
     <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" s="4"/>
       <c r="B15" s="1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>31</v>
@@ -2410,7 +4021,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A495CC8-2D75-4904-B60D-B994B74791C5}">
   <dimension ref="A3:B78"/>
   <sheetViews>
@@ -2431,1328 +4042,748 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="str">
-        <f>IF(Sheet1!E10=1,Sheet1!C10,"")</f>
+        <f>IF('list-pre-google-forms'!E10=1,'list-pre-google-forms'!C10,"")</f>
         <v>Nicolas.Rolland@dfo-mpo.gc.ca</v>
       </c>
       <c r="B4" t="str">
-        <f>IF(Sheet1!G10=1,Sheet1!C10,"")</f>
+        <f>IF('list-pre-google-forms'!G10=1,'list-pre-google-forms'!C10,"")</f>
         <v>Nicolas.Rolland@dfo-mpo.gc.ca</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="str">
-        <f>IF(Sheet1!E11=1,Sheet1!C11,"")</f>
+        <f>IF('list-pre-google-forms'!E11=1,'list-pre-google-forms'!C11,"")</f>
         <v>Francois-Etienne.Sylvain@dfo-mpo.gc.ca</v>
       </c>
       <c r="B5" t="str">
-        <f>IF(Sheet1!G11=1,Sheet1!C11,"")</f>
+        <f>IF('list-pre-google-forms'!G11=1,'list-pre-google-forms'!C11,"")</f>
         <v>Francois-Etienne.Sylvain@dfo-mpo.gc.ca</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="str">
-        <f>IF(Sheet1!E12=1,Sheet1!C12,"")</f>
+        <f>IF('list-pre-google-forms'!E12=1,'list-pre-google-forms'!C12,"")</f>
         <v>Jolene.Sutton@dfo-mpo.gc.ca</v>
       </c>
       <c r="B6" t="str">
-        <f>IF(Sheet1!G12=1,Sheet1!C12,"")</f>
+        <f>IF('list-pre-google-forms'!G12=1,'list-pre-google-forms'!C12,"")</f>
         <v>Jolene.Sutton@dfo-mpo.gc.ca</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="str">
-        <f>IF(Sheet1!E13=1,Sheet1!C13,"")</f>
+        <f>IF('list-pre-google-forms'!E13=1,'list-pre-google-forms'!C13,"")</f>
         <v>Suncica.Avlijas@dfo-mpo.gc.ca</v>
       </c>
       <c r="B7" t="str">
-        <f>IF(Sheet1!G13=1,Sheet1!C13,"")</f>
+        <f>IF('list-pre-google-forms'!G13=1,'list-pre-google-forms'!C13,"")</f>
         <v>Suncica.Avlijas@dfo-mpo.gc.ca</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="str">
-        <f>IF(Sheet1!E14=1,Sheet1!C14,"")</f>
+        <f>IF('list-pre-google-forms'!E14=1,'list-pre-google-forms'!C14,"")</f>
         <v/>
       </c>
       <c r="B8" t="str">
-        <f>IF(Sheet1!G14=1,Sheet1!C14,"")</f>
+        <f>IF('list-pre-google-forms'!G14=1,'list-pre-google-forms'!C14,"")</f>
         <v/>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="str">
-        <f>IF(Sheet1!E15=1,Sheet1!C15,"")</f>
+        <f>IF('list-pre-google-forms'!E15=1,'list-pre-google-forms'!C15,"")</f>
         <v>Karen.Robertson@dfo-mpo.gc.ca</v>
       </c>
       <c r="B9" t="str">
-        <f>IF(Sheet1!G15=1,Sheet1!C15,"")</f>
+        <f>IF('list-pre-google-forms'!G15=1,'list-pre-google-forms'!C15,"")</f>
         <v>Karen.Robertson@dfo-mpo.gc.ca</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="str">
-        <f>IF(Sheet1!E16=1,Sheet1!C16,"")</f>
+        <f>IF('list-pre-google-forms'!E16=1,'list-pre-google-forms'!C16,"")</f>
         <v>Joeleen.Savoie@dfo-mpo.gc.ca</v>
       </c>
       <c r="B10" t="str">
-        <f>IF(Sheet1!G16=1,Sheet1!C16,"")</f>
+        <f>IF('list-pre-google-forms'!G16=1,'list-pre-google-forms'!C16,"")</f>
         <v/>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="str">
-        <f>IF(Sheet1!E17=1,Sheet1!C17,"")</f>
+        <f>IF('list-pre-google-forms'!E17=1,'list-pre-google-forms'!C17,"")</f>
         <v>Marie-France.Robichaud@dfo-mpo.gc.ca</v>
       </c>
       <c r="B11" t="str">
-        <f>IF(Sheet1!G17=1,Sheet1!C17,"")</f>
+        <f>IF('list-pre-google-forms'!G17=1,'list-pre-google-forms'!C17,"")</f>
         <v/>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="str">
-        <f>IF(Sheet1!E18=1,Sheet1!C18,"")</f>
+        <f>IF('list-pre-google-forms'!E18=1,'list-pre-google-forms'!C18,"")</f>
         <v>Sylvie.Robichaud@dfo-mpo.gc.ca</v>
       </c>
       <c r="B12" t="str">
-        <f>IF(Sheet1!G18=1,Sheet1!C18,"")</f>
+        <f>IF('list-pre-google-forms'!G18=1,'list-pre-google-forms'!C18,"")</f>
         <v>Sylvie.Robichaud@dfo-mpo.gc.ca</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="str">
-        <f>IF(Sheet1!E19=1,Sheet1!C19,"")</f>
+        <f>IF('list-pre-google-forms'!E19=1,'list-pre-google-forms'!C19,"")</f>
         <v>Andrew.Darcy@dfo-mpo.gc.ca</v>
       </c>
       <c r="B13" t="str">
-        <f>IF(Sheet1!G19=1,Sheet1!C19,"")</f>
+        <f>IF('list-pre-google-forms'!G19=1,'list-pre-google-forms'!C19,"")</f>
         <v>Andrew.Darcy@dfo-mpo.gc.ca</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="str">
-        <f>IF(Sheet1!E20=1,Sheet1!C20,"")</f>
+        <f>IF('list-pre-google-forms'!E20=1,'list-pre-google-forms'!C20,"")</f>
         <v>abby.daigle@dfo-mpo.gc.ca</v>
       </c>
       <c r="B14" t="str">
-        <f>IF(Sheet1!G20=1,Sheet1!C20,"")</f>
+        <f>IF('list-pre-google-forms'!G20=1,'list-pre-google-forms'!C20,"")</f>
         <v>abby.daigle@dfo-mpo.gc.ca</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="str">
-        <f>IF(Sheet1!E21=1,Sheet1!C21,"")</f>
+        <f>IF('list-pre-google-forms'!E21=1,'list-pre-google-forms'!C21,"")</f>
         <v>matthew.horsman@dfo-mpo.gc.ca</v>
       </c>
       <c r="B15" t="str">
-        <f>IF(Sheet1!G21=1,Sheet1!C21,"")</f>
+        <f>IF('list-pre-google-forms'!G21=1,'list-pre-google-forms'!C21,"")</f>
         <v>matthew.horsman@dfo-mpo.gc.ca</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" t="str">
-        <f>IF(Sheet1!E22=1,Sheet1!C22,"")</f>
+        <f>IF('list-pre-google-forms'!E22=1,'list-pre-google-forms'!C22,"")</f>
         <v>kirby.morrill@dfo-mpo.gc.ca</v>
       </c>
       <c r="B16" t="str">
-        <f>IF(Sheet1!G22=1,Sheet1!C22,"")</f>
+        <f>IF('list-pre-google-forms'!G22=1,'list-pre-google-forms'!C22,"")</f>
         <v>kirby.morrill@dfo-mpo.gc.ca</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" t="str">
-        <f>IF(Sheet1!E23=1,Sheet1!C23,"")</f>
+        <f>IF('list-pre-google-forms'!E23=1,'list-pre-google-forms'!C23,"")</f>
         <v/>
       </c>
       <c r="B17" t="str">
-        <f>IF(Sheet1!G23=1,Sheet1!C23,"")</f>
+        <f>IF('list-pre-google-forms'!G23=1,'list-pre-google-forms'!C23,"")</f>
         <v/>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" t="str">
-        <f>IF(Sheet1!E24=1,Sheet1!C24,"")</f>
+        <f>IF('list-pre-google-forms'!E24=1,'list-pre-google-forms'!C24,"")</f>
         <v/>
       </c>
       <c r="B18" t="str">
-        <f>IF(Sheet1!G24=1,Sheet1!C24,"")</f>
+        <f>IF('list-pre-google-forms'!G24=1,'list-pre-google-forms'!C24,"")</f>
         <v/>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" t="str">
-        <f>IF(Sheet1!E25=1,Sheet1!C25,"")</f>
+        <f>IF('list-pre-google-forms'!E25=1,'list-pre-google-forms'!C25,"")</f>
         <v>Peter.Comeau@dfo-mpo.gc.ca</v>
       </c>
       <c r="B19" t="str">
-        <f>IF(Sheet1!G25=1,Sheet1!C25,"")</f>
+        <f>IF('list-pre-google-forms'!G25=1,'list-pre-google-forms'!C25,"")</f>
         <v>Peter.Comeau@dfo-mpo.gc.ca</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" t="str">
-        <f>IF(Sheet1!E26=1,Sheet1!C26,"")</f>
+        <f>IF('list-pre-google-forms'!E26=1,'list-pre-google-forms'!C26,"")</f>
         <v>Nell.denHeyer@dfo-mpo.gc.ca</v>
       </c>
       <c r="B20" t="str">
-        <f>IF(Sheet1!G26=1,Sheet1!C26,"")</f>
+        <f>IF('list-pre-google-forms'!G26=1,'list-pre-google-forms'!C26,"")</f>
         <v>Nell.denHeyer@dfo-mpo.gc.ca</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" t="str">
-        <f>IF(Sheet1!E27=1,Sheet1!C27,"")</f>
+        <f>IF('list-pre-google-forms'!E27=1,'list-pre-google-forms'!C27,"")</f>
         <v>Quinn.McCurdy@dfo-mpo.gc.ca</v>
       </c>
       <c r="B21" t="str">
-        <f>IF(Sheet1!G27=1,Sheet1!C27,"")</f>
+        <f>IF('list-pre-google-forms'!G27=1,'list-pre-google-forms'!C27,"")</f>
         <v>Quinn.McCurdy@dfo-mpo.gc.ca</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" t="str">
-        <f>IF(Sheet1!E28=1,Sheet1!C28,"")</f>
+        <f>IF('list-pre-google-forms'!E28=1,'list-pre-google-forms'!C28,"")</f>
         <v>Dheeraj.Busawon@dfo-mpo.gc.ca</v>
       </c>
       <c r="B22" t="str">
-        <f>IF(Sheet1!G28=1,Sheet1!C28,"")</f>
+        <f>IF('list-pre-google-forms'!G28=1,'list-pre-google-forms'!C28,"")</f>
         <v/>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" t="str">
-        <f>IF(Sheet1!E29=1,Sheet1!C29,"")</f>
+        <f>IF('list-pre-google-forms'!E29=1,'list-pre-google-forms'!C29,"")</f>
         <v>George.Nau@dfo-mpo.gc.ca</v>
       </c>
       <c r="B23" t="str">
-        <f>IF(Sheet1!G29=1,Sheet1!C29,"")</f>
+        <f>IF('list-pre-google-forms'!G29=1,'list-pre-google-forms'!C29,"")</f>
         <v>George.Nau@dfo-mpo.gc.ca</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" t="str">
-        <f>IF(Sheet1!E30=1,Sheet1!C30,"")</f>
+        <f>IF('list-pre-google-forms'!E30=1,'list-pre-google-forms'!C30,"")</f>
         <v>Mark.Billard@dfo-mpo.gc.ca</v>
       </c>
       <c r="B24" t="str">
-        <f>IF(Sheet1!G30=1,Sheet1!C30,"")</f>
+        <f>IF('list-pre-google-forms'!G30=1,'list-pre-google-forms'!C30,"")</f>
         <v>Mark.Billard@dfo-mpo.gc.ca</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" t="str">
-        <f>IF(Sheet1!E31=1,Sheet1!C31,"")</f>
+        <f>IF('list-pre-google-forms'!E31=1,'list-pre-google-forms'!C31,"")</f>
         <v>lynn.collier@dfo-mpo.gc.ca</v>
       </c>
       <c r="B25" t="str">
-        <f>IF(Sheet1!G31=1,Sheet1!C31,"")</f>
+        <f>IF('list-pre-google-forms'!G31=1,'list-pre-google-forms'!C31,"")</f>
         <v>lynn.collier@dfo-mpo.gc.ca</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" t="str">
-        <f>IF(Sheet1!E32=1,Sheet1!C32,"")</f>
+        <f>IF('list-pre-google-forms'!E32=1,'list-pre-google-forms'!C32,"")</f>
         <v>Kelly.Kraska@dfo-mpo.gc.ca</v>
       </c>
       <c r="B26" t="str">
-        <f>IF(Sheet1!G32=1,Sheet1!C32,"")</f>
+        <f>IF('list-pre-google-forms'!G32=1,'list-pre-google-forms'!C32,"")</f>
         <v/>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" t="str">
-        <f>IF(Sheet1!E33=1,Sheet1!C33,"")</f>
+        <f>IF('list-pre-google-forms'!E33=1,'list-pre-google-forms'!C33,"")</f>
         <v>Tania.Davignon-Burton@dfo-mpo.gc.ca</v>
       </c>
       <c r="B27" t="str">
-        <f>IF(Sheet1!G33=1,Sheet1!C33,"")</f>
+        <f>IF('list-pre-google-forms'!G33=1,'list-pre-google-forms'!C33,"")</f>
         <v>Tania.Davignon-Burton@dfo-mpo.gc.ca</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" t="str">
-        <f>IF(Sheet1!E34=1,Sheet1!C34,"")</f>
+        <f>IF('list-pre-google-forms'!E34=1,'list-pre-google-forms'!C34,"")</f>
         <v>Gregory.Puncher@dfo-mpo.gc.ca</v>
       </c>
       <c r="B28" t="str">
-        <f>IF(Sheet1!G34=1,Sheet1!C34,"")</f>
+        <f>IF('list-pre-google-forms'!G34=1,'list-pre-google-forms'!C34,"")</f>
         <v/>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" t="str">
-        <f>IF(Sheet1!E35=1,Sheet1!C35,"")</f>
+        <f>IF('list-pre-google-forms'!E35=1,'list-pre-google-forms'!C35,"")</f>
         <v>Catriona.Regnier-McKellar@dfo-mpo.gc.ca</v>
       </c>
       <c r="B29" t="str">
-        <f>IF(Sheet1!G35=1,Sheet1!C35,"")</f>
+        <f>IF('list-pre-google-forms'!G35=1,'list-pre-google-forms'!C35,"")</f>
         <v/>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30" t="str">
-        <f>IF(Sheet1!E36=1,Sheet1!C36,"")</f>
+        <f>IF('list-pre-google-forms'!E36=1,'list-pre-google-forms'!C36,"")</f>
         <v/>
       </c>
       <c r="B30" t="str">
-        <f>IF(Sheet1!G36=1,Sheet1!C36,"")</f>
+        <f>IF('list-pre-google-forms'!G36=1,'list-pre-google-forms'!C36,"")</f>
         <v/>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31" t="str">
-        <f>IF(Sheet1!E37=1,Sheet1!C37,"")</f>
+        <f>IF('list-pre-google-forms'!E37=1,'list-pre-google-forms'!C37,"")</f>
         <v/>
       </c>
       <c r="B31" t="str">
-        <f>IF(Sheet1!G37=1,Sheet1!C37,"")</f>
+        <f>IF('list-pre-google-forms'!G37=1,'list-pre-google-forms'!C37,"")</f>
         <v/>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32" t="str">
-        <f>IF(Sheet1!E38=1,Sheet1!C38,"")</f>
+        <f>IF('list-pre-google-forms'!E38=1,'list-pre-google-forms'!C38,"")</f>
         <v>Kim.Emond@dfo-mpo.gc.ca</v>
       </c>
       <c r="B32" t="str">
-        <f>IF(Sheet1!G38=1,Sheet1!C38,"")</f>
+        <f>IF('list-pre-google-forms'!G38=1,'list-pre-google-forms'!C38,"")</f>
         <v>Kim.Emond@dfo-mpo.gc.ca</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33" t="str">
-        <f>IF(Sheet1!E39=1,Sheet1!C39,"")</f>
+        <f>IF('list-pre-google-forms'!E39=1,'list-pre-google-forms'!C39,"")</f>
         <v>Nicolas.LeCorre@dfo-mpo.gc.ca</v>
       </c>
       <c r="B33" t="str">
-        <f>IF(Sheet1!G39=1,Sheet1!C39,"")</f>
+        <f>IF('list-pre-google-forms'!G39=1,'list-pre-google-forms'!C39,"")</f>
         <v>Nicolas.LeCorre@dfo-mpo.gc.ca</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34" t="str">
-        <f>IF(Sheet1!E40=1,Sheet1!C40,"")</f>
+        <f>IF('list-pre-google-forms'!E40=1,'list-pre-google-forms'!C40,"")</f>
         <v>andrew.smith4@dfo-mpo.gc.ca</v>
       </c>
       <c r="B34" t="str">
-        <f>IF(Sheet1!G40=1,Sheet1!C40,"")</f>
+        <f>IF('list-pre-google-forms'!G40=1,'list-pre-google-forms'!C40,"")</f>
         <v>andrew.smith4@dfo-mpo.gc.ca</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35" t="str">
-        <f>IF(Sheet1!E41=1,Sheet1!C41,"")</f>
+        <f>IF('list-pre-google-forms'!E41=1,'list-pre-google-forms'!C41,"")</f>
         <v>Renald.Belley@dfo-mpo.gc.ca</v>
       </c>
       <c r="B35" t="str">
-        <f>IF(Sheet1!G41=1,Sheet1!C41,"")</f>
+        <f>IF('list-pre-google-forms'!G41=1,'list-pre-google-forms'!C41,"")</f>
         <v>Renald.Belley@dfo-mpo.gc.ca</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A36" t="str">
-        <f>IF(Sheet1!E42=1,Sheet1!C42,"")</f>
+        <f>IF('list-pre-google-forms'!E42=1,'list-pre-google-forms'!C42,"")</f>
         <v>Mathieu.Desgagnes@dfo-mpo.gc.ca</v>
       </c>
       <c r="B36" t="str">
-        <f>IF(Sheet1!G42=1,Sheet1!C42,"")</f>
+        <f>IF('list-pre-google-forms'!G42=1,'list-pre-google-forms'!C42,"")</f>
         <v>Mathieu.Desgagnes@dfo-mpo.gc.ca</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A37" t="str">
-        <f>IF(Sheet1!E43=1,Sheet1!C43,"")</f>
+        <f>IF('list-pre-google-forms'!E43=1,'list-pre-google-forms'!C43,"")</f>
         <v>helene.dionne@dfo-mpo.gc.ca</v>
       </c>
       <c r="B37" t="str">
-        <f>IF(Sheet1!G43=1,Sheet1!C43,"")</f>
+        <f>IF('list-pre-google-forms'!G43=1,'list-pre-google-forms'!C43,"")</f>
         <v>helene.dionne@dfo-mpo.gc.ca</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A38" t="str">
-        <f>IF(Sheet1!E44=1,Sheet1!C44,"")</f>
+        <f>IF('list-pre-google-forms'!E44=1,'list-pre-google-forms'!C44,"")</f>
         <v/>
       </c>
       <c r="B38" t="str">
-        <f>IF(Sheet1!G44=1,Sheet1!C44,"")</f>
+        <f>IF('list-pre-google-forms'!G44=1,'list-pre-google-forms'!C44,"")</f>
         <v/>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A39" t="str">
-        <f>IF(Sheet1!E45=1,Sheet1!C45,"")</f>
+        <f>IF('list-pre-google-forms'!E45=1,'list-pre-google-forms'!C45,"")</f>
         <v/>
       </c>
       <c r="B39" t="str">
-        <f>IF(Sheet1!G45=1,Sheet1!C45,"")</f>
+        <f>IF('list-pre-google-forms'!G45=1,'list-pre-google-forms'!C45,"")</f>
         <v/>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A40" t="str">
-        <f>IF(Sheet1!E46=1,Sheet1!C46,"")</f>
+        <f>IF('list-pre-google-forms'!E46=1,'list-pre-google-forms'!C46,"")</f>
         <v>Laura.Alsip@dfo-mpo.gc.ca</v>
       </c>
       <c r="B40" t="str">
-        <f>IF(Sheet1!G46=1,Sheet1!C46,"")</f>
+        <f>IF('list-pre-google-forms'!G46=1,'list-pre-google-forms'!C46,"")</f>
         <v>Laura.Alsip@dfo-mpo.gc.ca</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A41" t="str">
-        <f>IF(Sheet1!E47=1,Sheet1!C47,"")</f>
+        <f>IF('list-pre-google-forms'!E47=1,'list-pre-google-forms'!C47,"")</f>
         <v>Wojciech.Walkusz@dfo-mpo.gc.ca</v>
       </c>
       <c r="B41" t="str">
-        <f>IF(Sheet1!G47=1,Sheet1!C47,"")</f>
+        <f>IF('list-pre-google-forms'!G47=1,'list-pre-google-forms'!C47,"")</f>
         <v/>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A42" t="str">
-        <f>IF(Sheet1!E48=1,Sheet1!C48,"")</f>
+        <f>IF('list-pre-google-forms'!E48=1,'list-pre-google-forms'!C48,"")</f>
         <v>Lauren.Wiens@dfo-mpo.gc.ca</v>
       </c>
       <c r="B42" t="str">
-        <f>IF(Sheet1!G48=1,Sheet1!C48,"")</f>
+        <f>IF('list-pre-google-forms'!G48=1,'list-pre-google-forms'!C48,"")</f>
         <v>Lauren.Wiens@dfo-mpo.gc.ca</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A43" t="str">
-        <f>IF(Sheet1!E49=1,Sheet1!C49,"")</f>
+        <f>IF('list-pre-google-forms'!E49=1,'list-pre-google-forms'!C49,"")</f>
         <v/>
       </c>
       <c r="B43" t="str">
-        <f>IF(Sheet1!G49=1,Sheet1!C49,"")</f>
+        <f>IF('list-pre-google-forms'!G49=1,'list-pre-google-forms'!C49,"")</f>
         <v/>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A44" t="str">
-        <f>IF(Sheet1!E50=1,Sheet1!C50,"")</f>
+        <f>IF('list-pre-google-forms'!E50=1,'list-pre-google-forms'!C50,"")</f>
         <v/>
       </c>
       <c r="B44" t="str">
-        <f>IF(Sheet1!G50=1,Sheet1!C50,"")</f>
+        <f>IF('list-pre-google-forms'!G50=1,'list-pre-google-forms'!C50,"")</f>
         <v/>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A45" t="str">
-        <f>IF(Sheet1!E51=1,Sheet1!C51,"")</f>
+        <f>IF('list-pre-google-forms'!E51=1,'list-pre-google-forms'!C51,"")</f>
         <v>Tracey.Loewen@dfo-mpo.gc.ca</v>
       </c>
       <c r="B45" t="str">
-        <f>IF(Sheet1!G51=1,Sheet1!C51,"")</f>
+        <f>IF('list-pre-google-forms'!G51=1,'list-pre-google-forms'!C51,"")</f>
         <v>Tracey.Loewen@dfo-mpo.gc.ca</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A46" t="str">
-        <f>IF(Sheet1!E52=1,Sheet1!C52,"")</f>
+        <f>IF('list-pre-google-forms'!E52=1,'list-pre-google-forms'!C52,"")</f>
         <v>Brendan.Malley@dfo-mpo.gc.ca</v>
       </c>
       <c r="B46" t="str">
-        <f>IF(Sheet1!G52=1,Sheet1!C52,"")</f>
+        <f>IF('list-pre-google-forms'!G52=1,'list-pre-google-forms'!C52,"")</f>
         <v/>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A47" t="str">
-        <f>IF(Sheet1!E53=1,Sheet1!C53,"")</f>
+        <f>IF('list-pre-google-forms'!E53=1,'list-pre-google-forms'!C53,"")</f>
         <v/>
       </c>
       <c r="B47" t="str">
-        <f>IF(Sheet1!G53=1,Sheet1!C53,"")</f>
+        <f>IF('list-pre-google-forms'!G53=1,'list-pre-google-forms'!C53,"")</f>
         <v/>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A48" t="str">
-        <f>IF(Sheet1!E54=1,Sheet1!C54,"")</f>
+        <f>IF('list-pre-google-forms'!E54=1,'list-pre-google-forms'!C54,"")</f>
         <v/>
       </c>
       <c r="B48" t="str">
-        <f>IF(Sheet1!G54=1,Sheet1!C54,"")</f>
+        <f>IF('list-pre-google-forms'!G54=1,'list-pre-google-forms'!C54,"")</f>
         <v/>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A49" t="str">
-        <f>IF(Sheet1!E55=1,Sheet1!C55,"")</f>
+        <f>IF('list-pre-google-forms'!E55=1,'list-pre-google-forms'!C55,"")</f>
         <v>Sarah.Hawkshaw@dfo-mpo.gc.ca</v>
       </c>
       <c r="B49" t="str">
-        <f>IF(Sheet1!G55=1,Sheet1!C55,"")</f>
+        <f>IF('list-pre-google-forms'!G55=1,'list-pre-google-forms'!C55,"")</f>
         <v>Sarah.Hawkshaw@dfo-mpo.gc.ca</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A50" t="str">
-        <f>IF(Sheet1!E56=1,Sheet1!C56,"")</f>
+        <f>IF('list-pre-google-forms'!E56=1,'list-pre-google-forms'!C56,"")</f>
         <v>Madeline.Lavery@dfo-mpo.gc.ca</v>
       </c>
       <c r="B50" t="str">
-        <f>IF(Sheet1!G56=1,Sheet1!C56,"")</f>
+        <f>IF('list-pre-google-forms'!G56=1,'list-pre-google-forms'!C56,"")</f>
         <v>Madeline.Lavery@dfo-mpo.gc.ca</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A51" t="str">
-        <f>IF(Sheet1!E57=1,Sheet1!C57,"")</f>
+        <f>IF('list-pre-google-forms'!E57=1,'list-pre-google-forms'!C57,"")</f>
         <v>Emily.Yungwirth@dfo-mpo.gc.ca</v>
       </c>
       <c r="B51" t="str">
-        <f>IF(Sheet1!G57=1,Sheet1!C57,"")</f>
+        <f>IF('list-pre-google-forms'!G57=1,'list-pre-google-forms'!C57,"")</f>
         <v>Emily.Yungwirth@dfo-mpo.gc.ca</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A52" t="str">
-        <f>IF(Sheet1!E58=1,Sheet1!C58,"")</f>
+        <f>IF('list-pre-google-forms'!E58=1,'list-pre-google-forms'!C58,"")</f>
         <v>dana.haggarty@dfo-mpo.gc.ca</v>
       </c>
       <c r="B52" t="str">
-        <f>IF(Sheet1!G58=1,Sheet1!C58,"")</f>
+        <f>IF('list-pre-google-forms'!G58=1,'list-pre-google-forms'!C58,"")</f>
         <v>dana.haggarty@dfo-mpo.gc.ca</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A53" t="str">
-        <f>IF(Sheet1!E59=1,Sheet1!C59,"")</f>
+        <f>IF('list-pre-google-forms'!E59=1,'list-pre-google-forms'!C59,"")</f>
         <v>Kendra.Holt@dfo-mpo.gc.ca</v>
       </c>
       <c r="B53" t="str">
-        <f>IF(Sheet1!G59=1,Sheet1!C59,"")</f>
+        <f>IF('list-pre-google-forms'!G59=1,'list-pre-google-forms'!C59,"")</f>
         <v>Kendra.Holt@dfo-mpo.gc.ca</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A54" t="str">
-        <f>IF(Sheet1!E60=1,Sheet1!C60,"")</f>
+        <f>IF('list-pre-google-forms'!E60=1,'list-pre-google-forms'!C60,"")</f>
         <v>Matthew.Siegle@dfo-mpo.gc.ca</v>
       </c>
       <c r="B54" t="str">
-        <f>IF(Sheet1!G60=1,Sheet1!C60,"")</f>
+        <f>IF('list-pre-google-forms'!G60=1,'list-pre-google-forms'!C60,"")</f>
         <v/>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A55" t="str">
-        <f>IF(Sheet1!E61=1,Sheet1!C61,"")</f>
+        <f>IF('list-pre-google-forms'!E61=1,'list-pre-google-forms'!C61,"")</f>
         <v>Mackenzie.Mazur@dfo-mpo.gc.ca</v>
       </c>
       <c r="B55" t="str">
-        <f>IF(Sheet1!G61=1,Sheet1!C61,"")</f>
+        <f>IF('list-pre-google-forms'!G61=1,'list-pre-google-forms'!C61,"")</f>
         <v/>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A56" t="str">
-        <f>IF(Sheet1!E62=1,Sheet1!C62,"")</f>
+        <f>IF('list-pre-google-forms'!E62=1,'list-pre-google-forms'!C62,"")</f>
         <v>Karalea.Cantera@dfo-mpo.gc.ca</v>
       </c>
       <c r="B56" t="str">
-        <f>IF(Sheet1!G62=1,Sheet1!C62,"")</f>
+        <f>IF('list-pre-google-forms'!G62=1,'list-pre-google-forms'!C62,"")</f>
         <v/>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A57" t="str">
-        <f>IF(Sheet1!E63=1,Sheet1!C63,"")</f>
+        <f>IF('list-pre-google-forms'!E63=1,'list-pre-google-forms'!C63,"")</f>
         <v>Kiana.Matwichuk@dfo-mpo.gc.ca</v>
       </c>
       <c r="B57" t="str">
-        <f>IF(Sheet1!G63=1,Sheet1!C63,"")</f>
+        <f>IF('list-pre-google-forms'!G63=1,'list-pre-google-forms'!C63,"")</f>
         <v/>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A58" t="str">
-        <f>IF(Sheet1!E64=1,Sheet1!C64,"")</f>
+        <f>IF('list-pre-google-forms'!E64=1,'list-pre-google-forms'!C64,"")</f>
         <v>Erin.Herder@dfo-mpo.gc.ca</v>
       </c>
       <c r="B58" t="str">
-        <f>IF(Sheet1!G64=1,Sheet1!C64,"")</f>
+        <f>IF('list-pre-google-forms'!G64=1,'list-pre-google-forms'!C64,"")</f>
         <v>Erin.Herder@dfo-mpo.gc.ca</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A59" t="str">
-        <f>IF(Sheet1!E65=1,Sheet1!C65,"")</f>
+        <f>IF('list-pre-google-forms'!E65=1,'list-pre-google-forms'!C65,"")</f>
         <v>Robyn.Forrest@dfo-mpo.gc.ca</v>
       </c>
       <c r="B59" t="str">
-        <f>IF(Sheet1!G65=1,Sheet1!C65,"")</f>
+        <f>IF('list-pre-google-forms'!G65=1,'list-pre-google-forms'!C65,"")</f>
         <v>Robyn.Forrest@dfo-mpo.gc.ca</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A60" t="str">
-        <f>IF(Sheet1!E66=1,Sheet1!C66,"")</f>
+        <f>IF('list-pre-google-forms'!E66=1,'list-pre-google-forms'!C66,"")</f>
         <v>yeongha.jung@dfo-mpo.gc.ca</v>
       </c>
       <c r="B60" t="str">
-        <f>IF(Sheet1!G66=1,Sheet1!C66,"")</f>
+        <f>IF('list-pre-google-forms'!G66=1,'list-pre-google-forms'!C66,"")</f>
         <v>yeongha.jung@dfo-mpo.gc.ca</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A61" t="str">
-        <f>IF(Sheet1!E67=1,Sheet1!C67,"")</f>
+        <f>IF('list-pre-google-forms'!E67=1,'list-pre-google-forms'!C67,"")</f>
         <v>barbara.campbell@dfo-mpo.gc.ca</v>
       </c>
       <c r="B61" t="str">
-        <f>IF(Sheet1!G67=1,Sheet1!C67,"")</f>
+        <f>IF('list-pre-google-forms'!G67=1,'list-pre-google-forms'!C67,"")</f>
         <v>barbara.campbell@dfo-mpo.gc.ca</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A62" t="str">
-        <f>IF(Sheet1!E68=1,Sheet1!C68,"")</f>
+        <f>IF('list-pre-google-forms'!E68=1,'list-pre-google-forms'!C68,"")</f>
         <v>stephen.wischniowski@dfo-mpo.gc.ca</v>
       </c>
       <c r="B62" t="str">
-        <f>IF(Sheet1!G68=1,Sheet1!C68,"")</f>
+        <f>IF('list-pre-google-forms'!G68=1,'list-pre-google-forms'!C68,"")</f>
         <v/>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A63" t="str">
-        <f>IF(Sheet1!E69=1,Sheet1!C69,"")</f>
+        <f>IF('list-pre-google-forms'!E69=1,'list-pre-google-forms'!C69,"")</f>
         <v/>
       </c>
       <c r="B63" t="str">
-        <f>IF(Sheet1!G69=1,Sheet1!C69,"")</f>
+        <f>IF('list-pre-google-forms'!G69=1,'list-pre-google-forms'!C69,"")</f>
         <v/>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A64" t="str">
-        <f>IF(Sheet1!E70=1,Sheet1!C70,"")</f>
+        <f>IF('list-pre-google-forms'!E70=1,'list-pre-google-forms'!C70,"")</f>
         <v/>
       </c>
       <c r="B64" t="str">
-        <f>IF(Sheet1!G70=1,Sheet1!C70,"")</f>
+        <f>IF('list-pre-google-forms'!G70=1,'list-pre-google-forms'!C70,"")</f>
         <v/>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A65" t="str">
-        <f>IF(Sheet1!E71=1,Sheet1!C71,"")</f>
+        <f>IF('list-pre-google-forms'!E71=1,'list-pre-google-forms'!C71,"")</f>
         <v>Gillian.Forbes@dfo-mpo.gc.ca</v>
       </c>
       <c r="B65" t="str">
-        <f>IF(Sheet1!G71=1,Sheet1!C71,"")</f>
+        <f>IF('list-pre-google-forms'!G71=1,'list-pre-google-forms'!C71,"")</f>
         <v/>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A66" t="str">
-        <f>IF(Sheet1!E72=1,Sheet1!C72,"")</f>
+        <f>IF('list-pre-google-forms'!E72=1,'list-pre-google-forms'!C72,"")</f>
         <v>Divya.Varkey@dfo-mpo.gc.ca</v>
       </c>
       <c r="B66" t="str">
-        <f>IF(Sheet1!G72=1,Sheet1!C72,"")</f>
+        <f>IF('list-pre-google-forms'!G72=1,'list-pre-google-forms'!C72,"")</f>
         <v/>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A67" t="str">
-        <f>IF(Sheet1!E73=1,Sheet1!C73,"")</f>
+        <f>IF('list-pre-google-forms'!E73=1,'list-pre-google-forms'!C73,"")</f>
         <v>Aaron.Adamack@dfo-mpo.gc.ca</v>
       </c>
       <c r="B67" t="str">
-        <f>IF(Sheet1!G73=1,Sheet1!C73,"")</f>
+        <f>IF('list-pre-google-forms'!G73=1,'list-pre-google-forms'!C73,"")</f>
         <v>Aaron.Adamack@dfo-mpo.gc.ca</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A68" t="str">
-        <f>IF(Sheet1!E74=1,Sheet1!C74,"")</f>
+        <f>IF('list-pre-google-forms'!E74=1,'list-pre-google-forms'!C74,"")</f>
         <v>Meredith.Schofield@dfo-mpo.gc.ca</v>
       </c>
       <c r="B68" t="str">
-        <f>IF(Sheet1!G74=1,Sheet1!C74,"")</f>
+        <f>IF('list-pre-google-forms'!G74=1,'list-pre-google-forms'!C74,"")</f>
         <v>Meredith.Schofield@dfo-mpo.gc.ca</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A69" t="str">
-        <f>IF(Sheet1!E75=1,Sheet1!C75,"")</f>
+        <f>IF('list-pre-google-forms'!E75=1,'list-pre-google-forms'!C75,"")</f>
         <v>Andrea.Perreault@dfo-mpo.gc.ca</v>
       </c>
       <c r="B69" t="str">
-        <f>IF(Sheet1!G75=1,Sheet1!C75,"")</f>
+        <f>IF('list-pre-google-forms'!G75=1,'list-pre-google-forms'!C75,"")</f>
         <v>Andrea.Perreault@dfo-mpo.gc.ca</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A70" t="str">
-        <f>IF(Sheet1!E76=1,Sheet1!C76,"")</f>
+        <f>IF('list-pre-google-forms'!E76=1,'list-pre-google-forms'!C76,"")</f>
         <v>Laura.Wheeland@dfo-mpo.gc.ca</v>
       </c>
       <c r="B70" t="str">
-        <f>IF(Sheet1!G76=1,Sheet1!C76,"")</f>
+        <f>IF('list-pre-google-forms'!G76=1,'list-pre-google-forms'!C76,"")</f>
         <v>Laura.Wheeland@dfo-mpo.gc.ca</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A71" t="str">
-        <f>IF(Sheet1!E77=1,Sheet1!C77,"")</f>
+        <f>IF('list-pre-google-forms'!E77=1,'list-pre-google-forms'!C77,"")</f>
         <v/>
       </c>
       <c r="B71" t="str">
-        <f>IF(Sheet1!G77=1,Sheet1!C77,"")</f>
+        <f>IF('list-pre-google-forms'!G77=1,'list-pre-google-forms'!C77,"")</f>
         <v/>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A72" t="str">
-        <f>IF(Sheet1!E78=1,Sheet1!C78,"")</f>
+        <f>IF('list-pre-google-forms'!E78=1,'list-pre-google-forms'!C78,"")</f>
         <v/>
       </c>
       <c r="B72" t="str">
-        <f>IF(Sheet1!G78=1,Sheet1!C78,"")</f>
+        <f>IF('list-pre-google-forms'!G78=1,'list-pre-google-forms'!C78,"")</f>
         <v/>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A73" t="str">
-        <f>IF(Sheet1!E79=1,Sheet1!C79,"")</f>
+        <f>IF('list-pre-google-forms'!E79=1,'list-pre-google-forms'!C79,"")</f>
         <v/>
       </c>
       <c r="B73" t="str">
-        <f>IF(Sheet1!G79=1,Sheet1!C79,"")</f>
+        <f>IF('list-pre-google-forms'!G79=1,'list-pre-google-forms'!C79,"")</f>
         <v/>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A74" t="str">
-        <f>IF(Sheet1!E80=1,Sheet1!C80,"")</f>
+        <f>IF('list-pre-google-forms'!E80=1,'list-pre-google-forms'!C80,"")</f>
         <v/>
       </c>
       <c r="B74" t="str">
-        <f>IF(Sheet1!G80=1,Sheet1!C80,"")</f>
+        <f>IF('list-pre-google-forms'!G80=1,'list-pre-google-forms'!C80,"")</f>
         <v/>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A75" t="str">
-        <f>IF(Sheet1!E81=1,Sheet1!C81,"")</f>
+        <f>IF('list-pre-google-forms'!E81=1,'list-pre-google-forms'!C81,"")</f>
         <v/>
       </c>
       <c r="B75" t="str">
-        <f>IF(Sheet1!G81=1,Sheet1!C81,"")</f>
+        <f>IF('list-pre-google-forms'!G81=1,'list-pre-google-forms'!C81,"")</f>
         <v/>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A76" t="str">
-        <f>IF(Sheet1!E82=1,Sheet1!C82,"")</f>
+        <f>IF('list-pre-google-forms'!E82=1,'list-pre-google-forms'!C82,"")</f>
         <v/>
       </c>
       <c r="B76" t="str">
-        <f>IF(Sheet1!G82=1,Sheet1!C82,"")</f>
+        <f>IF('list-pre-google-forms'!G82=1,'list-pre-google-forms'!C82,"")</f>
         <v/>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A77" t="str">
-        <f>IF(Sheet1!E83=1,Sheet1!C83,"")</f>
+        <f>IF('list-pre-google-forms'!E83=1,'list-pre-google-forms'!C83,"")</f>
         <v/>
       </c>
       <c r="B77" t="str">
-        <f>IF(Sheet1!G83=1,Sheet1!C83,"")</f>
+        <f>IF('list-pre-google-forms'!G83=1,'list-pre-google-forms'!C83,"")</f>
         <v/>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B78" t="str">
-        <f>IF(Sheet1!G88=1,Sheet1!C88,"")</f>
-        <v/>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7648514F-C50B-429E-8CE0-7F6A61E6FA38}">
-  <dimension ref="B3:G51"/>
-  <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="A40" sqref="A40"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="4" max="4" width="22.26953125" customWidth="1"/>
-    <col min="6" max="6" width="29.81640625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="C3" t="s">
-        <v>167</v>
-      </c>
-      <c r="D3" t="s">
-        <v>168</v>
-      </c>
-      <c r="E3" t="s">
-        <v>169</v>
-      </c>
-      <c r="G3" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B5" t="s">
-        <v>149</v>
-      </c>
-      <c r="C5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="F5" s="2"/>
-      <c r="G5" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B6" t="s">
-        <v>149</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="F6" s="2"/>
-      <c r="G6" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B7" t="s">
-        <v>149</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="F7" s="2"/>
-      <c r="G7" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B8" t="s">
-        <v>149</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="F8" s="2"/>
-      <c r="G8" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="2"/>
-    </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="D10" s="1"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-    </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="D11" s="1"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-    </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B12" t="s">
-        <v>149</v>
-      </c>
-      <c r="C12" t="s">
-        <v>16</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="G12" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B13" t="s">
-        <v>149</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="G13" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B14" t="s">
-        <v>149</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="E14" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="G14" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B15" t="s">
-        <v>149</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="G15" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B16" t="s">
-        <v>148</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="E16" s="6" t="s">
-        <v>147</v>
-      </c>
-      <c r="G16" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B17" t="s">
-        <v>149</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="G17" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B18" t="s">
-        <v>149</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="G18" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B19" t="s">
-        <v>149</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="G19" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="D21" s="1"/>
-      <c r="E21" s="2"/>
-    </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="D22" s="1"/>
-      <c r="E22" s="2"/>
-    </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="D23" s="1"/>
-      <c r="E23" s="2"/>
-    </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="D24" s="1"/>
-      <c r="E24" s="6"/>
-    </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B25" t="s">
-        <v>149</v>
-      </c>
-      <c r="C25" t="s">
-        <v>6</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G25" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B26" t="s">
-        <v>149</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="E26" s="8" t="s">
-        <v>132</v>
-      </c>
-      <c r="G26" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B27" t="s">
-        <v>149</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="G27" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="28" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B28" t="s">
-        <v>149</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E28" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="G28" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="29" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B29" t="s">
-        <v>149</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="G29" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="30" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B30" t="s">
-        <v>149</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="E30" s="8" t="s">
-        <v>131</v>
-      </c>
-      <c r="G30" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="31" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B31" t="s">
-        <v>149</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="E31" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="G31" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="32" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="D32" s="1"/>
-      <c r="E32" s="8"/>
-    </row>
-    <row r="34" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B34" t="s">
-        <v>149</v>
-      </c>
-      <c r="C34" t="s">
-        <v>8</v>
-      </c>
-      <c r="D34" t="s">
-        <v>144</v>
-      </c>
-      <c r="E34" t="s">
-        <v>145</v>
-      </c>
-      <c r="G34" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="35" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B35" t="s">
-        <v>149</v>
-      </c>
-      <c r="D35" t="s">
-        <v>152</v>
-      </c>
-      <c r="E35" t="s">
-        <v>151</v>
-      </c>
-      <c r="G35" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="36" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B36" t="s">
-        <v>149</v>
-      </c>
-      <c r="D36" t="s">
-        <v>154</v>
-      </c>
-      <c r="E36" t="s">
-        <v>153</v>
-      </c>
-      <c r="G36" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="37" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B37" t="s">
-        <v>149</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="E37" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="G37" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="38" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B38" t="s">
-        <v>149</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="E38" s="8" t="s">
-        <v>137</v>
-      </c>
-      <c r="G38" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="39" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B39" t="s">
-        <v>149</v>
-      </c>
-      <c r="D39" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="E39" t="s">
-        <v>170</v>
-      </c>
-      <c r="G39" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="41" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B41" t="s">
-        <v>149</v>
-      </c>
-      <c r="C41" t="s">
-        <v>7</v>
-      </c>
-      <c r="D41" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="E41" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="G41" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="42" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B42" t="s">
-        <v>149</v>
-      </c>
-      <c r="D42" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="E42" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="G42" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="43" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B43" t="s">
-        <v>149</v>
-      </c>
-      <c r="D43" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="E43" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="G43" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="44" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B44" t="s">
-        <v>149</v>
-      </c>
-      <c r="D44" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="E44" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="G44" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="45" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B45" t="s">
-        <v>149</v>
-      </c>
-      <c r="D45" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="E45" s="8" t="s">
-        <v>113</v>
-      </c>
-      <c r="G45" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="47" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B47" t="s">
-        <v>149</v>
-      </c>
-      <c r="C47" t="s">
-        <v>155</v>
-      </c>
-      <c r="D47" t="s">
-        <v>156</v>
-      </c>
-      <c r="E47" t="s">
-        <v>158</v>
-      </c>
-      <c r="G47" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="48" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B48" t="s">
-        <v>149</v>
-      </c>
-      <c r="D48" t="s">
-        <v>159</v>
-      </c>
-      <c r="E48" t="s">
-        <v>160</v>
-      </c>
-      <c r="G48" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="49" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B49" t="s">
-        <v>148</v>
-      </c>
-      <c r="D49" t="s">
-        <v>163</v>
-      </c>
-      <c r="E49" t="s">
-        <v>164</v>
-      </c>
-      <c r="G49" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="50" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B50" t="s">
-        <v>149</v>
-      </c>
-      <c r="D50" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E50" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G50" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="51" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B51" t="s">
-        <v>149</v>
-      </c>
-      <c r="D51" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="E51" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="G51" t="s">
-        <v>140</v>
+        <f>IF('list-pre-google-forms'!G88=1,'list-pre-google-forms'!C88,"")</f>
+        <v/>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update README and add backbone main presentation
</commit_message>
<xml_diff>
--- a/planning/workshop-participants.xlsx
+++ b/planning/workshop-participants.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RicardD\Documents\GitHub\ageing-best-practices-2022\planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D00A274-D07B-45DD-A714-D1E088CA77BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{308D755D-7FDC-4C0C-8F16-23966F61A80F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="615" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="44880" yWindow="4965" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="outlook-responses" sheetId="3" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="437" uniqueCount="199">
   <si>
     <t>Name</t>
   </si>
@@ -470,9 +470,6 @@
     <t>Sutton, Jolene</t>
   </si>
   <si>
-    <t>Drover, Dwigth</t>
-  </si>
-  <si>
     <t>dwight.drover@dfo-mpo.gc.ca</t>
   </si>
   <si>
@@ -630,6 +627,12 @@
   </si>
   <si>
     <t>Total</t>
+  </si>
+  <si>
+    <t xml:space="preserve">McArthur, Judy </t>
+  </si>
+  <si>
+    <t>Judy.McArthur@dfo-mpo.gc.ca</t>
   </si>
 </sst>
 </file>
@@ -992,71 +995,73 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7648514F-C50B-429E-8CE0-7F6A61E6FA38}">
-  <dimension ref="A2:O66"/>
+  <dimension ref="A2:O67"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A39" sqref="A39"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="22.26953125" customWidth="1"/>
-    <col min="7" max="7" width="29.81640625" customWidth="1"/>
+    <col min="5" max="5" width="22.28515625" customWidth="1"/>
+    <col min="7" max="7" width="29.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="L2" s="1" t="s">
         <v>125</v>
       </c>
       <c r="M2">
-        <f>SUM(M6:M66)</f>
-        <v>56</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
+        <f>SUM(M6:M67)</f>
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D3" t="s">
+        <v>164</v>
+      </c>
+      <c r="E3" t="s">
         <v>165</v>
       </c>
-      <c r="E3" t="s">
-        <v>166</v>
-      </c>
       <c r="G3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="L3" t="s">
         <v>140</v>
       </c>
       <c r="M3">
-        <f>SUM(O6:O66)</f>
-        <v>35</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
+        <f>SUM(O6:O67)</f>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B4">
-        <f>B6+B18+B32+B42+B51+B58</f>
-        <v>56</v>
+        <f>B6+B18+B33+B43+B52+B59</f>
+        <v>57</v>
       </c>
       <c r="L4" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="M4">
-        <f>SUM(N6:N66)</f>
+        <f>SUM(N6:N67)</f>
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="N5" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="O5" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -1075,21 +1080,21 @@
         <v>122</v>
       </c>
       <c r="I6" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="M6">
         <v>1</v>
       </c>
       <c r="N6">
-        <f>IF(G6="In person",1,0)</f>
+        <f t="shared" ref="N6:N16" si="0">IF(G6="In person",1,0)</f>
         <v>1</v>
       </c>
       <c r="O6">
-        <f>IF(G6="Virtual",1,0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
+        <f t="shared" ref="O6:O16" si="1">IF(G6="Virtual",1,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D7" s="1" t="s">
         <v>43</v>
       </c>
@@ -1107,17 +1112,17 @@
         <v>1</v>
       </c>
       <c r="N7">
-        <f>IF(G7="In person",1,0)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="O7">
-        <f>IF(G7="Virtual",1,0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D8" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>31</v>
@@ -1127,21 +1132,21 @@
         <v>122</v>
       </c>
       <c r="I8" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="M8">
         <v>1</v>
       </c>
       <c r="N8">
-        <f>IF(G8="In person",1,0)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="O8">
-        <f>IF(G8="Virtual",1,0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D9" s="1" t="s">
         <v>29</v>
       </c>
@@ -1159,15 +1164,15 @@
         <v>1</v>
       </c>
       <c r="N9">
-        <f>IF(G9="In person",1,0)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="O9">
-        <f>IF(G9="Virtual",1,0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D10" s="1" t="s">
         <v>114</v>
       </c>
@@ -1185,69 +1190,69 @@
         <v>1</v>
       </c>
       <c r="N10">
-        <f>IF(G10="In person",1,0)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="O10">
-        <f>IF(G10="Virtual",1,0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D11" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="E11" s="8" t="s">
         <v>186</v>
-      </c>
-      <c r="E11" s="8" t="s">
-        <v>187</v>
       </c>
       <c r="F11" s="2"/>
       <c r="G11" t="s">
         <v>122</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="M11">
         <v>1</v>
       </c>
       <c r="N11">
-        <f>IF(G11="In person",1,0)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="O11">
-        <f>IF(G11="Virtual",1,0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D12" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="E12" s="8" t="s">
         <v>188</v>
-      </c>
-      <c r="E12" s="8" t="s">
-        <v>189</v>
       </c>
       <c r="F12" s="2"/>
       <c r="G12" t="s">
         <v>122</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="M12">
         <v>1</v>
       </c>
       <c r="N12">
-        <f>IF(G12="In person",1,0)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="O12">
-        <f>IF(G12="Virtual",1,0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D13" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E13" s="8" t="s">
         <v>117</v>
@@ -1257,23 +1262,23 @@
         <v>122</v>
       </c>
       <c r="I13" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="M13">
+        <v>1</v>
+      </c>
+      <c r="N13">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="O13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="D14" s="1" t="s">
         <v>190</v>
-      </c>
-      <c r="M13">
-        <v>1</v>
-      </c>
-      <c r="N13">
-        <f>IF(G13="In person",1,0)</f>
-        <v>1</v>
-      </c>
-      <c r="O13">
-        <f>IF(G13="Virtual",1,0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="D14" s="1" t="s">
-        <v>191</v>
       </c>
       <c r="E14" s="8" t="s">
         <v>11</v>
@@ -1283,21 +1288,21 @@
         <v>122</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="M14">
         <v>1</v>
       </c>
       <c r="N14">
-        <f>IF(G14="In person",1,0)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="O14">
-        <f>IF(G14="Virtual",1,0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.35">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D15" s="1" t="s">
         <v>141</v>
       </c>
@@ -1315,17 +1320,17 @@
         <v>1</v>
       </c>
       <c r="N15">
-        <f>IF(G15="In person",1,0)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="O15">
-        <f>IF(G15="Virtual",1,0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D16" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E16" s="8" t="s">
         <v>28</v>
@@ -1335,32 +1340,32 @@
         <v>122</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="M16">
         <v>1</v>
       </c>
       <c r="N16">
-        <f>IF(G16="In person",1,0)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="O16">
-        <f>IF(G16="Virtual",1,0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.35">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D17" s="1"/>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>16</v>
       </c>
       <c r="B18">
-        <f>SUM(M18:M30)</f>
-        <v>13</v>
+        <f>SUM(M18:M31)</f>
+        <v>14</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>84</v>
@@ -1378,7 +1383,7 @@
         <v>1</v>
       </c>
       <c r="N18">
-        <f>IF(G18="In person",1,0)</f>
+        <f t="shared" ref="N18:N31" si="2">IF(G18="In person",1,0)</f>
         <v>0</v>
       </c>
       <c r="O18">
@@ -1386,7 +1391,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D19" s="1" t="s">
         <v>85</v>
       </c>
@@ -1403,15 +1408,15 @@
         <v>1</v>
       </c>
       <c r="N19">
-        <f>IF(G19="In person",1,0)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="O19">
-        <f t="shared" ref="O19:O30" si="0">IF(G19="Virtual",1,0)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.35">
+        <f t="shared" ref="O19:O31" si="3">IF(G19="Virtual",1,0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D20" s="1" t="s">
         <v>78</v>
       </c>
@@ -1428,15 +1433,15 @@
         <v>1</v>
       </c>
       <c r="N20">
-        <f>IF(G20="In person",1,0)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="O20">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.35">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D21" s="1" t="s">
         <v>83</v>
       </c>
@@ -1453,40 +1458,40 @@
         <v>1</v>
       </c>
       <c r="N21">
-        <f>IF(G21="In person",1,0)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="O21">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.35">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D22" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="E22" s="6" t="s">
         <v>146</v>
-      </c>
-      <c r="E22" s="6" t="s">
-        <v>147</v>
       </c>
       <c r="G22" t="s">
         <v>140</v>
       </c>
       <c r="I22" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="M22">
         <v>1</v>
       </c>
       <c r="N22">
-        <f>IF(G22="In person",1,0)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="O22">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.35">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D23" s="1" t="s">
         <v>92</v>
       </c>
@@ -1503,15 +1508,15 @@
         <v>1</v>
       </c>
       <c r="N23">
-        <f>IF(G23="In person",1,0)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="O23">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.35">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D24" s="1" t="s">
         <v>80</v>
       </c>
@@ -1528,15 +1533,15 @@
         <v>1</v>
       </c>
       <c r="N24">
-        <f>IF(G24="In person",1,0)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="O24">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.35">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D25" s="1" t="s">
         <v>82</v>
       </c>
@@ -1553,15 +1558,15 @@
         <v>1</v>
       </c>
       <c r="N25">
-        <f>IF(G25="In person",1,0)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="O25">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.35">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D26" s="1" t="s">
         <v>96</v>
       </c>
@@ -1578,20 +1583,20 @@
         <v>1</v>
       </c>
       <c r="N26">
-        <f>IF(G26="In person",1,0)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="O26">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.35">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D27" s="1" t="s">
         <v>93</v>
       </c>
       <c r="E27" s="8" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="G27" t="s">
         <v>140</v>
@@ -1603,17 +1608,17 @@
         <v>1</v>
       </c>
       <c r="N27">
-        <f>IF(G27="In person",1,0)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="O27">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.35">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D28" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E28" s="8" t="s">
         <v>59</v>
@@ -1622,23 +1627,23 @@
         <v>140</v>
       </c>
       <c r="I28" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="M28">
+        <v>1</v>
+      </c>
+      <c r="N28">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O28">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="D29" s="1" t="s">
         <v>194</v>
-      </c>
-      <c r="M28">
-        <v>1</v>
-      </c>
-      <c r="N28">
-        <f>IF(G28="In person",1,0)</f>
-        <v>0</v>
-      </c>
-      <c r="O28">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="D29" s="1" t="s">
-        <v>195</v>
       </c>
       <c r="E29" s="8" t="s">
         <v>39</v>
@@ -1647,21 +1652,21 @@
         <v>140</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="M29">
         <v>1</v>
       </c>
       <c r="N29">
-        <f>IF(G29="In person",1,0)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="O29">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.35">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D30" s="1" t="s">
         <v>25</v>
       </c>
@@ -1678,840 +1683,868 @@
         <v>1</v>
       </c>
       <c r="N30">
-        <f>IF(G30="In person",1,0)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="O30">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="D31" s="1"/>
-      <c r="E31" s="6"/>
-    </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A32" t="s">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="D31" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="E31" s="8" t="s">
+        <v>198</v>
+      </c>
+      <c r="G31" t="s">
+        <v>140</v>
+      </c>
+      <c r="I31" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="M31">
+        <v>1</v>
+      </c>
+      <c r="N31">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O31">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="D32" s="1"/>
+      <c r="E32" s="6"/>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
         <v>6</v>
       </c>
-      <c r="B32">
-        <f>SUM(M32:M40)</f>
+      <c r="B33">
+        <f>SUM(M33:M41)</f>
         <v>9</v>
       </c>
-      <c r="D32" s="1" t="s">
+      <c r="D33" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="E32" s="1" t="s">
+      <c r="E33" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="G32" t="s">
-        <v>140</v>
-      </c>
-      <c r="I32" t="s">
-        <v>70</v>
-      </c>
-      <c r="M32">
-        <v>1</v>
-      </c>
-      <c r="N32">
-        <f>IF(G32="In person",1,0)</f>
-        <v>0</v>
-      </c>
-      <c r="O32">
-        <f t="shared" ref="O32:O40" si="1">IF(G32="Virtual",1,0)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="D33" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="E33" s="8" t="s">
-        <v>132</v>
       </c>
       <c r="G33" t="s">
         <v>140</v>
       </c>
       <c r="I33" t="s">
+        <v>70</v>
+      </c>
+      <c r="M33">
+        <v>1</v>
+      </c>
+      <c r="N33">
+        <f t="shared" ref="N33:N41" si="4">IF(G33="In person",1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="O33">
+        <f t="shared" ref="O33:O41" si="5">IF(G33="Virtual",1,0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="D34" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="M33">
-        <v>1</v>
-      </c>
-      <c r="N33">
-        <f>IF(G33="In person",1,0)</f>
-        <v>0</v>
-      </c>
-      <c r="O33">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="D34" s="1" t="s">
+      <c r="E34" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="G34" t="s">
+        <v>140</v>
+      </c>
+      <c r="I34" t="s">
+        <v>130</v>
+      </c>
+      <c r="M34">
+        <v>1</v>
+      </c>
+      <c r="N34">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="O34">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="D35" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="E34" s="1" t="s">
+      <c r="E35" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="G34" t="s">
+      <c r="G35" t="s">
         <v>122</v>
       </c>
-      <c r="I34" t="s">
+      <c r="I35" t="s">
         <v>72</v>
       </c>
-      <c r="M34">
-        <v>1</v>
-      </c>
-      <c r="N34">
-        <f>IF(G34="In person",1,0)</f>
-        <v>1</v>
-      </c>
-      <c r="O34">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="D35" s="1" t="s">
+      <c r="M35">
+        <v>1</v>
+      </c>
+      <c r="N35">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="O35">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="D36" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E35" s="3" t="s">
+      <c r="E36" s="3" t="s">
         <v>32</v>
-      </c>
-      <c r="G35" t="s">
-        <v>140</v>
-      </c>
-      <c r="I35" t="s">
-        <v>32</v>
-      </c>
-      <c r="M35">
-        <v>1</v>
-      </c>
-      <c r="N35">
-        <f>IF(G35="In person",1,0)</f>
-        <v>0</v>
-      </c>
-      <c r="O35">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="D36" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="E36" s="1" t="s">
-        <v>160</v>
       </c>
       <c r="G36" t="s">
         <v>140</v>
       </c>
       <c r="I36" t="s">
+        <v>32</v>
+      </c>
+      <c r="M36">
+        <v>1</v>
+      </c>
+      <c r="N36">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="O36">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="D37" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="E37" s="1" t="s">
         <v>159</v>
-      </c>
-      <c r="M36">
-        <v>1</v>
-      </c>
-      <c r="N36">
-        <f>IF(G36="In person",1,0)</f>
-        <v>0</v>
-      </c>
-      <c r="O36">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="D37" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="E37" s="8" t="s">
-        <v>131</v>
       </c>
       <c r="G37" t="s">
         <v>140</v>
       </c>
       <c r="I37" t="s">
+        <v>158</v>
+      </c>
+      <c r="M37">
+        <v>1</v>
+      </c>
+      <c r="N37">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="O37">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="D38" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="M37">
-        <v>1</v>
-      </c>
-      <c r="N37">
-        <f>IF(G37="In person",1,0)</f>
-        <v>0</v>
-      </c>
-      <c r="O37">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="D38" s="1" t="s">
+      <c r="E38" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="G38" t="s">
+        <v>140</v>
+      </c>
+      <c r="I38" t="s">
+        <v>129</v>
+      </c>
+      <c r="M38">
+        <v>1</v>
+      </c>
+      <c r="N38">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="O38">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="D39" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="E38" s="8" t="s">
+      <c r="E39" s="8" t="s">
         <v>62</v>
-      </c>
-      <c r="G38" t="s">
-        <v>122</v>
-      </c>
-      <c r="M38">
-        <v>1</v>
-      </c>
-      <c r="N38">
-        <f>IF(G38="In person",1,0)</f>
-        <v>1</v>
-      </c>
-      <c r="O38">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="D39" t="s">
-        <v>69</v>
-      </c>
-      <c r="E39" s="8" t="s">
-        <v>15</v>
       </c>
       <c r="G39" t="s">
         <v>122</v>
       </c>
-      <c r="I39" t="s">
+      <c r="I39" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="M39">
+        <v>1</v>
+      </c>
+      <c r="N39">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="O39">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="D40" t="s">
         <v>69</v>
       </c>
-      <c r="M39">
-        <v>1</v>
-      </c>
-      <c r="N39">
-        <f>IF(G39="In person",1,0)</f>
-        <v>1</v>
-      </c>
-      <c r="O39">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="D40" t="s">
+      <c r="E40" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="G40" t="s">
+        <v>122</v>
+      </c>
+      <c r="I40" t="s">
+        <v>69</v>
+      </c>
+      <c r="M40">
+        <v>1</v>
+      </c>
+      <c r="N40">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="O40">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="D41" t="s">
         <v>71</v>
       </c>
-      <c r="E40" t="s">
-        <v>179</v>
-      </c>
-      <c r="G40" t="s">
+      <c r="E41" t="s">
+        <v>178</v>
+      </c>
+      <c r="G41" t="s">
         <v>140</v>
       </c>
-      <c r="I40" t="s">
+      <c r="I41" t="s">
         <v>71</v>
       </c>
-      <c r="M40">
-        <v>1</v>
-      </c>
-      <c r="N40">
-        <f>IF(G40="In person",1,0)</f>
-        <v>0</v>
-      </c>
-      <c r="O40">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A42" t="s">
+      <c r="M41">
+        <v>1</v>
+      </c>
+      <c r="N41">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="O41">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
         <v>8</v>
       </c>
-      <c r="B42">
-        <f>SUM(M42:M49)</f>
+      <c r="B43">
+        <f>SUM(M43:M50)</f>
         <v>8</v>
       </c>
-      <c r="D42" t="s">
+      <c r="D43" t="s">
+        <v>171</v>
+      </c>
+      <c r="E43" t="s">
         <v>144</v>
-      </c>
-      <c r="E42" t="s">
-        <v>145</v>
-      </c>
-      <c r="G42" t="s">
-        <v>140</v>
-      </c>
-      <c r="I42" t="s">
-        <v>172</v>
-      </c>
-      <c r="M42">
-        <v>1</v>
-      </c>
-      <c r="N42">
-        <f>IF(G42="In person",1,0)</f>
-        <v>0</v>
-      </c>
-      <c r="O42">
-        <f t="shared" ref="O42:O66" si="2">IF(G42="Virtual",1,0)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="D43" t="s">
-        <v>150</v>
-      </c>
-      <c r="E43" t="s">
-        <v>149</v>
       </c>
       <c r="G43" t="s">
         <v>140</v>
       </c>
       <c r="I43" t="s">
-        <v>150</v>
+        <v>171</v>
       </c>
       <c r="M43">
         <v>1</v>
       </c>
       <c r="N43">
-        <f>IF(G43="In person",1,0)</f>
+        <f t="shared" ref="N43:N50" si="6">IF(G43="In person",1,0)</f>
         <v>0</v>
       </c>
       <c r="O43">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.35">
+        <f t="shared" ref="O43:O67" si="7">IF(G43="Virtual",1,0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D44" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="E44" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="G44" t="s">
         <v>140</v>
       </c>
       <c r="I44" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="M44">
         <v>1</v>
       </c>
       <c r="N44">
-        <f>IF(G44="In person",1,0)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="O44">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="D45" s="1" t="s">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="D45" t="s">
+        <v>151</v>
+      </c>
+      <c r="E45" t="s">
+        <v>150</v>
+      </c>
+      <c r="G45" t="s">
+        <v>140</v>
+      </c>
+      <c r="I45" t="s">
+        <v>151</v>
+      </c>
+      <c r="M45">
+        <v>1</v>
+      </c>
+      <c r="N45">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="O45">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="D46" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="E45" s="1" t="s">
+      <c r="E46" s="1" t="s">
         <v>54</v>
-      </c>
-      <c r="G45" t="s">
-        <v>122</v>
-      </c>
-      <c r="I45" t="s">
-        <v>88</v>
-      </c>
-      <c r="M45">
-        <v>1</v>
-      </c>
-      <c r="N45">
-        <f>IF(G45="In person",1,0)</f>
-        <v>1</v>
-      </c>
-      <c r="O45">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="D46" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="E46" s="8" t="s">
-        <v>137</v>
       </c>
       <c r="G46" t="s">
         <v>122</v>
       </c>
       <c r="I46" t="s">
+        <v>88</v>
+      </c>
+      <c r="M46">
+        <v>1</v>
+      </c>
+      <c r="N46">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="O46">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="D47" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="M46">
-        <v>1</v>
-      </c>
-      <c r="N46">
-        <f>IF(G46="In person",1,0)</f>
-        <v>1</v>
-      </c>
-      <c r="O46">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="D47" s="1" t="s">
+      <c r="E47" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="G47" t="s">
+        <v>122</v>
+      </c>
+      <c r="I47" t="s">
+        <v>136</v>
+      </c>
+      <c r="M47">
+        <v>1</v>
+      </c>
+      <c r="N47">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="O47">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="D48" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="E47" t="s">
-        <v>167</v>
-      </c>
-      <c r="G47" t="s">
-        <v>140</v>
-      </c>
-      <c r="I47" t="s">
-        <v>87</v>
-      </c>
-      <c r="M47">
-        <v>1</v>
-      </c>
-      <c r="N47">
-        <f>IF(G47="In person",1,0)</f>
-        <v>0</v>
-      </c>
-      <c r="O47">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="D48" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="E48" s="8" t="s">
-        <v>56</v>
+      <c r="E48" t="s">
+        <v>166</v>
       </c>
       <c r="G48" t="s">
         <v>140</v>
       </c>
-      <c r="I48" s="1" t="s">
+      <c r="I48" t="s">
+        <v>87</v>
+      </c>
+      <c r="M48">
+        <v>1</v>
+      </c>
+      <c r="N48">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="O48">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="D49" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="M48">
-        <v>1</v>
-      </c>
-      <c r="N48">
-        <f>IF(G48="In person",1,0)</f>
-        <v>0</v>
-      </c>
-      <c r="O48">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="D49" s="1" t="s">
-        <v>184</v>
-      </c>
       <c r="E49" s="8" t="s">
-        <v>185</v>
+        <v>56</v>
       </c>
       <c r="G49" t="s">
         <v>140</v>
       </c>
       <c r="I49" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="M49">
+        <v>1</v>
+      </c>
+      <c r="N49">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="O49">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="D50" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="E50" s="8" t="s">
         <v>184</v>
       </c>
-      <c r="M49">
-        <v>1</v>
-      </c>
-      <c r="N49">
-        <f>IF(G49="In person",1,0)</f>
-        <v>0</v>
-      </c>
-      <c r="O49">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A51" t="s">
+      <c r="G50" t="s">
+        <v>140</v>
+      </c>
+      <c r="I50" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="M50">
+        <v>1</v>
+      </c>
+      <c r="N50">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="O50">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
         <v>7</v>
       </c>
-      <c r="B51">
-        <f>SUM(M51:M56)</f>
+      <c r="B52">
+        <f>SUM(M52:M57)</f>
         <v>6</v>
       </c>
-      <c r="D51" s="1" t="s">
+      <c r="D52" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="E51" s="1" t="s">
+      <c r="E52" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="G51" t="s">
+      <c r="G52" t="s">
         <v>140</v>
       </c>
-      <c r="I51" t="s">
-        <v>171</v>
-      </c>
-      <c r="M51">
-        <v>1</v>
-      </c>
-      <c r="N51">
-        <f>IF(G51="In person",1,0)</f>
-        <v>0</v>
-      </c>
-      <c r="O51">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="D52" s="1" t="s">
+      <c r="I52" t="s">
+        <v>170</v>
+      </c>
+      <c r="M52">
+        <v>1</v>
+      </c>
+      <c r="N52">
+        <f t="shared" ref="N52:N57" si="8">IF(G52="In person",1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="O52">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="D53" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="E52" s="1" t="s">
+      <c r="E53" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="G52" t="s">
+      <c r="G53" t="s">
         <v>122</v>
       </c>
-      <c r="I52" t="s">
+      <c r="I53" t="s">
         <v>73</v>
       </c>
-      <c r="M52">
-        <v>1</v>
-      </c>
-      <c r="N52">
-        <f>IF(G52="In person",1,0)</f>
-        <v>1</v>
-      </c>
-      <c r="O52">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="D53" s="1" t="s">
+      <c r="M53">
+        <v>1</v>
+      </c>
+      <c r="N53">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="O53">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="D54" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="E53" s="1" t="s">
+      <c r="E54" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="G53" t="s">
+      <c r="G54" t="s">
         <v>140</v>
       </c>
-      <c r="I53" t="s">
-        <v>170</v>
-      </c>
-      <c r="M53">
-        <v>1</v>
-      </c>
-      <c r="N53">
-        <f>IF(G53="In person",1,0)</f>
-        <v>0</v>
-      </c>
-      <c r="O53">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="D54" s="1" t="s">
+      <c r="I54" t="s">
+        <v>169</v>
+      </c>
+      <c r="M54">
+        <v>1</v>
+      </c>
+      <c r="N54">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="O54">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="D55" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="E54" s="1" t="s">
+      <c r="E55" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="G54" t="s">
+      <c r="G55" t="s">
         <v>122</v>
       </c>
-      <c r="I54" t="s">
+      <c r="I55" t="s">
         <v>118</v>
       </c>
-      <c r="M54">
-        <v>1</v>
-      </c>
-      <c r="N54">
-        <f>IF(G54="In person",1,0)</f>
-        <v>1</v>
-      </c>
-      <c r="O54">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="D55" s="1" t="s">
+      <c r="M55">
+        <v>1</v>
+      </c>
+      <c r="N55">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="O55">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="D56" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="E55" s="8" t="s">
+      <c r="E56" s="8" t="s">
         <v>113</v>
-      </c>
-      <c r="G55" t="s">
-        <v>140</v>
-      </c>
-      <c r="I55" t="s">
-        <v>110</v>
-      </c>
-      <c r="M55">
-        <v>1</v>
-      </c>
-      <c r="N55">
-        <f>IF(G55="In person",1,0)</f>
-        <v>0</v>
-      </c>
-      <c r="O55">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="D56" t="s">
-        <v>183</v>
-      </c>
-      <c r="E56" t="s">
-        <v>112</v>
       </c>
       <c r="G56" t="s">
         <v>140</v>
       </c>
       <c r="I56" t="s">
-        <v>183</v>
+        <v>110</v>
       </c>
       <c r="M56">
         <v>1</v>
       </c>
       <c r="N56">
-        <f>IF(G56="In person",1,0)</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="O56">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A58" t="s">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="D57" t="s">
+        <v>182</v>
+      </c>
+      <c r="E57" t="s">
+        <v>112</v>
+      </c>
+      <c r="G57" t="s">
+        <v>140</v>
+      </c>
+      <c r="I57" t="s">
+        <v>182</v>
+      </c>
+      <c r="M57">
+        <v>1</v>
+      </c>
+      <c r="N57">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="O57">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>152</v>
+      </c>
+      <c r="B59">
+        <f>SUM(M59:M67)</f>
+        <v>9</v>
+      </c>
+      <c r="D59" t="s">
         <v>153</v>
       </c>
-      <c r="B58">
-        <f>SUM(M58:M66)</f>
-        <v>9</v>
-      </c>
-      <c r="D58" t="s">
-        <v>154</v>
-      </c>
-      <c r="E58" t="s">
+      <c r="E59" t="s">
+        <v>155</v>
+      </c>
+      <c r="G59" t="s">
+        <v>122</v>
+      </c>
+      <c r="I59" t="s">
+        <v>153</v>
+      </c>
+      <c r="M59">
+        <v>1</v>
+      </c>
+      <c r="N59">
+        <f t="shared" ref="N59:N64" si="9">IF(G59="In person",1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="O59">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="D60" t="s">
         <v>156</v>
       </c>
-      <c r="G58" t="s">
-        <v>122</v>
-      </c>
-      <c r="I58" t="s">
-        <v>154</v>
-      </c>
-      <c r="M58">
-        <v>1</v>
-      </c>
-      <c r="N58">
-        <f>IF(G58="In person",1,0)</f>
-        <v>1</v>
-      </c>
-      <c r="O58">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="D59" t="s">
+      <c r="E60" t="s">
         <v>157</v>
-      </c>
-      <c r="E59" t="s">
-        <v>158</v>
-      </c>
-      <c r="G59" t="s">
-        <v>140</v>
-      </c>
-      <c r="I59" t="s">
-        <v>175</v>
-      </c>
-      <c r="M59">
-        <v>1</v>
-      </c>
-      <c r="N59">
-        <f>IF(G59="In person",1,0)</f>
-        <v>0</v>
-      </c>
-      <c r="O59">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="D60" t="s">
-        <v>161</v>
-      </c>
-      <c r="E60" t="s">
-        <v>162</v>
       </c>
       <c r="G60" t="s">
         <v>140</v>
       </c>
       <c r="I60" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="M60">
         <v>1</v>
       </c>
       <c r="N60">
-        <f>IF(G60="In person",1,0)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="O60">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="D61" s="1" t="s">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="D61" t="s">
+        <v>160</v>
+      </c>
+      <c r="E61" t="s">
+        <v>161</v>
+      </c>
+      <c r="G61" t="s">
+        <v>140</v>
+      </c>
+      <c r="I61" t="s">
+        <v>176</v>
+      </c>
+      <c r="M61">
+        <v>1</v>
+      </c>
+      <c r="N61">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="O61">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="D62" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E61" s="1" t="s">
+      <c r="E62" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G61" t="s">
+      <c r="G62" t="s">
         <v>122</v>
       </c>
-      <c r="I61" t="s">
+      <c r="I62" t="s">
         <v>22</v>
       </c>
-      <c r="M61">
-        <v>1</v>
-      </c>
-      <c r="N61">
-        <f>IF(G61="In person",1,0)</f>
-        <v>1</v>
-      </c>
-      <c r="O61">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="D62" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="E62" s="2" t="s">
+      <c r="M62">
+        <v>1</v>
+      </c>
+      <c r="N62">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="O62">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="D63" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="G62" t="s">
-        <v>140</v>
-      </c>
-      <c r="I62" t="s">
-        <v>174</v>
-      </c>
-      <c r="M62">
-        <v>1</v>
-      </c>
-      <c r="N62">
-        <f>IF(G62="In person",1,0)</f>
-        <v>0</v>
-      </c>
-      <c r="O62">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="D63" t="s">
-        <v>178</v>
-      </c>
-      <c r="E63" t="s">
-        <v>180</v>
+      <c r="E63" s="2" t="s">
+        <v>162</v>
       </c>
       <c r="G63" t="s">
         <v>140</v>
       </c>
       <c r="I63" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="M63">
         <v>1</v>
       </c>
       <c r="N63">
-        <f>IF(G63="In person",1,0)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="O63">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.35">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D64" t="s">
-        <v>77</v>
+        <v>177</v>
       </c>
       <c r="E64" t="s">
-        <v>57</v>
+        <v>179</v>
       </c>
       <c r="G64" t="s">
         <v>140</v>
       </c>
       <c r="I64" t="s">
+        <v>177</v>
+      </c>
+      <c r="M64">
+        <v>1</v>
+      </c>
+      <c r="N64">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="O64">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="D65" t="s">
         <v>77</v>
       </c>
-      <c r="M64">
-        <v>1</v>
-      </c>
-      <c r="N64">
-        <f t="shared" ref="N64:N66" si="3">IF(G64="In person",1,0)</f>
-        <v>0</v>
-      </c>
-      <c r="O64">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="65" spans="4:15" x14ac:dyDescent="0.35">
-      <c r="D65" t="s">
-        <v>176</v>
-      </c>
       <c r="E65" t="s">
-        <v>181</v>
+        <v>57</v>
       </c>
       <c r="G65" t="s">
         <v>140</v>
       </c>
       <c r="I65" t="s">
-        <v>176</v>
+        <v>77</v>
       </c>
       <c r="M65">
         <v>1</v>
       </c>
       <c r="N65">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="N65:N67" si="10">IF(G65="In person",1,0)</f>
         <v>0</v>
       </c>
       <c r="O65">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="66" spans="4:15" x14ac:dyDescent="0.35">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D66" t="s">
-        <v>74</v>
+        <v>175</v>
       </c>
       <c r="E66" t="s">
-        <v>13</v>
+        <v>180</v>
       </c>
       <c r="G66" t="s">
         <v>140</v>
       </c>
       <c r="I66" t="s">
+        <v>175</v>
+      </c>
+      <c r="M66">
+        <v>1</v>
+      </c>
+      <c r="N66">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="O66">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="D67" t="s">
         <v>74</v>
       </c>
-      <c r="M66">
-        <v>1</v>
-      </c>
-      <c r="N66">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="O66">
-        <f t="shared" si="2"/>
+      <c r="E67" t="s">
+        <v>13</v>
+      </c>
+      <c r="G67" t="s">
+        <v>140</v>
+      </c>
+      <c r="I67" t="s">
+        <v>74</v>
+      </c>
+      <c r="M67">
+        <v>1</v>
+      </c>
+      <c r="N67">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="O67">
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
     </row>
@@ -2528,26 +2561,26 @@
       <selection activeCell="E5" sqref="E5:F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.1796875" style="1"/>
-    <col min="2" max="2" width="24.7265625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="37.7265625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="25.1796875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="21.26953125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="12.1796875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="11.453125" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="2" width="24.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="37.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="25.140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="21.28515625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="12.140625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="11.42578125" customWidth="1"/>
     <col min="8" max="8" width="11" customWidth="1"/>
-    <col min="9" max="9" width="10.81640625" customWidth="1"/>
-    <col min="10" max="10" width="10.54296875" customWidth="1"/>
+    <col min="9" max="9" width="10.85546875" customWidth="1"/>
+    <col min="10" max="10" width="10.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B3" s="7" t="s">
         <v>4</v>
       </c>
@@ -2559,7 +2592,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B4" s="7"/>
       <c r="E4" s="1" t="s">
         <v>124</v>
@@ -2569,7 +2602,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B5" s="7"/>
       <c r="E5" s="1" t="s">
         <v>125</v>
@@ -2579,11 +2612,11 @@
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B6" s="7"/>
       <c r="F6"/>
     </row>
-    <row r="7" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>1</v>
       </c>
@@ -2609,11 +2642,11 @@
         <v>121</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E8"/>
       <c r="F8"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>5</v>
       </c>
@@ -2634,7 +2667,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="B10" s="1" t="s">
         <v>141</v>
@@ -2660,7 +2693,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" s="1" t="s">
         <v>142</v>
@@ -2686,7 +2719,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
       <c r="B12" s="1" t="s">
         <v>143</v>
@@ -2712,7 +2745,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
       <c r="B13" s="1" t="s">
         <v>29</v>
@@ -2738,7 +2771,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="E14" t="str">
         <f t="shared" si="0"/>
@@ -2749,10 +2782,10 @@
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>31</v>
@@ -2775,7 +2808,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="B16" s="1" t="s">
         <v>66</v>
@@ -2801,7 +2834,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
       <c r="B17" s="1" t="s">
         <v>65</v>
@@ -2827,7 +2860,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="B18" s="1" t="s">
         <v>116</v>
@@ -2847,7 +2880,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
       <c r="B19" s="1" t="s">
         <v>64</v>
@@ -2873,7 +2906,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
       <c r="B20" s="1" t="s">
         <v>43</v>
@@ -2899,7 +2932,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
       <c r="B21" s="1" t="s">
         <v>101</v>
@@ -2925,7 +2958,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
       <c r="B22" s="1" t="s">
         <v>105</v>
@@ -2948,7 +2981,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="4"/>
       <c r="E23" t="str">
         <f t="shared" si="0"/>
@@ -2956,7 +2989,7 @@
       </c>
       <c r="F23"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>6</v>
       </c>
@@ -2969,7 +3002,7 @@
         <v/>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
       <c r="B25" s="1" t="s">
         <v>126</v>
@@ -2988,7 +3021,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
       <c r="B26" s="1" t="s">
         <v>33</v>
@@ -3011,7 +3044,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
       <c r="B27" s="1" t="s">
         <v>67</v>
@@ -3034,7 +3067,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
       <c r="B28" s="1" t="s">
         <v>68</v>
@@ -3060,7 +3093,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
       <c r="B29" s="1" t="s">
         <v>69</v>
@@ -3083,7 +3116,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="4"/>
       <c r="B30" s="1" t="s">
         <v>70</v>
@@ -3106,7 +3139,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="4"/>
       <c r="B31" s="2" t="s">
         <v>71</v>
@@ -3129,7 +3162,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="4"/>
       <c r="B32" s="1" t="s">
         <v>129</v>
@@ -3146,7 +3179,7 @@
         <v/>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="4"/>
       <c r="B33" s="1" t="s">
         <v>72</v>
@@ -3169,7 +3202,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="4"/>
       <c r="B34" s="1" t="s">
         <v>130</v>
@@ -3186,7 +3219,7 @@
         <v/>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="4"/>
       <c r="B35" s="1" t="s">
         <v>133</v>
@@ -3200,13 +3233,13 @@
       </c>
       <c r="F35"/>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="4"/>
       <c r="C36" s="8"/>
       <c r="E36"/>
       <c r="F36"/>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
         <v>7</v>
       </c>
@@ -3219,7 +3252,7 @@
         <v/>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="4"/>
       <c r="B38" s="1" t="s">
         <v>73</v>
@@ -3242,7 +3275,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="4"/>
       <c r="B39" s="1" t="s">
         <v>107</v>
@@ -3262,7 +3295,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="4"/>
       <c r="B40" s="1" t="s">
         <v>109</v>
@@ -3279,7 +3312,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="4"/>
       <c r="B41" s="1" t="s">
         <v>110</v>
@@ -3296,7 +3329,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="4"/>
       <c r="B42" s="1" t="s">
         <v>111</v>
@@ -3313,7 +3346,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="4"/>
       <c r="B43" s="1" t="s">
         <v>118</v>
@@ -3330,12 +3363,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="4"/>
       <c r="E44"/>
       <c r="F44"/>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
         <v>12</v>
       </c>
@@ -3348,7 +3381,7 @@
         <v/>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="4"/>
       <c r="B46" s="1" t="s">
         <v>74</v>
@@ -3371,7 +3404,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="4"/>
       <c r="B47" s="1" t="s">
         <v>75</v>
@@ -3388,7 +3421,7 @@
         <v/>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="4"/>
       <c r="B48" s="1" t="s">
         <v>76</v>
@@ -3411,12 +3444,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="4"/>
       <c r="E49"/>
       <c r="F49"/>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
         <v>21</v>
       </c>
@@ -3429,7 +3462,7 @@
         <v/>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="4"/>
       <c r="B51" s="1" t="s">
         <v>22</v>
@@ -3452,7 +3485,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="4"/>
       <c r="B52" s="1" t="s">
         <v>77</v>
@@ -3469,7 +3502,7 @@
         <v/>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="4"/>
       <c r="E53" t="str">
         <f t="shared" si="4"/>
@@ -3480,7 +3513,7 @@
         <v/>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
         <v>16</v>
       </c>
@@ -3493,7 +3526,7 @@
         <v/>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="4"/>
       <c r="B55" s="1" t="s">
         <v>78</v>
@@ -3516,7 +3549,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="4"/>
       <c r="B56" s="1" t="s">
         <v>25</v>
@@ -3539,7 +3572,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="4"/>
       <c r="B57" s="1" t="s">
         <v>79</v>
@@ -3562,7 +3595,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="4"/>
       <c r="B58" s="2" t="s">
         <v>41</v>
@@ -3585,7 +3618,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="4"/>
       <c r="B59" s="1" t="s">
         <v>80</v>
@@ -3608,7 +3641,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="4"/>
       <c r="B60" s="1" t="s">
         <v>81</v>
@@ -3625,7 +3658,7 @@
         <v/>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="4"/>
       <c r="B61" s="1" t="s">
         <v>82</v>
@@ -3642,7 +3675,7 @@
         <v/>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="4"/>
       <c r="B62" s="1" t="s">
         <v>83</v>
@@ -3659,7 +3692,7 @@
         <v/>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="4"/>
       <c r="B63" s="1" t="s">
         <v>84</v>
@@ -3676,7 +3709,7 @@
         <v/>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="4"/>
       <c r="B64" s="1" t="s">
         <v>85</v>
@@ -3699,7 +3732,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" s="4"/>
       <c r="B65" s="1" t="s">
         <v>58</v>
@@ -3722,7 +3755,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" s="4"/>
       <c r="B66" s="1" t="s">
         <v>92</v>
@@ -3745,7 +3778,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" s="4"/>
       <c r="B67" s="1" t="s">
         <v>93</v>
@@ -3768,7 +3801,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" s="4"/>
       <c r="B68" s="1" t="s">
         <v>96</v>
@@ -3788,7 +3821,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" s="4"/>
       <c r="C69" s="2"/>
       <c r="E69" t="str">
@@ -3800,7 +3833,7 @@
         <v/>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" s="4" t="s">
         <v>8</v>
       </c>
@@ -3813,7 +3846,7 @@
         <v/>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" s="4"/>
       <c r="B71" s="1" t="s">
         <v>136</v>
@@ -3830,7 +3863,7 @@
         <v/>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" s="4"/>
       <c r="B72" s="1" t="s">
         <v>86</v>
@@ -3847,7 +3880,7 @@
         <v/>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" s="4"/>
       <c r="B73" s="1" t="s">
         <v>87</v>
@@ -3870,7 +3903,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" s="4"/>
       <c r="B74" s="1" t="s">
         <v>88</v>
@@ -3893,7 +3926,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" s="4"/>
       <c r="B75" s="1" t="s">
         <v>89</v>
@@ -3916,7 +3949,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" s="4"/>
       <c r="B76" s="1" t="s">
         <v>138</v>
@@ -3936,23 +3969,23 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" s="4"/>
       <c r="E77"/>
       <c r="F77"/>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E78"/>
       <c r="F78"/>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E79"/>
       <c r="F79"/>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B80" s="1" t="s">
         <v>58</v>
       </c>
@@ -3962,7 +3995,7 @@
       <c r="E80"/>
       <c r="F80"/>
     </row>
-    <row r="81" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="81" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B81" s="1" t="s">
         <v>60</v>
       </c>
@@ -3972,7 +4005,7 @@
       <c r="E81"/>
       <c r="F81"/>
     </row>
-    <row r="82" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="82" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B82" s="1" t="s">
         <v>126</v>
       </c>
@@ -3985,7 +4018,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="83" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="83" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B83" s="1" t="s">
         <v>114</v>
       </c>
@@ -3998,18 +4031,18 @@
         <v>122</v>
       </c>
     </row>
-    <row r="84" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="84" spans="2:8" x14ac:dyDescent="0.25">
       <c r="E84"/>
       <c r="F84"/>
     </row>
-    <row r="85" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="85" spans="2:8" x14ac:dyDescent="0.25">
       <c r="E85"/>
       <c r="F85"/>
     </row>
-    <row r="86" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="86" spans="2:8" x14ac:dyDescent="0.25">
       <c r="F86"/>
     </row>
-    <row r="87" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="87" spans="2:8" x14ac:dyDescent="0.25">
       <c r="F87"/>
     </row>
   </sheetData>
@@ -4027,12 +4060,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="37.453125" customWidth="1"/>
+    <col min="1" max="1" width="37.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>135</v>
       </c>
@@ -4040,7 +4073,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="str">
         <f>IF('list-pre-google-forms'!E10=1,'list-pre-google-forms'!C10,"")</f>
         <v>Nicolas.Rolland@dfo-mpo.gc.ca</v>
@@ -4050,7 +4083,7 @@
         <v>Nicolas.Rolland@dfo-mpo.gc.ca</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="str">
         <f>IF('list-pre-google-forms'!E11=1,'list-pre-google-forms'!C11,"")</f>
         <v>Francois-Etienne.Sylvain@dfo-mpo.gc.ca</v>
@@ -4060,7 +4093,7 @@
         <v>Francois-Etienne.Sylvain@dfo-mpo.gc.ca</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="str">
         <f>IF('list-pre-google-forms'!E12=1,'list-pre-google-forms'!C12,"")</f>
         <v>Jolene.Sutton@dfo-mpo.gc.ca</v>
@@ -4070,7 +4103,7 @@
         <v>Jolene.Sutton@dfo-mpo.gc.ca</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="str">
         <f>IF('list-pre-google-forms'!E13=1,'list-pre-google-forms'!C13,"")</f>
         <v>Suncica.Avlijas@dfo-mpo.gc.ca</v>
@@ -4080,7 +4113,7 @@
         <v>Suncica.Avlijas@dfo-mpo.gc.ca</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="str">
         <f>IF('list-pre-google-forms'!E14=1,'list-pre-google-forms'!C14,"")</f>
         <v/>
@@ -4090,7 +4123,7 @@
         <v/>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="str">
         <f>IF('list-pre-google-forms'!E15=1,'list-pre-google-forms'!C15,"")</f>
         <v>Karen.Robertson@dfo-mpo.gc.ca</v>
@@ -4100,7 +4133,7 @@
         <v>Karen.Robertson@dfo-mpo.gc.ca</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="str">
         <f>IF('list-pre-google-forms'!E16=1,'list-pre-google-forms'!C16,"")</f>
         <v>Joeleen.Savoie@dfo-mpo.gc.ca</v>
@@ -4110,7 +4143,7 @@
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="str">
         <f>IF('list-pre-google-forms'!E17=1,'list-pre-google-forms'!C17,"")</f>
         <v>Marie-France.Robichaud@dfo-mpo.gc.ca</v>
@@ -4120,7 +4153,7 @@
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="str">
         <f>IF('list-pre-google-forms'!E18=1,'list-pre-google-forms'!C18,"")</f>
         <v>Sylvie.Robichaud@dfo-mpo.gc.ca</v>
@@ -4130,7 +4163,7 @@
         <v>Sylvie.Robichaud@dfo-mpo.gc.ca</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="str">
         <f>IF('list-pre-google-forms'!E19=1,'list-pre-google-forms'!C19,"")</f>
         <v>Andrew.Darcy@dfo-mpo.gc.ca</v>
@@ -4140,7 +4173,7 @@
         <v>Andrew.Darcy@dfo-mpo.gc.ca</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="str">
         <f>IF('list-pre-google-forms'!E20=1,'list-pre-google-forms'!C20,"")</f>
         <v>abby.daigle@dfo-mpo.gc.ca</v>
@@ -4150,7 +4183,7 @@
         <v>abby.daigle@dfo-mpo.gc.ca</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="str">
         <f>IF('list-pre-google-forms'!E21=1,'list-pre-google-forms'!C21,"")</f>
         <v>matthew.horsman@dfo-mpo.gc.ca</v>
@@ -4160,7 +4193,7 @@
         <v>matthew.horsman@dfo-mpo.gc.ca</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="str">
         <f>IF('list-pre-google-forms'!E22=1,'list-pre-google-forms'!C22,"")</f>
         <v>kirby.morrill@dfo-mpo.gc.ca</v>
@@ -4170,7 +4203,7 @@
         <v>kirby.morrill@dfo-mpo.gc.ca</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="str">
         <f>IF('list-pre-google-forms'!E23=1,'list-pre-google-forms'!C23,"")</f>
         <v/>
@@ -4180,7 +4213,7 @@
         <v/>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="str">
         <f>IF('list-pre-google-forms'!E24=1,'list-pre-google-forms'!C24,"")</f>
         <v/>
@@ -4190,7 +4223,7 @@
         <v/>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="str">
         <f>IF('list-pre-google-forms'!E25=1,'list-pre-google-forms'!C25,"")</f>
         <v>Peter.Comeau@dfo-mpo.gc.ca</v>
@@ -4200,7 +4233,7 @@
         <v>Peter.Comeau@dfo-mpo.gc.ca</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="str">
         <f>IF('list-pre-google-forms'!E26=1,'list-pre-google-forms'!C26,"")</f>
         <v>Nell.denHeyer@dfo-mpo.gc.ca</v>
@@ -4210,7 +4243,7 @@
         <v>Nell.denHeyer@dfo-mpo.gc.ca</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="str">
         <f>IF('list-pre-google-forms'!E27=1,'list-pre-google-forms'!C27,"")</f>
         <v>Quinn.McCurdy@dfo-mpo.gc.ca</v>
@@ -4220,7 +4253,7 @@
         <v>Quinn.McCurdy@dfo-mpo.gc.ca</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="str">
         <f>IF('list-pre-google-forms'!E28=1,'list-pre-google-forms'!C28,"")</f>
         <v>Dheeraj.Busawon@dfo-mpo.gc.ca</v>
@@ -4230,7 +4263,7 @@
         <v/>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="str">
         <f>IF('list-pre-google-forms'!E29=1,'list-pre-google-forms'!C29,"")</f>
         <v>George.Nau@dfo-mpo.gc.ca</v>
@@ -4240,7 +4273,7 @@
         <v>George.Nau@dfo-mpo.gc.ca</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="str">
         <f>IF('list-pre-google-forms'!E30=1,'list-pre-google-forms'!C30,"")</f>
         <v>Mark.Billard@dfo-mpo.gc.ca</v>
@@ -4250,7 +4283,7 @@
         <v>Mark.Billard@dfo-mpo.gc.ca</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="str">
         <f>IF('list-pre-google-forms'!E31=1,'list-pre-google-forms'!C31,"")</f>
         <v>lynn.collier@dfo-mpo.gc.ca</v>
@@ -4260,7 +4293,7 @@
         <v>lynn.collier@dfo-mpo.gc.ca</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="str">
         <f>IF('list-pre-google-forms'!E32=1,'list-pre-google-forms'!C32,"")</f>
         <v>Kelly.Kraska@dfo-mpo.gc.ca</v>
@@ -4270,7 +4303,7 @@
         <v/>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="str">
         <f>IF('list-pre-google-forms'!E33=1,'list-pre-google-forms'!C33,"")</f>
         <v>Tania.Davignon-Burton@dfo-mpo.gc.ca</v>
@@ -4280,7 +4313,7 @@
         <v>Tania.Davignon-Burton@dfo-mpo.gc.ca</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="str">
         <f>IF('list-pre-google-forms'!E34=1,'list-pre-google-forms'!C34,"")</f>
         <v>Gregory.Puncher@dfo-mpo.gc.ca</v>
@@ -4290,7 +4323,7 @@
         <v/>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="str">
         <f>IF('list-pre-google-forms'!E35=1,'list-pre-google-forms'!C35,"")</f>
         <v>Catriona.Regnier-McKellar@dfo-mpo.gc.ca</v>
@@ -4300,7 +4333,7 @@
         <v/>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="str">
         <f>IF('list-pre-google-forms'!E36=1,'list-pre-google-forms'!C36,"")</f>
         <v/>
@@ -4310,7 +4343,7 @@
         <v/>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="str">
         <f>IF('list-pre-google-forms'!E37=1,'list-pre-google-forms'!C37,"")</f>
         <v/>
@@ -4320,7 +4353,7 @@
         <v/>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="str">
         <f>IF('list-pre-google-forms'!E38=1,'list-pre-google-forms'!C38,"")</f>
         <v>Kim.Emond@dfo-mpo.gc.ca</v>
@@ -4330,7 +4363,7 @@
         <v>Kim.Emond@dfo-mpo.gc.ca</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="str">
         <f>IF('list-pre-google-forms'!E39=1,'list-pre-google-forms'!C39,"")</f>
         <v>Nicolas.LeCorre@dfo-mpo.gc.ca</v>
@@ -4340,7 +4373,7 @@
         <v>Nicolas.LeCorre@dfo-mpo.gc.ca</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="str">
         <f>IF('list-pre-google-forms'!E40=1,'list-pre-google-forms'!C40,"")</f>
         <v>andrew.smith4@dfo-mpo.gc.ca</v>
@@ -4350,7 +4383,7 @@
         <v>andrew.smith4@dfo-mpo.gc.ca</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="str">
         <f>IF('list-pre-google-forms'!E41=1,'list-pre-google-forms'!C41,"")</f>
         <v>Renald.Belley@dfo-mpo.gc.ca</v>
@@ -4360,7 +4393,7 @@
         <v>Renald.Belley@dfo-mpo.gc.ca</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="str">
         <f>IF('list-pre-google-forms'!E42=1,'list-pre-google-forms'!C42,"")</f>
         <v>Mathieu.Desgagnes@dfo-mpo.gc.ca</v>
@@ -4370,7 +4403,7 @@
         <v>Mathieu.Desgagnes@dfo-mpo.gc.ca</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="str">
         <f>IF('list-pre-google-forms'!E43=1,'list-pre-google-forms'!C43,"")</f>
         <v>helene.dionne@dfo-mpo.gc.ca</v>
@@ -4380,7 +4413,7 @@
         <v>helene.dionne@dfo-mpo.gc.ca</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="str">
         <f>IF('list-pre-google-forms'!E44=1,'list-pre-google-forms'!C44,"")</f>
         <v/>
@@ -4390,7 +4423,7 @@
         <v/>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="str">
         <f>IF('list-pre-google-forms'!E45=1,'list-pre-google-forms'!C45,"")</f>
         <v/>
@@ -4400,7 +4433,7 @@
         <v/>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="str">
         <f>IF('list-pre-google-forms'!E46=1,'list-pre-google-forms'!C46,"")</f>
         <v>Laura.Alsip@dfo-mpo.gc.ca</v>
@@ -4410,7 +4443,7 @@
         <v>Laura.Alsip@dfo-mpo.gc.ca</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="str">
         <f>IF('list-pre-google-forms'!E47=1,'list-pre-google-forms'!C47,"")</f>
         <v>Wojciech.Walkusz@dfo-mpo.gc.ca</v>
@@ -4420,7 +4453,7 @@
         <v/>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="str">
         <f>IF('list-pre-google-forms'!E48=1,'list-pre-google-forms'!C48,"")</f>
         <v>Lauren.Wiens@dfo-mpo.gc.ca</v>
@@ -4430,7 +4463,7 @@
         <v>Lauren.Wiens@dfo-mpo.gc.ca</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="str">
         <f>IF('list-pre-google-forms'!E49=1,'list-pre-google-forms'!C49,"")</f>
         <v/>
@@ -4440,7 +4473,7 @@
         <v/>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="str">
         <f>IF('list-pre-google-forms'!E50=1,'list-pre-google-forms'!C50,"")</f>
         <v/>
@@ -4450,7 +4483,7 @@
         <v/>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="str">
         <f>IF('list-pre-google-forms'!E51=1,'list-pre-google-forms'!C51,"")</f>
         <v>Tracey.Loewen@dfo-mpo.gc.ca</v>
@@ -4460,7 +4493,7 @@
         <v>Tracey.Loewen@dfo-mpo.gc.ca</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="str">
         <f>IF('list-pre-google-forms'!E52=1,'list-pre-google-forms'!C52,"")</f>
         <v>Brendan.Malley@dfo-mpo.gc.ca</v>
@@ -4470,7 +4503,7 @@
         <v/>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="str">
         <f>IF('list-pre-google-forms'!E53=1,'list-pre-google-forms'!C53,"")</f>
         <v/>
@@ -4480,7 +4513,7 @@
         <v/>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="str">
         <f>IF('list-pre-google-forms'!E54=1,'list-pre-google-forms'!C54,"")</f>
         <v/>
@@ -4490,7 +4523,7 @@
         <v/>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="str">
         <f>IF('list-pre-google-forms'!E55=1,'list-pre-google-forms'!C55,"")</f>
         <v>Sarah.Hawkshaw@dfo-mpo.gc.ca</v>
@@ -4500,7 +4533,7 @@
         <v>Sarah.Hawkshaw@dfo-mpo.gc.ca</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="str">
         <f>IF('list-pre-google-forms'!E56=1,'list-pre-google-forms'!C56,"")</f>
         <v>Madeline.Lavery@dfo-mpo.gc.ca</v>
@@ -4510,7 +4543,7 @@
         <v>Madeline.Lavery@dfo-mpo.gc.ca</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="str">
         <f>IF('list-pre-google-forms'!E57=1,'list-pre-google-forms'!C57,"")</f>
         <v>Emily.Yungwirth@dfo-mpo.gc.ca</v>
@@ -4520,7 +4553,7 @@
         <v>Emily.Yungwirth@dfo-mpo.gc.ca</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="str">
         <f>IF('list-pre-google-forms'!E58=1,'list-pre-google-forms'!C58,"")</f>
         <v>dana.haggarty@dfo-mpo.gc.ca</v>
@@ -4530,7 +4563,7 @@
         <v>dana.haggarty@dfo-mpo.gc.ca</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="str">
         <f>IF('list-pre-google-forms'!E59=1,'list-pre-google-forms'!C59,"")</f>
         <v>Kendra.Holt@dfo-mpo.gc.ca</v>
@@ -4540,7 +4573,7 @@
         <v>Kendra.Holt@dfo-mpo.gc.ca</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="str">
         <f>IF('list-pre-google-forms'!E60=1,'list-pre-google-forms'!C60,"")</f>
         <v>Matthew.Siegle@dfo-mpo.gc.ca</v>
@@ -4550,7 +4583,7 @@
         <v/>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="str">
         <f>IF('list-pre-google-forms'!E61=1,'list-pre-google-forms'!C61,"")</f>
         <v>Mackenzie.Mazur@dfo-mpo.gc.ca</v>
@@ -4560,7 +4593,7 @@
         <v/>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="str">
         <f>IF('list-pre-google-forms'!E62=1,'list-pre-google-forms'!C62,"")</f>
         <v>Karalea.Cantera@dfo-mpo.gc.ca</v>
@@ -4570,7 +4603,7 @@
         <v/>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="str">
         <f>IF('list-pre-google-forms'!E63=1,'list-pre-google-forms'!C63,"")</f>
         <v>Kiana.Matwichuk@dfo-mpo.gc.ca</v>
@@ -4580,7 +4613,7 @@
         <v/>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="str">
         <f>IF('list-pre-google-forms'!E64=1,'list-pre-google-forms'!C64,"")</f>
         <v>Erin.Herder@dfo-mpo.gc.ca</v>
@@ -4590,7 +4623,7 @@
         <v>Erin.Herder@dfo-mpo.gc.ca</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="str">
         <f>IF('list-pre-google-forms'!E65=1,'list-pre-google-forms'!C65,"")</f>
         <v>Robyn.Forrest@dfo-mpo.gc.ca</v>
@@ -4600,7 +4633,7 @@
         <v>Robyn.Forrest@dfo-mpo.gc.ca</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="str">
         <f>IF('list-pre-google-forms'!E66=1,'list-pre-google-forms'!C66,"")</f>
         <v>yeongha.jung@dfo-mpo.gc.ca</v>
@@ -4610,7 +4643,7 @@
         <v>yeongha.jung@dfo-mpo.gc.ca</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="str">
         <f>IF('list-pre-google-forms'!E67=1,'list-pre-google-forms'!C67,"")</f>
         <v>barbara.campbell@dfo-mpo.gc.ca</v>
@@ -4620,7 +4653,7 @@
         <v>barbara.campbell@dfo-mpo.gc.ca</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="str">
         <f>IF('list-pre-google-forms'!E68=1,'list-pre-google-forms'!C68,"")</f>
         <v>stephen.wischniowski@dfo-mpo.gc.ca</v>
@@ -4630,7 +4663,7 @@
         <v/>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="str">
         <f>IF('list-pre-google-forms'!E69=1,'list-pre-google-forms'!C69,"")</f>
         <v/>
@@ -4640,7 +4673,7 @@
         <v/>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="str">
         <f>IF('list-pre-google-forms'!E70=1,'list-pre-google-forms'!C70,"")</f>
         <v/>
@@ -4650,7 +4683,7 @@
         <v/>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="str">
         <f>IF('list-pre-google-forms'!E71=1,'list-pre-google-forms'!C71,"")</f>
         <v>Gillian.Forbes@dfo-mpo.gc.ca</v>
@@ -4660,7 +4693,7 @@
         <v/>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="str">
         <f>IF('list-pre-google-forms'!E72=1,'list-pre-google-forms'!C72,"")</f>
         <v>Divya.Varkey@dfo-mpo.gc.ca</v>
@@ -4670,7 +4703,7 @@
         <v/>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="str">
         <f>IF('list-pre-google-forms'!E73=1,'list-pre-google-forms'!C73,"")</f>
         <v>Aaron.Adamack@dfo-mpo.gc.ca</v>
@@ -4680,7 +4713,7 @@
         <v>Aaron.Adamack@dfo-mpo.gc.ca</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="str">
         <f>IF('list-pre-google-forms'!E74=1,'list-pre-google-forms'!C74,"")</f>
         <v>Meredith.Schofield@dfo-mpo.gc.ca</v>
@@ -4690,7 +4723,7 @@
         <v>Meredith.Schofield@dfo-mpo.gc.ca</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="str">
         <f>IF('list-pre-google-forms'!E75=1,'list-pre-google-forms'!C75,"")</f>
         <v>Andrea.Perreault@dfo-mpo.gc.ca</v>
@@ -4700,7 +4733,7 @@
         <v>Andrea.Perreault@dfo-mpo.gc.ca</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" t="str">
         <f>IF('list-pre-google-forms'!E76=1,'list-pre-google-forms'!C76,"")</f>
         <v>Laura.Wheeland@dfo-mpo.gc.ca</v>
@@ -4710,7 +4743,7 @@
         <v>Laura.Wheeland@dfo-mpo.gc.ca</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" t="str">
         <f>IF('list-pre-google-forms'!E77=1,'list-pre-google-forms'!C77,"")</f>
         <v/>
@@ -4720,7 +4753,7 @@
         <v/>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="str">
         <f>IF('list-pre-google-forms'!E78=1,'list-pre-google-forms'!C78,"")</f>
         <v/>
@@ -4730,7 +4763,7 @@
         <v/>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" t="str">
         <f>IF('list-pre-google-forms'!E79=1,'list-pre-google-forms'!C79,"")</f>
         <v/>
@@ -4740,7 +4773,7 @@
         <v/>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" t="str">
         <f>IF('list-pre-google-forms'!E80=1,'list-pre-google-forms'!C80,"")</f>
         <v/>
@@ -4750,7 +4783,7 @@
         <v/>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" t="str">
         <f>IF('list-pre-google-forms'!E81=1,'list-pre-google-forms'!C81,"")</f>
         <v/>
@@ -4760,7 +4793,7 @@
         <v/>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" t="str">
         <f>IF('list-pre-google-forms'!E82=1,'list-pre-google-forms'!C82,"")</f>
         <v/>
@@ -4770,7 +4803,7 @@
         <v/>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" t="str">
         <f>IF('list-pre-google-forms'!E83=1,'list-pre-google-forms'!C83,"")</f>
         <v/>
@@ -4780,7 +4813,7 @@
         <v/>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B78" t="str">
         <f>IF('list-pre-google-forms'!G88=1,'list-pre-google-forms'!C88,"")</f>
         <v/>

</xml_diff>

<commit_message>
add schedule as Word document, update Karen's talks, add land acknowledgements slides from Robyn and update participants
</commit_message>
<xml_diff>
--- a/planning/workshop-participants.xlsx
+++ b/planning/workshop-participants.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RicardD\Documents\GitHub\ageing-best-practices-2022\planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5408AC26-077E-471F-BD08-9319000FDE09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44CC550F-08DC-4BF9-A66E-D5016B3F7E75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="16440" windowHeight="28440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="16440" windowHeight="28440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="attendance" sheetId="5" r:id="rId1"/>
@@ -2745,7 +2745,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FE87253-3AFE-489E-871D-A05432044822}">
   <dimension ref="A1:Q74"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -6215,7 +6215,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7648514F-C50B-429E-8CE0-7F6A61E6FA38}">
   <dimension ref="A1:O83"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -6588,11 +6588,11 @@
         <v>1</v>
       </c>
       <c r="N19">
-        <f>IF(H19="In person",1,0)</f>
+        <f t="shared" ref="N19:N34" si="2">IF(H19="In person",1,0)</f>
         <v>1</v>
       </c>
       <c r="O19">
-        <f>IF(H19="Virtual",1,0)</f>
+        <f t="shared" ref="O19:O34" si="3">IF(H19="Virtual",1,0)</f>
         <v>0</v>
       </c>
     </row>
@@ -6620,11 +6620,11 @@
         <v>1</v>
       </c>
       <c r="N20">
-        <f>IF(H20="In person",1,0)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="O20">
-        <f>IF(H20="Virtual",1,0)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -6652,11 +6652,11 @@
         <v>1</v>
       </c>
       <c r="N21">
-        <f>IF(H21="In person",1,0)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="O21">
-        <f>IF(H21="Virtual",1,0)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -6684,11 +6684,11 @@
         <v>1</v>
       </c>
       <c r="N22">
-        <f>IF(H22="In person",1,0)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="O22">
-        <f>IF(H22="Virtual",1,0)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -6716,11 +6716,11 @@
         <v>1</v>
       </c>
       <c r="N23">
-        <f>IF(H23="In person",1,0)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="O23">
-        <f>IF(H23="Virtual",1,0)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -6748,11 +6748,11 @@
         <v>1</v>
       </c>
       <c r="N24">
-        <f>IF(H24="In person",1,0)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="O24">
-        <f>IF(H24="Virtual",1,0)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -6780,11 +6780,11 @@
         <v>1</v>
       </c>
       <c r="N25">
-        <f>IF(H25="In person",1,0)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="O25">
-        <f>IF(H25="Virtual",1,0)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -6812,11 +6812,11 @@
         <v>1</v>
       </c>
       <c r="N26">
-        <f>IF(H26="In person",1,0)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="O26">
-        <f>IF(H26="Virtual",1,0)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -6844,11 +6844,11 @@
         <v>1</v>
       </c>
       <c r="N27">
-        <f>IF(H27="In person",1,0)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="O27">
-        <f>IF(H27="Virtual",1,0)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -6876,11 +6876,11 @@
         <v>1</v>
       </c>
       <c r="N28">
-        <f>IF(H28="In person",1,0)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="O28">
-        <f>IF(H28="Virtual",1,0)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -6908,11 +6908,11 @@
         <v>1</v>
       </c>
       <c r="N29">
-        <f>IF(H29="In person",1,0)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="O29">
-        <f>IF(H29="Virtual",1,0)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -6940,11 +6940,11 @@
         <v>1</v>
       </c>
       <c r="N30">
-        <f>IF(H30="In person",1,0)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="O30">
-        <f>IF(H30="Virtual",1,0)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -6972,11 +6972,11 @@
         <v>1</v>
       </c>
       <c r="N31">
-        <f>IF(H31="In person",1,0)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="O31">
-        <f>IF(H31="Virtual",1,0)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -7004,11 +7004,11 @@
         <v>1</v>
       </c>
       <c r="N32">
-        <f>IF(H32="In person",1,0)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="O32">
-        <f>IF(H32="Virtual",1,0)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -7036,11 +7036,11 @@
         <v>1</v>
       </c>
       <c r="N33">
-        <f>IF(H33="In person",1,0)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="O33">
-        <f>IF(H33="Virtual",1,0)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -7068,11 +7068,11 @@
         <v>1</v>
       </c>
       <c r="N34">
-        <f>IF(H34="In person",1,0)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="O34">
-        <f>IF(H34="Virtual",1,0)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -7103,11 +7103,11 @@
         <v>1</v>
       </c>
       <c r="N36">
-        <f t="shared" ref="N36:N49" si="2">IF(H36="In person",1,0)</f>
+        <f t="shared" ref="N36:N49" si="4">IF(H36="In person",1,0)</f>
         <v>0</v>
       </c>
       <c r="O36">
-        <f t="shared" ref="O36:O49" si="3">IF(H36="Virtual",1,0)</f>
+        <f t="shared" ref="O36:O49" si="5">IF(H36="Virtual",1,0)</f>
         <v>1</v>
       </c>
     </row>
@@ -7134,11 +7134,11 @@
         <v>1</v>
       </c>
       <c r="N37">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="O37">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
     </row>
@@ -7165,11 +7165,11 @@
         <v>1</v>
       </c>
       <c r="N38">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="O38">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -7196,11 +7196,11 @@
         <v>1</v>
       </c>
       <c r="N39">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="O39">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
     </row>
@@ -7227,11 +7227,11 @@
         <v>1</v>
       </c>
       <c r="N40">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="O40">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
     </row>
@@ -7258,11 +7258,11 @@
         <v>1</v>
       </c>
       <c r="N41">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="O41">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
     </row>
@@ -7289,11 +7289,11 @@
         <v>1</v>
       </c>
       <c r="N42">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="O42">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -7320,11 +7320,11 @@
         <v>1</v>
       </c>
       <c r="N43">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="O43">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
     </row>
@@ -7351,11 +7351,11 @@
         <v>1</v>
       </c>
       <c r="N44">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="O44">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -7382,11 +7382,11 @@
         <v>1</v>
       </c>
       <c r="N45">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="O45">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -7413,11 +7413,11 @@
         <v>1</v>
       </c>
       <c r="N46">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="O46">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
     </row>
@@ -7444,11 +7444,11 @@
         <v>1</v>
       </c>
       <c r="N47">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="O47">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -7475,11 +7475,11 @@
         <v>1</v>
       </c>
       <c r="N48">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="O48">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
     </row>
@@ -7506,11 +7506,11 @@
         <v>1</v>
       </c>
       <c r="N49">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="O49">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
     </row>
@@ -7541,11 +7541,11 @@
         <v>1</v>
       </c>
       <c r="N51">
-        <f t="shared" ref="N51:N58" si="4">IF(H51="In person",1,0)</f>
+        <f t="shared" ref="N51:N58" si="6">IF(H51="In person",1,0)</f>
         <v>0</v>
       </c>
       <c r="O51">
-        <f t="shared" ref="O51:O58" si="5">IF(H51="Virtual",1,0)</f>
+        <f t="shared" ref="O51:O58" si="7">IF(H51="Virtual",1,0)</f>
         <v>1</v>
       </c>
     </row>
@@ -7572,11 +7572,11 @@
         <v>1</v>
       </c>
       <c r="N52">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="O52">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
     </row>
@@ -7603,11 +7603,11 @@
         <v>1</v>
       </c>
       <c r="N53">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="O53">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
     </row>
@@ -7634,11 +7634,11 @@
         <v>1</v>
       </c>
       <c r="N54">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="O54">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -7665,11 +7665,11 @@
         <v>1</v>
       </c>
       <c r="N55">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="O55">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
     </row>
@@ -7696,11 +7696,11 @@
         <v>1</v>
       </c>
       <c r="N56">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="O56">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
     </row>
@@ -7727,11 +7727,11 @@
         <v>1</v>
       </c>
       <c r="N57">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="O57">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
     </row>
@@ -7758,11 +7758,11 @@
         <v>1</v>
       </c>
       <c r="N58">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="O58">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
     </row>
@@ -7884,11 +7884,11 @@
         <v>1</v>
       </c>
       <c r="N63">
-        <f t="shared" ref="N63:N77" si="6">IF(H63="In person",1,0)</f>
+        <f t="shared" ref="N63:N77" si="8">IF(H63="In person",1,0)</f>
         <v>0</v>
       </c>
       <c r="O63">
-        <f t="shared" ref="O63:O77" si="7">IF(H63="Virtual",1,0)</f>
+        <f t="shared" ref="O63:O77" si="9">IF(H63="Virtual",1,0)</f>
         <v>1</v>
       </c>
     </row>
@@ -7915,11 +7915,11 @@
         <v>1</v>
       </c>
       <c r="N64">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="O64">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
     </row>
@@ -7946,7 +7946,7 @@
         <v>1</v>
       </c>
       <c r="N65">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="O65">
@@ -7976,11 +7976,11 @@
         <v>1</v>
       </c>
       <c r="N66">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="O66">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
     </row>
@@ -8007,11 +8007,11 @@
         <v>1</v>
       </c>
       <c r="N67">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="O67">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
     </row>
@@ -8038,11 +8038,11 @@
         <v>1</v>
       </c>
       <c r="N68">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="O68">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
     </row>
@@ -8069,11 +8069,11 @@
         <v>1</v>
       </c>
       <c r="N69">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="O69">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
     </row>
@@ -8100,11 +8100,11 @@
         <v>1</v>
       </c>
       <c r="N70">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="O70">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
     </row>
@@ -8131,11 +8131,11 @@
         <v>1</v>
       </c>
       <c r="N71">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="O71">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
     </row>
@@ -8162,11 +8162,11 @@
         <v>1</v>
       </c>
       <c r="N72">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="O72">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
     </row>
@@ -8193,11 +8193,11 @@
         <v>1</v>
       </c>
       <c r="N73">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="O73">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
     </row>
@@ -8224,11 +8224,11 @@
         <v>1</v>
       </c>
       <c r="N74">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="O74">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
     </row>
@@ -8255,11 +8255,11 @@
         <v>1</v>
       </c>
       <c r="N75">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="O75">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
     </row>
@@ -8286,11 +8286,11 @@
         <v>1</v>
       </c>
       <c r="N76">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="O76">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
     </row>
@@ -8317,11 +8317,11 @@
         <v>1</v>
       </c>
       <c r="N77">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="O77">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
     </row>
@@ -8352,11 +8352,11 @@
         <v>1</v>
       </c>
       <c r="N79">
-        <f t="shared" ref="N79:N83" si="8">IF(H79="In person",1,0)</f>
+        <f t="shared" ref="N79:N83" si="10">IF(H79="In person",1,0)</f>
         <v>0</v>
       </c>
       <c r="O79">
-        <f t="shared" ref="O79:O83" si="9">IF(H79="Virtual",1,0)</f>
+        <f t="shared" ref="O79:O83" si="11">IF(H79="Virtual",1,0)</f>
         <v>1</v>
       </c>
     </row>
@@ -8383,11 +8383,11 @@
         <v>1</v>
       </c>
       <c r="N80">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="O80">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
@@ -8414,11 +8414,11 @@
         <v>1</v>
       </c>
       <c r="N81">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="O81">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>
@@ -8445,11 +8445,11 @@
         <v>1</v>
       </c>
       <c r="N82">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="O82">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
     </row>
@@ -8476,11 +8476,11 @@
         <v>1</v>
       </c>
       <c r="N83">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="O83">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updates to README, participants and presentations
</commit_message>
<xml_diff>
--- a/planning/workshop-participants.xlsx
+++ b/planning/workshop-participants.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RicardD\Documents\GitHub\ageing-best-practices-2022\planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44CC550F-08DC-4BF9-A66E-D5016B3F7E75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81CD4AD7-66C1-4BCF-BDF2-14BFDED7BCC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="16440" windowHeight="28440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="attendance" sheetId="5" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1041" uniqueCount="305">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1039" uniqueCount="305">
   <si>
     <t>Name</t>
   </si>
@@ -1321,14 +1321,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1351,7 +1351,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="str">
         <f>'for-README'!F4</f>
         <v>Laura Alsip</v>
@@ -1369,7 +1369,7 @@
         <v>Virtual</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" t="str">
         <f>'for-README'!F5</f>
         <v>Lauren Burke</v>
@@ -1387,7 +1387,7 @@
         <v>Virtual</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" t="str">
         <f>'for-README'!F6</f>
         <v>Kevin J Hedges</v>
@@ -1405,7 +1405,7 @@
         <v>Virtual</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" t="str">
         <f>'for-README'!F7</f>
         <v>Michael Legge</v>
@@ -1423,7 +1423,7 @@
         <v>In person</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" t="str">
         <f>'for-README'!F8</f>
         <v>Tracey Loewen</v>
@@ -1441,7 +1441,7 @@
         <v>In person</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" t="str">
         <f>'for-README'!F9</f>
         <v>Brendan K Malley</v>
@@ -1459,7 +1459,7 @@
         <v>Virtual</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" t="str">
         <f>'for-README'!F10</f>
         <v>Lenore J Vandenbyllaardt</v>
@@ -1477,7 +1477,7 @@
         <v>Virtual</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" t="str">
         <f>'for-README'!F11</f>
         <v>Rick J Wastle</v>
@@ -1495,7 +1495,7 @@
         <v>Virtual</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" t="str">
         <f>'for-README'!F12</f>
         <v>Xinhua Zhu</v>
@@ -1513,7 +1513,7 @@
         <v>Virtual</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" t="str">
         <f>'for-README'!F13</f>
         <v>Jacob Burbank</v>
@@ -1540,7 +1540,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" t="str">
         <f>'for-README'!F14</f>
         <v>Abby Daigle</v>
@@ -1567,7 +1567,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" t="str">
         <f>'for-README'!F15</f>
         <v>Andrew Darcy</v>
@@ -1594,7 +1594,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15" t="str">
         <f>'for-README'!F16</f>
         <v>Isabelle Forest</v>
@@ -1621,7 +1621,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16" t="str">
         <f>'for-README'!F17</f>
         <v>Matthew Horsman</v>
@@ -1648,7 +1648,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17" t="str">
         <f>'for-README'!F18</f>
         <v>Samantha Hudson</v>
@@ -1675,7 +1675,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18" t="str">
         <f>'for-README'!F19</f>
         <v>Colin MacFarlane</v>
@@ -1702,7 +1702,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A19" t="str">
         <f>'for-README'!F20</f>
         <v>Kelsey McGee</v>
@@ -1729,7 +1729,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A20" t="str">
         <f>'for-README'!F21</f>
         <v>Kirby Morrill</v>
@@ -1756,7 +1756,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A21" t="str">
         <f>'for-README'!F22</f>
         <v>Daniel Ricard</v>
@@ -1783,7 +1783,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A22" t="str">
         <f>'for-README'!F23</f>
         <v>Karen Robertson</v>
@@ -1810,7 +1810,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A23" t="str">
         <f>'for-README'!F24</f>
         <v>Sylvie Robichaud</v>
@@ -1837,7 +1837,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A24" t="str">
         <f>'for-README'!F25</f>
         <v>Nicolas Rolland</v>
@@ -1858,7 +1858,7 @@
       <c r="F24" s="11"/>
       <c r="G24" s="11"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A25" t="str">
         <f>'for-README'!F26</f>
         <v>Jolene Sutton</v>
@@ -1876,7 +1876,7 @@
         <v>In person</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A26" t="str">
         <f>'for-README'!F27</f>
         <v>François-Étienne Sylvain</v>
@@ -1903,7 +1903,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A27" t="str">
         <f>'for-README'!F29</f>
         <v>Mark Billard</v>
@@ -1921,7 +1921,7 @@
         <v>Virtual</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A28" t="str">
         <f>'for-README'!F30</f>
         <v>Lynn Collier</v>
@@ -1939,7 +1939,7 @@
         <v>Virtual</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A29" t="str">
         <f>'for-README'!F31</f>
         <v>Peter Comeau</v>
@@ -1957,7 +1957,7 @@
         <v>In person</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A30" t="str">
         <f>'for-README'!F32</f>
         <v>Tania Davignon-Burton</v>
@@ -1975,7 +1975,7 @@
         <v>Virtual</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A31" t="str">
         <f>'for-README'!F33</f>
         <v>Nell den Heyer</v>
@@ -1993,7 +1993,7 @@
         <v>Virtual</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A32" t="str">
         <f>'for-README'!F34</f>
         <v>Danni Harper</v>
@@ -2011,7 +2011,7 @@
         <v>Virtual</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33" t="str">
         <f>'for-README'!F35</f>
         <v>Kelly Kraska</v>
@@ -2029,7 +2029,7 @@
         <v>In person</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34" t="str">
         <f>'for-README'!F36</f>
         <v>Lingbo Lee</v>
@@ -2047,7 +2047,7 @@
         <v>Virtual</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A35" t="str">
         <f>'for-README'!F37</f>
         <v>Ellen MacEachern</v>
@@ -2065,7 +2065,7 @@
         <v>In person</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A36" t="str">
         <f>'for-README'!F38</f>
         <v>Liz Miller</v>
@@ -2083,7 +2083,7 @@
         <v>In person</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A37" t="str">
         <f>'for-README'!F39</f>
         <v>George Nau</v>
@@ -2101,7 +2101,7 @@
         <v>Virtual</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A38" t="str">
         <f>'for-README'!F40</f>
         <v>Gregory Puncher</v>
@@ -2119,7 +2119,7 @@
         <v>In person</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A39" t="str">
         <f>'for-README'!F41</f>
         <v>Catriona Regnier-McKellar</v>
@@ -2137,7 +2137,7 @@
         <v>Virtual</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A40" t="str">
         <f>'for-README'!F43</f>
         <v>Aaron Adamack</v>
@@ -2155,7 +2155,7 @@
         <v>Virtual</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A41" t="str">
         <f>'for-README'!F44</f>
         <v>Kelly Antaya</v>
@@ -2173,7 +2173,7 @@
         <v>Virtual</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A42" t="str">
         <f>'for-README'!F45</f>
         <v>Dwight Drover</v>
@@ -2191,7 +2191,7 @@
         <v>Virtual</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A43" t="str">
         <f>'for-README'!F46</f>
         <v>Gillian Forbes</v>
@@ -2209,7 +2209,7 @@
         <v>In person</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A44" t="str">
         <f>'for-README'!F47</f>
         <v>Victoria Healey</v>
@@ -2227,7 +2227,7 @@
         <v>Virtual</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A45" t="str">
         <f>'for-README'!F48</f>
         <v>Marc Legresley</v>
@@ -2245,7 +2245,7 @@
         <v>Virtual</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A46" t="str">
         <f>'for-README'!F49</f>
         <v>Andrea Perreault</v>
@@ -2263,7 +2263,7 @@
         <v>Virtual</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A47" t="str">
         <f>'for-README'!F50</f>
         <v>Hannah Polaczek</v>
@@ -2281,7 +2281,7 @@
         <v>Virtual</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A48" t="str">
         <f>'for-README'!F51</f>
         <v>Kierstyn Rideout</v>
@@ -2299,7 +2299,7 @@
         <v>In person</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A49" t="str">
         <f>'for-README'!F52</f>
         <v>Meredith Schofield</v>
@@ -2317,7 +2317,7 @@
         <v>In person</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A50" t="str">
         <f>'for-README'!F53</f>
         <v>Jaime Thomson</v>
@@ -2335,7 +2335,7 @@
         <v>In person</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A51" t="str">
         <f>'for-README'!F54</f>
         <v>Barbara Campbell</v>
@@ -2353,7 +2353,7 @@
         <v>Virtual</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A52" t="str">
         <f>'for-README'!F55</f>
         <v>Karalea Cantera</v>
@@ -2371,7 +2371,7 @@
         <v>Virtual</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A53" t="str">
         <f>'for-README'!F56</f>
         <v>Chelsea Cooke</v>
@@ -2389,7 +2389,7 @@
         <v>Virtual</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A54" t="str">
         <f>'for-README'!F57</f>
         <v>Robyn Forrest</v>
@@ -2407,7 +2407,7 @@
         <v>Virtual</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A55" t="str">
         <f>'for-README'!F58</f>
         <v>Sarah Hawkshaw</v>
@@ -2425,7 +2425,7 @@
         <v>Virtual</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A56" t="str">
         <f>'for-README'!F59</f>
         <v>Erin Herder</v>
@@ -2443,7 +2443,7 @@
         <v>Virtual</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A57" t="str">
         <f>'for-README'!F60</f>
         <v>Kendra Holt</v>
@@ -2461,7 +2461,7 @@
         <v>Virtual</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A58" t="str">
         <f>'for-README'!F61</f>
         <v>Yeongha Jung</v>
@@ -2479,7 +2479,7 @@
         <v>Virtual</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A59" t="str">
         <f>'for-README'!F62</f>
         <v>Madeline Lavery</v>
@@ -2497,7 +2497,7 @@
         <v>Virtual</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A60" t="str">
         <f>'for-README'!F63</f>
         <v>Kiana Matwichuk</v>
@@ -2515,7 +2515,7 @@
         <v>Virtual</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A61" t="str">
         <f>'for-README'!F64</f>
         <v>Mackenzie Mazur</v>
@@ -2533,7 +2533,7 @@
         <v>Virtual</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A62" t="str">
         <f>'for-README'!F65</f>
         <v>Judy McArthur</v>
@@ -2551,7 +2551,7 @@
         <v>Virtual</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A63" t="str">
         <f>'for-README'!F66</f>
         <v>Audrey Ty</v>
@@ -2569,7 +2569,7 @@
         <v>Virtual</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A64" t="str">
         <f>'for-README'!F67</f>
         <v>Stephen Wischniowski</v>
@@ -2587,7 +2587,7 @@
         <v>Virtual</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A65" t="str">
         <f>'for-README'!F68</f>
         <v>Emily Yungwirth</v>
@@ -2605,7 +2605,7 @@
         <v>Virtual</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A66" t="str">
         <f>'for-README'!F69</f>
         <v>Mathieu Desgagnés</v>
@@ -2623,7 +2623,7 @@
         <v>Virtual</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A67" t="str">
         <f>'for-README'!F70</f>
         <v>Hélène Dionne</v>
@@ -2641,7 +2641,7 @@
         <v>In person</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A68" t="str">
         <f>'for-README'!F71</f>
         <v>Kim Emond</v>
@@ -2659,7 +2659,7 @@
         <v>In person</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A69" t="str">
         <f>'for-README'!F72</f>
         <v>Nicolas Le Corre</v>
@@ -2677,7 +2677,7 @@
         <v>Virtual</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A70" t="str">
         <f>'for-README'!F73</f>
         <v>Andrew Smith</v>
@@ -2743,16 +2743,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FE87253-3AFE-489E-871D-A05432044822}">
-  <dimension ref="A1:Q74"/>
+  <dimension ref="A1:Q73"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="17" max="17" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A1" t="str">
         <f ca="1">CONCATENATE("List of the ", N1, " participants as of ", TEXT(TODAY(),"yyyy-mm-dd"), " (",L2, " in person and ", L1, " virtual)")</f>
         <v>List of the 70 participants as of 2023-01-30 (28 in person and 42 virtual)</v>
@@ -2770,7 +2770,7 @@
       </c>
       <c r="Q1" s="10"/>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>191</v>
       </c>
@@ -2806,7 +2806,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>191</v>
       </c>
@@ -2835,7 +2835,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>191</v>
       </c>
@@ -2883,7 +2883,7 @@
         <v>Alsip, Laura</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>191</v>
       </c>
@@ -2931,7 +2931,7 @@
         <v>Burke, Lauren (Lauren.Burke@dfo-mpo.gc.ca)</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>191</v>
       </c>
@@ -2979,7 +2979,7 @@
         <v>Hedges, Kevin</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>191</v>
       </c>
@@ -3027,7 +3027,7 @@
         <v>Legge, Michael</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>191</v>
       </c>
@@ -3075,7 +3075,7 @@
         <v>Loewen, Tracey</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>191</v>
       </c>
@@ -3123,7 +3123,7 @@
         <v>Malley, Brendan K</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>191</v>
       </c>
@@ -3171,7 +3171,7 @@
         <v>Vandenbyllaardt, Lenore</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>191</v>
       </c>
@@ -3219,7 +3219,7 @@
         <v>Wastle, Rick</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>191</v>
       </c>
@@ -3267,7 +3267,7 @@
         <v>Zhu, Xinhua</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>191</v>
       </c>
@@ -3315,7 +3315,7 @@
         <v>Burbank, Jacob</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>191</v>
       </c>
@@ -3363,7 +3363,7 @@
         <v>Daigle, Abby</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>191</v>
       </c>
@@ -3411,7 +3411,7 @@
         <v>Darcy, Andrew</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>191</v>
       </c>
@@ -3459,7 +3459,7 @@
         <v xml:space="preserve">Forest, Isabelle </v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>191</v>
       </c>
@@ -3507,7 +3507,7 @@
         <v xml:space="preserve">Horsman, Matthew </v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>191</v>
       </c>
@@ -3555,7 +3555,7 @@
         <v>Hudson, Samantha</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>191</v>
       </c>
@@ -3603,7 +3603,7 @@
         <v>MacFarlane, Colin</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>191</v>
       </c>
@@ -3651,7 +3651,7 @@
         <v>McGee, Kelsey</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>191</v>
       </c>
@@ -3699,7 +3699,7 @@
         <v>Morrill, Kirby</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>191</v>
       </c>
@@ -3747,7 +3747,7 @@
         <v>Ricard, Daniel</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>191</v>
       </c>
@@ -3795,7 +3795,7 @@
         <v>Robertson, Karen</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>191</v>
       </c>
@@ -3843,7 +3843,7 @@
         <v xml:space="preserve">Robichaud, Sylvie </v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>191</v>
       </c>
@@ -3891,7 +3891,7 @@
         <v>Rolland, Nicolas</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>191</v>
       </c>
@@ -3939,7 +3939,7 @@
         <v xml:space="preserve">Sutton, Jolene </v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>191</v>
       </c>
@@ -3987,7 +3987,7 @@
         <v xml:space="preserve">Sylvain, François-Étienne </v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>191</v>
       </c>
@@ -4035,7 +4035,7 @@
         <v>Underhill, Kari</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>191</v>
       </c>
@@ -4083,7 +4083,7 @@
         <v>Billard, Mark</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>191</v>
       </c>
@@ -4131,7 +4131,7 @@
         <v>Collier, Lynn</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>191</v>
       </c>
@@ -4179,7 +4179,7 @@
         <v>Comeau, Peter</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>191</v>
       </c>
@@ -4227,7 +4227,7 @@
         <v>Davignon-Burton, Tania</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>191</v>
       </c>
@@ -4275,7 +4275,7 @@
         <v>den Heyer, Nell</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>191</v>
       </c>
@@ -4323,7 +4323,7 @@
         <v>Harper, Danni</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>191</v>
       </c>
@@ -4371,7 +4371,7 @@
         <v>Kraska, Kelly</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>191</v>
       </c>
@@ -4419,7 +4419,7 @@
         <v>Lee, Lingbo</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>191</v>
       </c>
@@ -4467,7 +4467,7 @@
         <v>MacEachern, Ellen</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>191</v>
       </c>
@@ -4515,7 +4515,7 @@
         <v>Miller, Liz</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>191</v>
       </c>
@@ -4563,7 +4563,7 @@
         <v>Nau, George</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>191</v>
       </c>
@@ -4611,7 +4611,7 @@
         <v>Puncher, Gregory</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>191</v>
       </c>
@@ -4659,7 +4659,7 @@
         <v>Regnier-McKellar, Catriona</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>191</v>
       </c>
@@ -4707,7 +4707,7 @@
         <v>Way-Nee, Emily</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>191</v>
       </c>
@@ -4755,7 +4755,7 @@
         <v>Adamack, Aaron</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>191</v>
       </c>
@@ -4803,7 +4803,7 @@
         <v>Antaya, Kelly</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>191</v>
       </c>
@@ -4851,7 +4851,7 @@
         <v>Drover, Dwight</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>191</v>
       </c>
@@ -4899,7 +4899,7 @@
         <v>Forbes, Gillian</v>
       </c>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>191</v>
       </c>
@@ -4947,7 +4947,7 @@
         <v>Healey, Victoria</v>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>191</v>
       </c>
@@ -4995,7 +4995,7 @@
         <v>Legresley, Marc</v>
       </c>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>191</v>
       </c>
@@ -5043,7 +5043,7 @@
         <v>Perreault, Andrea</v>
       </c>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>191</v>
       </c>
@@ -5091,7 +5091,7 @@
         <v>Polaczek, Hannah</v>
       </c>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>191</v>
       </c>
@@ -5139,7 +5139,7 @@
         <v>Rideout, Kierstyn</v>
       </c>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>191</v>
       </c>
@@ -5187,7 +5187,7 @@
         <v>Schofield, Meredith</v>
       </c>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>191</v>
       </c>
@@ -5235,7 +5235,7 @@
         <v xml:space="preserve">Thomson, Jaime </v>
       </c>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>191</v>
       </c>
@@ -5283,7 +5283,7 @@
         <v>Campbell, Barbara</v>
       </c>
     </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>191</v>
       </c>
@@ -5331,7 +5331,7 @@
         <v>Cantera, Karalea</v>
       </c>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>191</v>
       </c>
@@ -5379,7 +5379,7 @@
         <v>Cooke, Chelsea</v>
       </c>
     </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>191</v>
       </c>
@@ -5427,7 +5427,7 @@
         <v xml:space="preserve">Forrest, Robyn </v>
       </c>
     </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>191</v>
       </c>
@@ -5475,7 +5475,7 @@
         <v>Hawkshaw, Sarah</v>
       </c>
     </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>191</v>
       </c>
@@ -5523,7 +5523,7 @@
         <v>Herder, Erin</v>
       </c>
     </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>191</v>
       </c>
@@ -5571,7 +5571,7 @@
         <v>Holt, Kendra</v>
       </c>
     </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>191</v>
       </c>
@@ -5619,7 +5619,7 @@
         <v>Jung, Yeongha</v>
       </c>
     </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>191</v>
       </c>
@@ -5667,7 +5667,7 @@
         <v>Lavery, Madeline</v>
       </c>
     </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>191</v>
       </c>
@@ -5715,7 +5715,7 @@
         <v>Matwichuk, Kiana</v>
       </c>
     </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>191</v>
       </c>
@@ -5763,7 +5763,7 @@
         <v>Mazur, Mackenzie</v>
       </c>
     </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>191</v>
       </c>
@@ -5811,7 +5811,7 @@
         <v xml:space="preserve">McArthur, Judy </v>
       </c>
     </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>191</v>
       </c>
@@ -5859,7 +5859,7 @@
         <v>Ty, Audrey</v>
       </c>
     </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>191</v>
       </c>
@@ -5907,7 +5907,7 @@
         <v>Wischniowski, Stephen</v>
       </c>
     </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>191</v>
       </c>
@@ -5955,7 +5955,7 @@
         <v xml:space="preserve">Yungwirth, Emily </v>
       </c>
     </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>191</v>
       </c>
@@ -6003,7 +6003,7 @@
         <v xml:space="preserve">Desgagnés, Mathieu </v>
       </c>
     </row>
-    <row r="70" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>191</v>
       </c>
@@ -6051,7 +6051,7 @@
         <v>Dionne, Hélène</v>
       </c>
     </row>
-    <row r="71" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>191</v>
       </c>
@@ -6099,7 +6099,7 @@
         <v>Emond, Kim</v>
       </c>
     </row>
-    <row r="72" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>191</v>
       </c>
@@ -6147,7 +6147,7 @@
         <v>LeCorre, Nicolas</v>
       </c>
     </row>
-    <row r="73" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>191</v>
       </c>
@@ -6193,17 +6193,6 @@
       <c r="M73" t="str">
         <f>'outlook-responses'!E83</f>
         <v>Smith, Andrew</v>
-      </c>
-    </row>
-    <row r="74" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
-        <v>191</v>
-      </c>
-      <c r="B74">
-        <v>71</v>
-      </c>
-      <c r="C74" t="s">
-        <v>191</v>
       </c>
     </row>
   </sheetData>
@@ -6215,16 +6204,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7648514F-C50B-429E-8CE0-7F6A61E6FA38}">
   <dimension ref="A1:O83"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="5" max="5" width="19.42578125" customWidth="1"/>
-    <col min="6" max="6" width="12.5703125" customWidth="1"/>
-    <col min="8" max="8" width="17.42578125" customWidth="1"/>
+    <col min="5" max="5" width="19.453125" customWidth="1"/>
+    <col min="6" max="6" width="12.54296875" customWidth="1"/>
+    <col min="8" max="8" width="17.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B1" s="1" t="s">
         <v>125</v>
       </c>
@@ -6233,7 +6222,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
         <v>140</v>
       </c>
@@ -6242,7 +6231,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
         <v>173</v>
       </c>
@@ -6251,7 +6240,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
       <c r="C6" t="s">
         <v>187</v>
       </c>
@@ -6268,7 +6257,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
         <v>188</v>
       </c>
@@ -6277,7 +6266,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>197</v>
       </c>
@@ -6312,7 +6301,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>197</v>
       </c>
@@ -6343,7 +6332,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>197</v>
       </c>
@@ -6374,7 +6363,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>197</v>
       </c>
@@ -6405,7 +6394,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>197</v>
       </c>
@@ -6436,7 +6425,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>197</v>
       </c>
@@ -6467,7 +6456,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>197</v>
       </c>
@@ -6498,7 +6487,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>197</v>
       </c>
@@ -6529,7 +6518,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>197</v>
       </c>
@@ -6560,7 +6549,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>192</v>
       </c>
@@ -6596,7 +6585,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>192</v>
       </c>
@@ -6628,7 +6617,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>192</v>
       </c>
@@ -6660,7 +6649,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>192</v>
       </c>
@@ -6692,7 +6681,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>192</v>
       </c>
@@ -6724,7 +6713,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>192</v>
       </c>
@@ -6756,7 +6745,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>192</v>
       </c>
@@ -6788,7 +6777,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>192</v>
       </c>
@@ -6820,7 +6809,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>192</v>
       </c>
@@ -6852,7 +6841,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>192</v>
       </c>
@@ -6884,7 +6873,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>192</v>
       </c>
@@ -6916,7 +6905,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>192</v>
       </c>
@@ -6948,7 +6937,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>192</v>
       </c>
@@ -6980,7 +6969,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>192</v>
       </c>
@@ -7012,7 +7001,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>192</v>
       </c>
@@ -7044,7 +7033,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>192</v>
       </c>
@@ -7076,7 +7065,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>194</v>
       </c>
@@ -7111,7 +7100,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>194</v>
       </c>
@@ -7142,7 +7131,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>194</v>
       </c>
@@ -7173,7 +7162,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>194</v>
       </c>
@@ -7204,7 +7193,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>194</v>
       </c>
@@ -7235,7 +7224,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>194</v>
       </c>
@@ -7266,7 +7255,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>194</v>
       </c>
@@ -7297,7 +7286,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>194</v>
       </c>
@@ -7328,7 +7317,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>194</v>
       </c>
@@ -7359,7 +7348,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>194</v>
       </c>
@@ -7390,7 +7379,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>194</v>
       </c>
@@ -7421,7 +7410,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>194</v>
       </c>
@@ -7452,7 +7441,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>194</v>
       </c>
@@ -7483,7 +7472,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>194</v>
       </c>
@@ -7514,7 +7503,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>195</v>
       </c>
@@ -7549,7 +7538,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>195</v>
       </c>
@@ -7580,7 +7569,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>195</v>
       </c>
@@ -7611,7 +7600,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>195</v>
       </c>
@@ -7642,7 +7631,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>195</v>
       </c>
@@ -7673,7 +7662,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>195</v>
       </c>
@@ -7704,7 +7693,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>195</v>
       </c>
@@ -7735,7 +7724,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>195</v>
       </c>
@@ -7766,7 +7755,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>195</v>
       </c>
@@ -7795,7 +7784,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>195</v>
       </c>
@@ -7826,7 +7815,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>195</v>
       </c>
@@ -7857,7 +7846,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>193</v>
       </c>
@@ -7892,7 +7881,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>193</v>
       </c>
@@ -7923,7 +7912,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>193</v>
       </c>
@@ -7953,7 +7942,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>193</v>
       </c>
@@ -7984,7 +7973,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>193</v>
       </c>
@@ -8015,7 +8004,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>193</v>
       </c>
@@ -8046,7 +8035,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>193</v>
       </c>
@@ -8077,7 +8066,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>193</v>
       </c>
@@ -8108,7 +8097,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>193</v>
       </c>
@@ -8139,7 +8128,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>193</v>
       </c>
@@ -8170,7 +8159,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>193</v>
       </c>
@@ -8201,7 +8190,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>193</v>
       </c>
@@ -8232,7 +8221,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>193</v>
       </c>
@@ -8263,7 +8252,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>193</v>
       </c>
@@ -8294,7 +8283,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>193</v>
       </c>
@@ -8325,7 +8314,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>196</v>
       </c>
@@ -8360,7 +8349,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>196</v>
       </c>
@@ -8391,7 +8380,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>196</v>
       </c>
@@ -8422,7 +8411,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>196</v>
       </c>
@@ -8453,7 +8442,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
         <v>196</v>
       </c>
@@ -8499,12 +8488,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="37.42578125" customWidth="1"/>
+    <col min="1" max="1" width="37.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>135</v>
       </c>
@@ -8512,7 +8501,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="str">
         <f>IF('list-pre-google-forms'!E10=1,'list-pre-google-forms'!C10,"")</f>
         <v>Nicolas.Rolland@dfo-mpo.gc.ca</v>
@@ -8522,7 +8511,7 @@
         <v>Nicolas.Rolland@dfo-mpo.gc.ca</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="str">
         <f>IF('list-pre-google-forms'!E11=1,'list-pre-google-forms'!C11,"")</f>
         <v>Francois-Etienne.Sylvain@dfo-mpo.gc.ca</v>
@@ -8532,7 +8521,7 @@
         <v>Francois-Etienne.Sylvain@dfo-mpo.gc.ca</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="str">
         <f>IF('list-pre-google-forms'!E12=1,'list-pre-google-forms'!C12,"")</f>
         <v>Jolene.Sutton@dfo-mpo.gc.ca</v>
@@ -8542,7 +8531,7 @@
         <v>Jolene.Sutton@dfo-mpo.gc.ca</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="str">
         <f>IF('list-pre-google-forms'!E13=1,'list-pre-google-forms'!C13,"")</f>
         <v>Suncica.Avlijas@dfo-mpo.gc.ca</v>
@@ -8552,7 +8541,7 @@
         <v>Suncica.Avlijas@dfo-mpo.gc.ca</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="str">
         <f>IF('list-pre-google-forms'!E14=1,'list-pre-google-forms'!C14,"")</f>
         <v/>
@@ -8562,7 +8551,7 @@
         <v/>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="str">
         <f>IF('list-pre-google-forms'!E15=1,'list-pre-google-forms'!C15,"")</f>
         <v>Karen.Robertson@dfo-mpo.gc.ca</v>
@@ -8572,7 +8561,7 @@
         <v>Karen.Robertson@dfo-mpo.gc.ca</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="str">
         <f>IF('list-pre-google-forms'!E16=1,'list-pre-google-forms'!C16,"")</f>
         <v>Joeleen.Savoie@dfo-mpo.gc.ca</v>
@@ -8582,7 +8571,7 @@
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="str">
         <f>IF('list-pre-google-forms'!E17=1,'list-pre-google-forms'!C17,"")</f>
         <v>Marie-France.Robichaud@dfo-mpo.gc.ca</v>
@@ -8592,7 +8581,7 @@
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="str">
         <f>IF('list-pre-google-forms'!E18=1,'list-pre-google-forms'!C18,"")</f>
         <v>Sylvie.Robichaud@dfo-mpo.gc.ca</v>
@@ -8602,7 +8591,7 @@
         <v>Sylvie.Robichaud@dfo-mpo.gc.ca</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="str">
         <f>IF('list-pre-google-forms'!E19=1,'list-pre-google-forms'!C19,"")</f>
         <v>Andrew.Darcy@dfo-mpo.gc.ca</v>
@@ -8612,7 +8601,7 @@
         <v>Andrew.Darcy@dfo-mpo.gc.ca</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="str">
         <f>IF('list-pre-google-forms'!E20=1,'list-pre-google-forms'!C20,"")</f>
         <v>abby.daigle@dfo-mpo.gc.ca</v>
@@ -8622,7 +8611,7 @@
         <v>abby.daigle@dfo-mpo.gc.ca</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="str">
         <f>IF('list-pre-google-forms'!E21=1,'list-pre-google-forms'!C21,"")</f>
         <v>matthew.horsman@dfo-mpo.gc.ca</v>
@@ -8632,7 +8621,7 @@
         <v>matthew.horsman@dfo-mpo.gc.ca</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" t="str">
         <f>IF('list-pre-google-forms'!E22=1,'list-pre-google-forms'!C22,"")</f>
         <v>kirby.morrill@dfo-mpo.gc.ca</v>
@@ -8642,7 +8631,7 @@
         <v>kirby.morrill@dfo-mpo.gc.ca</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" t="str">
         <f>IF('list-pre-google-forms'!E23=1,'list-pre-google-forms'!C23,"")</f>
         <v/>
@@ -8652,7 +8641,7 @@
         <v/>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" t="str">
         <f>IF('list-pre-google-forms'!E24=1,'list-pre-google-forms'!C24,"")</f>
         <v/>
@@ -8662,7 +8651,7 @@
         <v/>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" t="str">
         <f>IF('list-pre-google-forms'!E25=1,'list-pre-google-forms'!C25,"")</f>
         <v>Peter.Comeau@dfo-mpo.gc.ca</v>
@@ -8672,7 +8661,7 @@
         <v>Peter.Comeau@dfo-mpo.gc.ca</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" t="str">
         <f>IF('list-pre-google-forms'!E26=1,'list-pre-google-forms'!C26,"")</f>
         <v>Nell.denHeyer@dfo-mpo.gc.ca</v>
@@ -8682,7 +8671,7 @@
         <v>Nell.denHeyer@dfo-mpo.gc.ca</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" t="str">
         <f>IF('list-pre-google-forms'!E27=1,'list-pre-google-forms'!C27,"")</f>
         <v>Quinn.McCurdy@dfo-mpo.gc.ca</v>
@@ -8692,7 +8681,7 @@
         <v>Quinn.McCurdy@dfo-mpo.gc.ca</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" t="str">
         <f>IF('list-pre-google-forms'!E28=1,'list-pre-google-forms'!C28,"")</f>
         <v>Dheeraj.Busawon@dfo-mpo.gc.ca</v>
@@ -8702,7 +8691,7 @@
         <v/>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" t="str">
         <f>IF('list-pre-google-forms'!E29=1,'list-pre-google-forms'!C29,"")</f>
         <v>George.Nau@dfo-mpo.gc.ca</v>
@@ -8712,7 +8701,7 @@
         <v>George.Nau@dfo-mpo.gc.ca</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" t="str">
         <f>IF('list-pre-google-forms'!E30=1,'list-pre-google-forms'!C30,"")</f>
         <v>Mark.Billard@dfo-mpo.gc.ca</v>
@@ -8722,7 +8711,7 @@
         <v>Mark.Billard@dfo-mpo.gc.ca</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" t="str">
         <f>IF('list-pre-google-forms'!E31=1,'list-pre-google-forms'!C31,"")</f>
         <v>lynn.collier@dfo-mpo.gc.ca</v>
@@ -8732,7 +8721,7 @@
         <v>lynn.collier@dfo-mpo.gc.ca</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" t="str">
         <f>IF('list-pre-google-forms'!E32=1,'list-pre-google-forms'!C32,"")</f>
         <v>Kelly.Kraska@dfo-mpo.gc.ca</v>
@@ -8742,7 +8731,7 @@
         <v/>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" t="str">
         <f>IF('list-pre-google-forms'!E33=1,'list-pre-google-forms'!C33,"")</f>
         <v>Tania.Davignon-Burton@dfo-mpo.gc.ca</v>
@@ -8752,7 +8741,7 @@
         <v>Tania.Davignon-Burton@dfo-mpo.gc.ca</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" t="str">
         <f>IF('list-pre-google-forms'!E34=1,'list-pre-google-forms'!C34,"")</f>
         <v>Gregory.Puncher@dfo-mpo.gc.ca</v>
@@ -8762,7 +8751,7 @@
         <v/>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" t="str">
         <f>IF('list-pre-google-forms'!E35=1,'list-pre-google-forms'!C35,"")</f>
         <v>Catriona.Regnier-McKellar@dfo-mpo.gc.ca</v>
@@ -8772,7 +8761,7 @@
         <v/>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30" t="str">
         <f>IF('list-pre-google-forms'!E36=1,'list-pre-google-forms'!C36,"")</f>
         <v/>
@@ -8782,7 +8771,7 @@
         <v/>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31" t="str">
         <f>IF('list-pre-google-forms'!E37=1,'list-pre-google-forms'!C37,"")</f>
         <v/>
@@ -8792,7 +8781,7 @@
         <v/>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32" t="str">
         <f>IF('list-pre-google-forms'!E38=1,'list-pre-google-forms'!C38,"")</f>
         <v>Kim.Emond@dfo-mpo.gc.ca</v>
@@ -8802,7 +8791,7 @@
         <v>Kim.Emond@dfo-mpo.gc.ca</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33" t="str">
         <f>IF('list-pre-google-forms'!E39=1,'list-pre-google-forms'!C39,"")</f>
         <v>Nicolas.LeCorre@dfo-mpo.gc.ca</v>
@@ -8812,7 +8801,7 @@
         <v>Nicolas.LeCorre@dfo-mpo.gc.ca</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34" t="str">
         <f>IF('list-pre-google-forms'!E40=1,'list-pre-google-forms'!C40,"")</f>
         <v>andrew.smith4@dfo-mpo.gc.ca</v>
@@ -8822,7 +8811,7 @@
         <v>andrew.smith4@dfo-mpo.gc.ca</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35" t="str">
         <f>IF('list-pre-google-forms'!E41=1,'list-pre-google-forms'!C41,"")</f>
         <v>Renald.Belley@dfo-mpo.gc.ca</v>
@@ -8832,7 +8821,7 @@
         <v>Renald.Belley@dfo-mpo.gc.ca</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A36" t="str">
         <f>IF('list-pre-google-forms'!E42=1,'list-pre-google-forms'!C42,"")</f>
         <v>Mathieu.Desgagnes@dfo-mpo.gc.ca</v>
@@ -8842,7 +8831,7 @@
         <v>Mathieu.Desgagnes@dfo-mpo.gc.ca</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A37" t="str">
         <f>IF('list-pre-google-forms'!E43=1,'list-pre-google-forms'!C43,"")</f>
         <v>helene.dionne@dfo-mpo.gc.ca</v>
@@ -8852,7 +8841,7 @@
         <v>helene.dionne@dfo-mpo.gc.ca</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A38" t="str">
         <f>IF('list-pre-google-forms'!E44=1,'list-pre-google-forms'!C44,"")</f>
         <v/>
@@ -8862,7 +8851,7 @@
         <v/>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A39" t="str">
         <f>IF('list-pre-google-forms'!E45=1,'list-pre-google-forms'!C45,"")</f>
         <v/>
@@ -8872,7 +8861,7 @@
         <v/>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A40" t="str">
         <f>IF('list-pre-google-forms'!E46=1,'list-pre-google-forms'!C46,"")</f>
         <v>Laura.Alsip@dfo-mpo.gc.ca</v>
@@ -8882,7 +8871,7 @@
         <v>Laura.Alsip@dfo-mpo.gc.ca</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A41" t="str">
         <f>IF('list-pre-google-forms'!E47=1,'list-pre-google-forms'!C47,"")</f>
         <v>Wojciech.Walkusz@dfo-mpo.gc.ca</v>
@@ -8892,7 +8881,7 @@
         <v/>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A42" t="str">
         <f>IF('list-pre-google-forms'!E48=1,'list-pre-google-forms'!C48,"")</f>
         <v>Lauren.Wiens@dfo-mpo.gc.ca</v>
@@ -8902,7 +8891,7 @@
         <v>Lauren.Wiens@dfo-mpo.gc.ca</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A43" t="str">
         <f>IF('list-pre-google-forms'!E49=1,'list-pre-google-forms'!C49,"")</f>
         <v/>
@@ -8912,7 +8901,7 @@
         <v/>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A44" t="str">
         <f>IF('list-pre-google-forms'!E50=1,'list-pre-google-forms'!C50,"")</f>
         <v/>
@@ -8922,7 +8911,7 @@
         <v/>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A45" t="str">
         <f>IF('list-pre-google-forms'!E51=1,'list-pre-google-forms'!C51,"")</f>
         <v>Tracey.Loewen@dfo-mpo.gc.ca</v>
@@ -8932,7 +8921,7 @@
         <v>Tracey.Loewen@dfo-mpo.gc.ca</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A46" t="str">
         <f>IF('list-pre-google-forms'!E52=1,'list-pre-google-forms'!C52,"")</f>
         <v>Brendan.Malley@dfo-mpo.gc.ca</v>
@@ -8942,7 +8931,7 @@
         <v/>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A47" t="str">
         <f>IF('list-pre-google-forms'!E53=1,'list-pre-google-forms'!C53,"")</f>
         <v/>
@@ -8952,7 +8941,7 @@
         <v/>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A48" t="str">
         <f>IF('list-pre-google-forms'!E54=1,'list-pre-google-forms'!C54,"")</f>
         <v/>
@@ -8962,7 +8951,7 @@
         <v/>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A49" t="str">
         <f>IF('list-pre-google-forms'!E55=1,'list-pre-google-forms'!C55,"")</f>
         <v>Sarah.Hawkshaw@dfo-mpo.gc.ca</v>
@@ -8972,7 +8961,7 @@
         <v>Sarah.Hawkshaw@dfo-mpo.gc.ca</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A50" t="str">
         <f>IF('list-pre-google-forms'!E56=1,'list-pre-google-forms'!C56,"")</f>
         <v>Madeline.Lavery@dfo-mpo.gc.ca</v>
@@ -8982,7 +8971,7 @@
         <v>Madeline.Lavery@dfo-mpo.gc.ca</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A51" t="str">
         <f>IF('list-pre-google-forms'!E57=1,'list-pre-google-forms'!C57,"")</f>
         <v>Emily.Yungwirth@dfo-mpo.gc.ca</v>
@@ -8992,7 +8981,7 @@
         <v>Emily.Yungwirth@dfo-mpo.gc.ca</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A52" t="str">
         <f>IF('list-pre-google-forms'!E58=1,'list-pre-google-forms'!C58,"")</f>
         <v>dana.haggarty@dfo-mpo.gc.ca</v>
@@ -9002,7 +8991,7 @@
         <v>dana.haggarty@dfo-mpo.gc.ca</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A53" t="str">
         <f>IF('list-pre-google-forms'!E59=1,'list-pre-google-forms'!C59,"")</f>
         <v>Kendra.Holt@dfo-mpo.gc.ca</v>
@@ -9012,7 +9001,7 @@
         <v>Kendra.Holt@dfo-mpo.gc.ca</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A54" t="str">
         <f>IF('list-pre-google-forms'!E60=1,'list-pre-google-forms'!C60,"")</f>
         <v>Matthew.Siegle@dfo-mpo.gc.ca</v>
@@ -9022,7 +9011,7 @@
         <v/>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A55" t="str">
         <f>IF('list-pre-google-forms'!E61=1,'list-pre-google-forms'!C61,"")</f>
         <v>Mackenzie.Mazur@dfo-mpo.gc.ca</v>
@@ -9032,7 +9021,7 @@
         <v/>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A56" t="str">
         <f>IF('list-pre-google-forms'!E62=1,'list-pre-google-forms'!C62,"")</f>
         <v>Karalea.Cantera@dfo-mpo.gc.ca</v>
@@ -9042,7 +9031,7 @@
         <v/>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A57" t="str">
         <f>IF('list-pre-google-forms'!E63=1,'list-pre-google-forms'!C63,"")</f>
         <v>Kiana.Matwichuk@dfo-mpo.gc.ca</v>
@@ -9052,7 +9041,7 @@
         <v/>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A58" t="str">
         <f>IF('list-pre-google-forms'!E64=1,'list-pre-google-forms'!C64,"")</f>
         <v>Erin.Herder@dfo-mpo.gc.ca</v>
@@ -9062,7 +9051,7 @@
         <v>Erin.Herder@dfo-mpo.gc.ca</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A59" t="str">
         <f>IF('list-pre-google-forms'!E65=1,'list-pre-google-forms'!C65,"")</f>
         <v>Robyn.Forrest@dfo-mpo.gc.ca</v>
@@ -9072,7 +9061,7 @@
         <v>Robyn.Forrest@dfo-mpo.gc.ca</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A60" t="str">
         <f>IF('list-pre-google-forms'!E66=1,'list-pre-google-forms'!C66,"")</f>
         <v>yeongha.jung@dfo-mpo.gc.ca</v>
@@ -9082,7 +9071,7 @@
         <v>yeongha.jung@dfo-mpo.gc.ca</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A61" t="str">
         <f>IF('list-pre-google-forms'!E67=1,'list-pre-google-forms'!C67,"")</f>
         <v>barbara.campbell@dfo-mpo.gc.ca</v>
@@ -9092,7 +9081,7 @@
         <v>barbara.campbell@dfo-mpo.gc.ca</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A62" t="str">
         <f>IF('list-pre-google-forms'!E68=1,'list-pre-google-forms'!C68,"")</f>
         <v>stephen.wischniowski@dfo-mpo.gc.ca</v>
@@ -9102,7 +9091,7 @@
         <v/>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A63" t="str">
         <f>IF('list-pre-google-forms'!E69=1,'list-pre-google-forms'!C69,"")</f>
         <v/>
@@ -9112,7 +9101,7 @@
         <v/>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A64" t="str">
         <f>IF('list-pre-google-forms'!E70=1,'list-pre-google-forms'!C70,"")</f>
         <v/>
@@ -9122,7 +9111,7 @@
         <v/>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A65" t="str">
         <f>IF('list-pre-google-forms'!E71=1,'list-pre-google-forms'!C71,"")</f>
         <v>Gillian.Forbes@dfo-mpo.gc.ca</v>
@@ -9132,7 +9121,7 @@
         <v/>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A66" t="str">
         <f>IF('list-pre-google-forms'!E72=1,'list-pre-google-forms'!C72,"")</f>
         <v>Divya.Varkey@dfo-mpo.gc.ca</v>
@@ -9142,7 +9131,7 @@
         <v/>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A67" t="str">
         <f>IF('list-pre-google-forms'!E73=1,'list-pre-google-forms'!C73,"")</f>
         <v>Aaron.Adamack@dfo-mpo.gc.ca</v>
@@ -9152,7 +9141,7 @@
         <v>Aaron.Adamack@dfo-mpo.gc.ca</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A68" t="str">
         <f>IF('list-pre-google-forms'!E74=1,'list-pre-google-forms'!C74,"")</f>
         <v>Meredith.Schofield@dfo-mpo.gc.ca</v>
@@ -9162,7 +9151,7 @@
         <v>Meredith.Schofield@dfo-mpo.gc.ca</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A69" t="str">
         <f>IF('list-pre-google-forms'!E75=1,'list-pre-google-forms'!C75,"")</f>
         <v>Andrea.Perreault@dfo-mpo.gc.ca</v>
@@ -9172,7 +9161,7 @@
         <v>Andrea.Perreault@dfo-mpo.gc.ca</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A70" t="str">
         <f>IF('list-pre-google-forms'!E76=1,'list-pre-google-forms'!C76,"")</f>
         <v>Laura.Wheeland@dfo-mpo.gc.ca</v>
@@ -9182,7 +9171,7 @@
         <v>Laura.Wheeland@dfo-mpo.gc.ca</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A71" t="str">
         <f>IF('list-pre-google-forms'!E77=1,'list-pre-google-forms'!C77,"")</f>
         <v/>
@@ -9192,7 +9181,7 @@
         <v/>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A72" t="str">
         <f>IF('list-pre-google-forms'!E78=1,'list-pre-google-forms'!C78,"")</f>
         <v/>
@@ -9202,7 +9191,7 @@
         <v/>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A73" t="str">
         <f>IF('list-pre-google-forms'!E79=1,'list-pre-google-forms'!C79,"")</f>
         <v/>
@@ -9212,7 +9201,7 @@
         <v/>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A74" t="str">
         <f>IF('list-pre-google-forms'!E80=1,'list-pre-google-forms'!C80,"")</f>
         <v/>
@@ -9222,7 +9211,7 @@
         <v/>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A75" t="str">
         <f>IF('list-pre-google-forms'!E81=1,'list-pre-google-forms'!C81,"")</f>
         <v/>
@@ -9232,7 +9221,7 @@
         <v/>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A76" t="str">
         <f>IF('list-pre-google-forms'!E82=1,'list-pre-google-forms'!C82,"")</f>
         <v/>
@@ -9242,7 +9231,7 @@
         <v/>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A77" t="str">
         <f>IF('list-pre-google-forms'!E83=1,'list-pre-google-forms'!C83,"")</f>
         <v/>
@@ -9252,7 +9241,7 @@
         <v/>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B78" t="str">
         <f>IF('list-pre-google-forms'!G88=1,'list-pre-google-forms'!C88,"")</f>
         <v/>
@@ -9271,26 +9260,26 @@
       <selection activeCell="E5" sqref="E5:F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="1"/>
-    <col min="2" max="2" width="24.7109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="37.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="25.140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="21.28515625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="12.140625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="11.42578125" customWidth="1"/>
+    <col min="1" max="1" width="9.1796875" style="1"/>
+    <col min="2" max="2" width="24.7265625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="37.7265625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="25.1796875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="21.26953125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="12.1796875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="11.453125" customWidth="1"/>
     <col min="8" max="8" width="11" customWidth="1"/>
-    <col min="9" max="9" width="10.85546875" customWidth="1"/>
-    <col min="10" max="10" width="10.5703125" customWidth="1"/>
+    <col min="9" max="9" width="10.81640625" customWidth="1"/>
+    <col min="10" max="10" width="10.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B2" s="1" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B3" s="7" t="s">
         <v>4</v>
       </c>
@@ -9302,7 +9291,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B4" s="7"/>
       <c r="E4" s="1" t="s">
         <v>124</v>
@@ -9312,7 +9301,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B5" s="7"/>
       <c r="E5" s="1" t="s">
         <v>125</v>
@@ -9322,11 +9311,11 @@
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B6" s="7"/>
       <c r="F6"/>
     </row>
-    <row r="7" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
         <v>1</v>
       </c>
@@ -9352,11 +9341,11 @@
         <v>121</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="E8"/>
       <c r="F8"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
         <v>5</v>
       </c>
@@ -9377,7 +9366,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" s="4"/>
       <c r="B10" s="1" t="s">
         <v>141</v>
@@ -9403,7 +9392,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" s="4"/>
       <c r="B11" s="1" t="s">
         <v>142</v>
@@ -9429,7 +9418,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" s="4"/>
       <c r="B12" s="1" t="s">
         <v>143</v>
@@ -9455,7 +9444,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" s="4"/>
       <c r="B13" s="1" t="s">
         <v>29</v>
@@ -9481,7 +9470,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" s="4"/>
       <c r="E14" t="str">
         <f t="shared" si="0"/>
@@ -9492,7 +9481,7 @@
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" s="4"/>
       <c r="B15" s="1" t="s">
         <v>147</v>
@@ -9518,7 +9507,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" s="4"/>
       <c r="B16" s="1" t="s">
         <v>66</v>
@@ -9544,7 +9533,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17" s="4"/>
       <c r="B17" s="1" t="s">
         <v>65</v>
@@ -9570,7 +9559,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A18" s="4"/>
       <c r="B18" s="1" t="s">
         <v>116</v>
@@ -9590,7 +9579,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A19" s="4"/>
       <c r="B19" s="1" t="s">
         <v>64</v>
@@ -9616,7 +9605,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A20" s="4"/>
       <c r="B20" s="1" t="s">
         <v>43</v>
@@ -9642,7 +9631,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A21" s="4"/>
       <c r="B21" s="1" t="s">
         <v>101</v>
@@ -9668,7 +9657,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A22" s="4"/>
       <c r="B22" s="1" t="s">
         <v>105</v>
@@ -9691,7 +9680,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A23" s="4"/>
       <c r="E23" t="str">
         <f t="shared" si="0"/>
@@ -9699,7 +9688,7 @@
       </c>
       <c r="F23"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A24" s="4" t="s">
         <v>6</v>
       </c>
@@ -9712,7 +9701,7 @@
         <v/>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A25" s="4"/>
       <c r="B25" s="1" t="s">
         <v>126</v>
@@ -9731,7 +9720,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A26" s="4"/>
       <c r="B26" s="1" t="s">
         <v>33</v>
@@ -9754,7 +9743,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A27" s="4"/>
       <c r="B27" s="1" t="s">
         <v>67</v>
@@ -9777,7 +9766,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A28" s="4"/>
       <c r="B28" s="1" t="s">
         <v>68</v>
@@ -9803,7 +9792,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A29" s="4"/>
       <c r="B29" s="1" t="s">
         <v>69</v>
@@ -9826,7 +9815,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A30" s="4"/>
       <c r="B30" s="1" t="s">
         <v>70</v>
@@ -9849,7 +9838,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A31" s="4"/>
       <c r="B31" s="2" t="s">
         <v>71</v>
@@ -9872,7 +9861,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A32" s="4"/>
       <c r="B32" s="1" t="s">
         <v>129</v>
@@ -9889,7 +9878,7 @@
         <v/>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A33" s="4"/>
       <c r="B33" s="1" t="s">
         <v>72</v>
@@ -9912,7 +9901,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A34" s="4"/>
       <c r="B34" s="1" t="s">
         <v>130</v>
@@ -9929,7 +9918,7 @@
         <v/>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A35" s="4"/>
       <c r="B35" s="1" t="s">
         <v>133</v>
@@ -9943,13 +9932,13 @@
       </c>
       <c r="F35"/>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A36" s="4"/>
       <c r="C36" s="8"/>
       <c r="E36"/>
       <c r="F36"/>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A37" s="4" t="s">
         <v>7</v>
       </c>
@@ -9962,7 +9951,7 @@
         <v/>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A38" s="4"/>
       <c r="B38" s="1" t="s">
         <v>73</v>
@@ -9985,7 +9974,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A39" s="4"/>
       <c r="B39" s="1" t="s">
         <v>107</v>
@@ -10005,7 +9994,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A40" s="4"/>
       <c r="B40" s="1" t="s">
         <v>109</v>
@@ -10022,7 +10011,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A41" s="4"/>
       <c r="B41" s="1" t="s">
         <v>110</v>
@@ -10039,7 +10028,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A42" s="4"/>
       <c r="B42" s="1" t="s">
         <v>111</v>
@@ -10056,7 +10045,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A43" s="4"/>
       <c r="B43" s="1" t="s">
         <v>118</v>
@@ -10073,12 +10062,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A44" s="4"/>
       <c r="E44"/>
       <c r="F44"/>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A45" s="4" t="s">
         <v>12</v>
       </c>
@@ -10091,7 +10080,7 @@
         <v/>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A46" s="4"/>
       <c r="B46" s="1" t="s">
         <v>74</v>
@@ -10114,7 +10103,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A47" s="4"/>
       <c r="B47" s="1" t="s">
         <v>75</v>
@@ -10131,7 +10120,7 @@
         <v/>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A48" s="4"/>
       <c r="B48" s="1" t="s">
         <v>76</v>
@@ -10154,12 +10143,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A49" s="4"/>
       <c r="E49"/>
       <c r="F49"/>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A50" s="4" t="s">
         <v>21</v>
       </c>
@@ -10172,7 +10161,7 @@
         <v/>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A51" s="4"/>
       <c r="B51" s="1" t="s">
         <v>22</v>
@@ -10195,7 +10184,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A52" s="4"/>
       <c r="B52" s="1" t="s">
         <v>77</v>
@@ -10212,7 +10201,7 @@
         <v/>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A53" s="4"/>
       <c r="E53" t="str">
         <f t="shared" si="4"/>
@@ -10223,7 +10212,7 @@
         <v/>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A54" s="4" t="s">
         <v>16</v>
       </c>
@@ -10236,7 +10225,7 @@
         <v/>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A55" s="4"/>
       <c r="B55" s="1" t="s">
         <v>78</v>
@@ -10259,7 +10248,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A56" s="4"/>
       <c r="B56" s="1" t="s">
         <v>25</v>
@@ -10282,7 +10271,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A57" s="4"/>
       <c r="B57" s="1" t="s">
         <v>79</v>
@@ -10305,7 +10294,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A58" s="4"/>
       <c r="B58" s="2" t="s">
         <v>41</v>
@@ -10328,7 +10317,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A59" s="4"/>
       <c r="B59" s="1" t="s">
         <v>80</v>
@@ -10351,7 +10340,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A60" s="4"/>
       <c r="B60" s="1" t="s">
         <v>81</v>
@@ -10368,7 +10357,7 @@
         <v/>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A61" s="4"/>
       <c r="B61" s="1" t="s">
         <v>82</v>
@@ -10385,7 +10374,7 @@
         <v/>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A62" s="4"/>
       <c r="B62" s="1" t="s">
         <v>83</v>
@@ -10402,7 +10391,7 @@
         <v/>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A63" s="4"/>
       <c r="B63" s="1" t="s">
         <v>84</v>
@@ -10419,7 +10408,7 @@
         <v/>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A64" s="4"/>
       <c r="B64" s="1" t="s">
         <v>85</v>
@@ -10442,7 +10431,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A65" s="4"/>
       <c r="B65" s="1" t="s">
         <v>58</v>
@@ -10465,7 +10454,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A66" s="4"/>
       <c r="B66" s="1" t="s">
         <v>92</v>
@@ -10488,7 +10477,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A67" s="4"/>
       <c r="B67" s="1" t="s">
         <v>93</v>
@@ -10511,7 +10500,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A68" s="4"/>
       <c r="B68" s="1" t="s">
         <v>96</v>
@@ -10531,7 +10520,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A69" s="4"/>
       <c r="C69" s="2"/>
       <c r="E69" t="str">
@@ -10543,7 +10532,7 @@
         <v/>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A70" s="4" t="s">
         <v>8</v>
       </c>
@@ -10556,7 +10545,7 @@
         <v/>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A71" s="4"/>
       <c r="B71" s="1" t="s">
         <v>136</v>
@@ -10573,7 +10562,7 @@
         <v/>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A72" s="4"/>
       <c r="B72" s="1" t="s">
         <v>86</v>
@@ -10590,7 +10579,7 @@
         <v/>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A73" s="4"/>
       <c r="B73" s="1" t="s">
         <v>87</v>
@@ -10613,7 +10602,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A74" s="4"/>
       <c r="B74" s="1" t="s">
         <v>88</v>
@@ -10636,7 +10625,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A75" s="4"/>
       <c r="B75" s="1" t="s">
         <v>89</v>
@@ -10659,7 +10648,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A76" s="4"/>
       <c r="B76" s="1" t="s">
         <v>138</v>
@@ -10679,23 +10668,23 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A77" s="4"/>
       <c r="E77"/>
       <c r="F77"/>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A78" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E78"/>
       <c r="F78"/>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.35">
       <c r="E79"/>
       <c r="F79"/>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B80" s="1" t="s">
         <v>58</v>
       </c>
@@ -10705,7 +10694,7 @@
       <c r="E80"/>
       <c r="F80"/>
     </row>
-    <row r="81" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B81" s="1" t="s">
         <v>60</v>
       </c>
@@ -10715,7 +10704,7 @@
       <c r="E81"/>
       <c r="F81"/>
     </row>
-    <row r="82" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B82" s="1" t="s">
         <v>126</v>
       </c>
@@ -10728,7 +10717,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="83" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B83" s="1" t="s">
         <v>114</v>
       </c>
@@ -10741,18 +10730,18 @@
         <v>122</v>
       </c>
     </row>
-    <row r="84" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:8" x14ac:dyDescent="0.35">
       <c r="E84"/>
       <c r="F84"/>
     </row>
-    <row r="85" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:8" x14ac:dyDescent="0.35">
       <c r="E85"/>
       <c r="F85"/>
     </row>
-    <row r="86" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:8" x14ac:dyDescent="0.35">
       <c r="F86"/>
     </row>
-    <row r="87" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="87" spans="2:8" x14ac:dyDescent="0.35">
       <c r="F87"/>
     </row>
   </sheetData>

</xml_diff>